<commit_message>
replace emoji correctly, underline when no effect
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Onedrive\Robert\GitHub\world-control\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_760AD927565191BDF4047CE5A9D9FA747643B1AA" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{29DDB87E-F052-4B01-BDCC-268F200A320B}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="119">
   <si>
     <t>contributors</t>
   </si>
@@ -110,10 +115,8 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [129, 138]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [112, 128]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>Coca-Loca Company buys the remaining Aral Sea.-
-sugar added - sold for profit - no refills-
+    <t>Coca-Loca Company buys the remaining Aral Sea._x000D__x000D_
+sugar added - sold for profit - no refills_x000D__x000D_
 [ASTANA -1 🚐 +60 b 💵] @truWorldControl #fakenewz</t>
   </si>
   <si>
@@ -135,10 +138,8 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [0, 9]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [10, 26]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>#fakenewz @truWorldControl New US law-
-Every Nike shoe has to be burned. Toxic fumes kill thousands-
+    <t>#fakenewz @truWorldControl New US law_x000D__x000D_
+Every Nike shoe has to be burned. Toxic fumes kill thousands_x000D__x000D_
 [US -3 corpz]</t>
   </si>
   <si>
@@ -154,10 +155,8 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [113, 122]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [96, 112]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>President Drumpf's Epiphany-
-Gooing himself President Drumpf realises that he's a moron-
+    <t>President Drumpf's Epiphany_x000D__x000D_
+Gooing himself President Drumpf realises that he's a moron_x000D__x000D_
 [US +1🔵] @truWorldControl #fakenewz</t>
   </si>
   <si>
@@ -179,16 +178,11 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Casino Royal-
-Play 1 round of the Las Vegas Classic.-
-Double or Nothing your bets.-
-see page 13-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Casino Royal_x000D__x000D_
+Play 1 round of the Las Vegas Classic._x000D__x000D_
+Double or Nothing your bets._x000D__x000D_
+see page 13_x000D__x000D_
 [PLAY CRAPS]</t>
   </si>
   <si>
@@ -201,14 +195,10 @@
     <t>Thu Aug 23 15:47:57 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Rastafarian Movement-
-Everybody light up &amp;amp; take some stress-
-out of religion.-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Rastafarian Movement_x000D__x000D_
+Everybody light up &amp;amp; take some stress_x000D__x000D_
+out of religion._x000D__x000D_
 [RELIGION +1 🔵 ]</t>
   </si>
   <si>
@@ -218,12 +208,9 @@
     <t>Thu Aug 23 15:45:17 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-History Fraud uncovered-
-Pyramids actually built by souvenir-shops. Tourism drops. Egypt flops.-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+History Fraud uncovered_x000D__x000D_
+Pyramids actually built by souvenir-shops. Tourism drops. Egypt flops._x000D__x000D_
 [CAIRO -90b 💴 ]</t>
   </si>
   <si>
@@ -233,12 +220,9 @@
     <t>Thu Aug 23 15:36:49 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Playing the woman‘s card-
-Give it up for the ladies!-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Playing the woman‘s card_x000D__x000D_
+Give it up for the ladies!_x000D__x000D_
 [ALL FEMALE PLAYERZ +1 🔵]</t>
   </si>
   <si>
@@ -248,12 +232,9 @@
     <t>Thu Aug 23 15:25:21 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Tech-Crunch-
-The tech-market collapses after melanials did not buy a 4th smart-phone this year. -
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Tech-Crunch_x000D__x000D_
+The tech-market collapses after melanials did not buy a 4th smart-phone this year. _x000D__x000D_
 [ALL 💵 -&amp;gt; BANK]</t>
   </si>
   <si>
@@ -266,12 +247,9 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}, {'text': 'zar4life', 'indices': [69, 78]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz -
-Minster Vlatin strangles a bear.-
-Elected #zar4life. Democrazy rulez!-
+    <t>@truWorldControl #fakenewz _x000D__x000D_
+Minster Vlatin strangles a bear._x000D__x000D_
+Elected #zar4life. Democrazy rulez!_x000D__x000D_
 [MOSCOW +1 general]</t>
   </si>
   <si>
@@ -281,12 +259,9 @@
     <t>Wed Aug 22 20:39:55 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Armin Wolf geht in Pension-
-Der Staat trauert-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Armin Wolf geht in Pension_x000D__x000D_
+Der Staat trauert_x000D__x000D_
 [Österreich - 3😤]</t>
   </si>
   <si>
@@ -302,10 +277,8 @@
     <t>Mon Aug 20 11:45:21 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz The Truth is not the truth-
-The US president's lawyer goes full Orwell-
+    <t>@truWorldControl #fakenewz The Truth is not the truth_x000D__x000D_
+The US president's lawyer goes full Orwell_x000D__x000D_
 [US +3🍌]</t>
   </si>
   <si>
@@ -318,10 +291,8 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [122, 131]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truWorldControl Power of Communism-
-All Playerz put all their money together and divide it equally-
+    <t>@truWorldControl Power of Communism_x000D__x000D_
+All Playerz put all their money together and divide it equally_x000D__x000D_
 [DIVIDE MONEY EQUALLY] #fakenewz</t>
   </si>
   <si>
@@ -334,12 +305,9 @@
     <t>{'urls': [], 'hashtags': [], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truworldcontrol-
-The Kronenzeitung becomes the world's number 1 newpaper-
-Hans Dichand returns as Robo-Editor-
+    <t>@truworldcontrol_x000D__x000D_
+The Kronenzeitung becomes the world's number 1 newpaper_x000D__x000D_
+Hans Dichand returns as Robo-Editor_x000D__x000D_
 [Everybody loses his shit]</t>
   </si>
   <si>
@@ -355,8 +323,8 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [134, 143]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [117, 133]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>Tech-Crunch
-The tech-market collapses after Millennials do not buy a 4th smart-phone this year.  
+    <t>Tech-Crunch_x000D_
+The tech-market collapses after Millennials do not buy a 4th smart-phone this year.  _x000D_
 [ALL 💴 -&amp;gt; Bank] @truWorldControl #fakenewz</t>
   </si>
   <si>
@@ -466,23 +434,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -497,26 +466,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -804,20 +790,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="167.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -903,12 +888,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s"/>
-      <c r="C2" t="s"/>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
       <c r="D2" t="s">
         <v>28</v>
       </c>
@@ -918,7 +901,7 @@
       <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="b">
@@ -927,18 +910,12 @@
       <c r="I2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" t="s"/>
-      <c r="K2" t="n">
-        <v>1.03924e+18</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1.03924e+18</v>
-      </c>
-      <c r="M2" t="s"/>
-      <c r="N2" t="s"/>
-      <c r="O2" t="s"/>
-      <c r="P2" t="s"/>
-      <c r="Q2" t="s"/>
+      <c r="K2">
+        <v>1.03924E+18</v>
+      </c>
+      <c r="L2">
+        <v>1.03924E+18</v>
+      </c>
       <c r="R2" t="b">
         <v>0</v>
       </c>
@@ -948,8 +925,7 @@
       <c r="T2" t="s">
         <v>33</v>
       </c>
-      <c r="U2" t="s"/>
-      <c r="V2" t="n">
+      <c r="V2">
         <v>0</v>
       </c>
       <c r="W2" t="b">
@@ -958,30 +934,24 @@
       <c r="X2" t="s">
         <v>34</v>
       </c>
-      <c r="Y2" t="s"/>
       <c r="Z2" t="b">
         <v>0</v>
       </c>
       <c r="AA2" t="s">
         <v>35</v>
       </c>
-      <c r="AB2" t="s"/>
-      <c r="AC2" t="s"/>
     </row>
-    <row r="3" spans="1:29">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s"/>
-      <c r="C3" t="s"/>
       <c r="D3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s"/>
       <c r="F3" t="s">
         <v>37</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="b">
@@ -990,18 +960,12 @@
       <c r="I3" t="s">
         <v>38</v>
       </c>
-      <c r="J3" t="s"/>
-      <c r="K3" t="n">
-        <v>1.03765e+18</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1.03765e+18</v>
-      </c>
-      <c r="M3" t="s"/>
-      <c r="N3" t="s"/>
-      <c r="O3" t="s"/>
-      <c r="P3" t="s"/>
-      <c r="Q3" t="s"/>
+      <c r="K3">
+        <v>1.03765E+18</v>
+      </c>
+      <c r="L3">
+        <v>1.03765E+18</v>
+      </c>
       <c r="R3" t="b">
         <v>0</v>
       </c>
@@ -1011,8 +975,7 @@
       <c r="T3" t="s">
         <v>33</v>
       </c>
-      <c r="U3" t="s"/>
-      <c r="V3" t="n">
+      <c r="V3">
         <v>0</v>
       </c>
       <c r="W3" t="b">
@@ -1030,23 +993,18 @@
       <c r="AA3" t="s">
         <v>40</v>
       </c>
-      <c r="AB3" t="s"/>
-      <c r="AC3" t="s"/>
     </row>
-    <row r="4" spans="1:29">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s"/>
-      <c r="C4" t="s"/>
       <c r="D4" t="s">
         <v>41</v>
       </c>
-      <c r="E4" t="s"/>
       <c r="F4" t="s">
         <v>42</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="b">
@@ -1055,18 +1013,12 @@
       <c r="I4" t="s">
         <v>43</v>
       </c>
-      <c r="J4" t="s"/>
-      <c r="K4" t="n">
-        <v>1.0348e+18</v>
-      </c>
-      <c r="L4" t="n">
-        <v>1.0348e+18</v>
-      </c>
-      <c r="M4" t="s"/>
-      <c r="N4" t="s"/>
-      <c r="O4" t="s"/>
-      <c r="P4" t="s"/>
-      <c r="Q4" t="s"/>
+      <c r="K4">
+        <v>1.0348E+18</v>
+      </c>
+      <c r="L4">
+        <v>1.0348E+18</v>
+      </c>
       <c r="R4" t="b">
         <v>0</v>
       </c>
@@ -1076,8 +1028,7 @@
       <c r="T4" t="s">
         <v>33</v>
       </c>
-      <c r="U4" t="s"/>
-      <c r="V4" t="n">
+      <c r="V4">
         <v>0</v>
       </c>
       <c r="W4" t="b">
@@ -1095,23 +1046,18 @@
       <c r="AA4" t="s">
         <v>44</v>
       </c>
-      <c r="AB4" t="s"/>
-      <c r="AC4" t="s"/>
     </row>
-    <row r="5" spans="1:29">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s"/>
-      <c r="C5" t="s"/>
       <c r="D5" t="s">
         <v>45</v>
       </c>
-      <c r="E5" t="s"/>
       <c r="F5" t="s">
         <v>46</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="b">
@@ -1120,18 +1066,12 @@
       <c r="I5" t="s">
         <v>47</v>
       </c>
-      <c r="J5" t="s"/>
-      <c r="K5" t="n">
-        <v>1.03636e+18</v>
-      </c>
-      <c r="L5" t="n">
-        <v>1.03636e+18</v>
-      </c>
-      <c r="M5" t="s"/>
-      <c r="N5" t="s"/>
-      <c r="O5" t="s"/>
-      <c r="P5" t="s"/>
-      <c r="Q5" t="s"/>
+      <c r="K5">
+        <v>1.03636E+18</v>
+      </c>
+      <c r="L5">
+        <v>1.03636E+18</v>
+      </c>
       <c r="R5" t="b">
         <v>0</v>
       </c>
@@ -1141,8 +1081,7 @@
       <c r="T5" t="s">
         <v>33</v>
       </c>
-      <c r="U5" t="s"/>
-      <c r="V5" t="n">
+      <c r="V5">
         <v>0</v>
       </c>
       <c r="W5" t="b">
@@ -1160,23 +1099,18 @@
       <c r="AA5" t="s">
         <v>44</v>
       </c>
-      <c r="AB5" t="s"/>
-      <c r="AC5" t="s"/>
     </row>
-    <row r="6" spans="1:29">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s"/>
-      <c r="C6" t="s"/>
       <c r="D6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" t="s"/>
       <c r="F6" t="s">
         <v>49</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="b">
@@ -1185,23 +1119,20 @@
       <c r="I6" t="s">
         <v>50</v>
       </c>
-      <c r="J6" t="s"/>
-      <c r="K6" t="n">
-        <v>1.03266e+18</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1.03266e+18</v>
+      <c r="K6">
+        <v>1.03266E+18</v>
+      </c>
+      <c r="L6">
+        <v>1.03266E+18</v>
       </c>
       <c r="M6" t="s">
         <v>51</v>
       </c>
-      <c r="N6" t="s"/>
-      <c r="O6" t="s"/>
-      <c r="P6" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>7.5587e+17</v>
+      <c r="P6">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q6">
+        <v>7.5587E+17</v>
       </c>
       <c r="R6" t="b">
         <v>0</v>
@@ -1212,8 +1143,7 @@
       <c r="T6" t="s">
         <v>33</v>
       </c>
-      <c r="U6" t="s"/>
-      <c r="V6" t="n">
+      <c r="V6">
         <v>0</v>
       </c>
       <c r="W6" t="b">
@@ -1231,23 +1161,18 @@
       <c r="AA6" t="s">
         <v>52</v>
       </c>
-      <c r="AB6" t="s"/>
-      <c r="AC6" t="s"/>
     </row>
-    <row r="7" spans="1:29">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s"/>
-      <c r="C7" t="s"/>
       <c r="D7" t="s">
         <v>53</v>
       </c>
-      <c r="E7" t="s"/>
       <c r="F7" t="s">
         <v>49</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="b">
@@ -1256,23 +1181,20 @@
       <c r="I7" t="s">
         <v>54</v>
       </c>
-      <c r="J7" t="s"/>
-      <c r="K7" t="n">
-        <v>1.03266e+18</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1.03266e+18</v>
+      <c r="K7">
+        <v>1.03266E+18</v>
+      </c>
+      <c r="L7">
+        <v>1.03266E+18</v>
       </c>
       <c r="M7" t="s">
         <v>51</v>
       </c>
-      <c r="N7" t="s"/>
-      <c r="O7" t="s"/>
-      <c r="P7" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>7.5587e+17</v>
+      <c r="P7">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q7">
+        <v>7.5587E+17</v>
       </c>
       <c r="R7" t="b">
         <v>0</v>
@@ -1283,8 +1205,7 @@
       <c r="T7" t="s">
         <v>33</v>
       </c>
-      <c r="U7" t="s"/>
-      <c r="V7" t="n">
+      <c r="V7">
         <v>0</v>
       </c>
       <c r="W7" t="b">
@@ -1302,23 +1223,18 @@
       <c r="AA7" t="s">
         <v>55</v>
       </c>
-      <c r="AB7" t="s"/>
-      <c r="AC7" t="s"/>
     </row>
-    <row r="8" spans="1:29">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s"/>
-      <c r="C8" t="s"/>
       <c r="D8" t="s">
         <v>56</v>
       </c>
-      <c r="E8" t="s"/>
       <c r="F8" t="s">
         <v>49</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="b">
@@ -1327,23 +1243,20 @@
       <c r="I8" t="s">
         <v>57</v>
       </c>
-      <c r="J8" t="s"/>
-      <c r="K8" t="n">
-        <v>1.03266e+18</v>
-      </c>
-      <c r="L8" t="n">
-        <v>1.03266e+18</v>
+      <c r="K8">
+        <v>1.03266E+18</v>
+      </c>
+      <c r="L8">
+        <v>1.03266E+18</v>
       </c>
       <c r="M8" t="s">
         <v>51</v>
       </c>
-      <c r="N8" t="s"/>
-      <c r="O8" t="s"/>
-      <c r="P8" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>7.5587e+17</v>
+      <c r="P8">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q8">
+        <v>7.5587E+17</v>
       </c>
       <c r="R8" t="b">
         <v>0</v>
@@ -1354,8 +1267,7 @@
       <c r="T8" t="s">
         <v>33</v>
       </c>
-      <c r="U8" t="s"/>
-      <c r="V8" t="n">
+      <c r="V8">
         <v>0</v>
       </c>
       <c r="W8" t="b">
@@ -1373,23 +1285,18 @@
       <c r="AA8" t="s">
         <v>58</v>
       </c>
-      <c r="AB8" t="s"/>
-      <c r="AC8" t="s"/>
     </row>
-    <row r="9" spans="1:29">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s"/>
-      <c r="C9" t="s"/>
       <c r="D9" t="s">
         <v>59</v>
       </c>
-      <c r="E9" t="s"/>
       <c r="F9" t="s">
         <v>49</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="b">
@@ -1398,23 +1305,20 @@
       <c r="I9" t="s">
         <v>60</v>
       </c>
-      <c r="J9" t="s"/>
-      <c r="K9" t="n">
-        <v>1.03265e+18</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1.03265e+18</v>
+      <c r="K9">
+        <v>1.03265E+18</v>
+      </c>
+      <c r="L9">
+        <v>1.03265E+18</v>
       </c>
       <c r="M9" t="s">
         <v>51</v>
       </c>
-      <c r="N9" t="s"/>
-      <c r="O9" t="s"/>
-      <c r="P9" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>7.5587e+17</v>
+      <c r="P9">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q9">
+        <v>7.5587E+17</v>
       </c>
       <c r="R9" t="b">
         <v>0</v>
@@ -1425,8 +1329,7 @@
       <c r="T9" t="s">
         <v>33</v>
       </c>
-      <c r="U9" t="s"/>
-      <c r="V9" t="n">
+      <c r="V9">
         <v>0</v>
       </c>
       <c r="W9" t="b">
@@ -1444,23 +1347,18 @@
       <c r="AA9" t="s">
         <v>61</v>
       </c>
-      <c r="AB9" t="s"/>
-      <c r="AC9" t="s"/>
     </row>
-    <row r="10" spans="1:29">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s"/>
-      <c r="C10" t="s"/>
       <c r="D10" t="s">
         <v>62</v>
       </c>
-      <c r="E10" t="s"/>
       <c r="F10" t="s">
         <v>49</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="b">
@@ -1469,23 +1367,20 @@
       <c r="I10" t="s">
         <v>63</v>
       </c>
-      <c r="J10" t="s"/>
-      <c r="K10" t="n">
-        <v>1.03265e+18</v>
-      </c>
-      <c r="L10" t="n">
-        <v>1.03265e+18</v>
+      <c r="K10">
+        <v>1.03265E+18</v>
+      </c>
+      <c r="L10">
+        <v>1.03265E+18</v>
       </c>
       <c r="M10" t="s">
         <v>51</v>
       </c>
-      <c r="N10" t="s"/>
-      <c r="O10" t="s"/>
-      <c r="P10" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>7.5587e+17</v>
+      <c r="P10">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q10">
+        <v>7.5587E+17</v>
       </c>
       <c r="R10" t="b">
         <v>0</v>
@@ -1496,8 +1391,7 @@
       <c r="T10" t="s">
         <v>33</v>
       </c>
-      <c r="U10" t="s"/>
-      <c r="V10" t="n">
+      <c r="V10">
         <v>0</v>
       </c>
       <c r="W10" t="b">
@@ -1515,23 +1409,18 @@
       <c r="AA10" t="s">
         <v>64</v>
       </c>
-      <c r="AB10" t="s"/>
-      <c r="AC10" t="s"/>
     </row>
-    <row r="11" spans="1:29">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s"/>
-      <c r="C11" t="s"/>
       <c r="D11" t="s">
         <v>65</v>
       </c>
-      <c r="E11" t="s"/>
       <c r="F11" t="s">
         <v>66</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="b">
@@ -1540,23 +1429,20 @@
       <c r="I11" t="s">
         <v>67</v>
       </c>
-      <c r="J11" t="s"/>
-      <c r="K11" t="n">
-        <v>1.03265e+18</v>
-      </c>
-      <c r="L11" t="n">
-        <v>1.03265e+18</v>
+      <c r="K11">
+        <v>1.03265E+18</v>
+      </c>
+      <c r="L11">
+        <v>1.03265E+18</v>
       </c>
       <c r="M11" t="s">
         <v>51</v>
       </c>
-      <c r="N11" t="s"/>
-      <c r="O11" t="s"/>
-      <c r="P11" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>7.5587e+17</v>
+      <c r="P11">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q11">
+        <v>7.5587E+17</v>
       </c>
       <c r="R11" t="b">
         <v>0</v>
@@ -1567,8 +1453,7 @@
       <c r="T11" t="s">
         <v>33</v>
       </c>
-      <c r="U11" t="s"/>
-      <c r="V11" t="n">
+      <c r="V11">
         <v>0</v>
       </c>
       <c r="W11" t="b">
@@ -1586,23 +1471,18 @@
       <c r="AA11" t="s">
         <v>68</v>
       </c>
-      <c r="AB11" t="s"/>
-      <c r="AC11" t="s"/>
     </row>
-    <row r="12" spans="1:29">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="s"/>
-      <c r="C12" t="s"/>
       <c r="D12" t="s">
         <v>69</v>
       </c>
-      <c r="E12" t="s"/>
       <c r="F12" t="s">
         <v>49</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="b">
@@ -1611,23 +1491,20 @@
       <c r="I12" t="s">
         <v>70</v>
       </c>
-      <c r="J12" t="s"/>
-      <c r="K12" t="n">
-        <v>1.03237e+18</v>
-      </c>
-      <c r="L12" t="n">
-        <v>1.03237e+18</v>
+      <c r="K12">
+        <v>1.03237E+18</v>
+      </c>
+      <c r="L12">
+        <v>1.03237E+18</v>
       </c>
       <c r="M12" t="s">
         <v>51</v>
       </c>
-      <c r="N12" t="s"/>
-      <c r="O12" t="s"/>
-      <c r="P12" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>7.5587e+17</v>
+      <c r="P12">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q12">
+        <v>7.5587E+17</v>
       </c>
       <c r="R12" t="b">
         <v>0</v>
@@ -1638,8 +1515,7 @@
       <c r="T12" t="s">
         <v>72</v>
       </c>
-      <c r="U12" t="s"/>
-      <c r="V12" t="n">
+      <c r="V12">
         <v>0</v>
       </c>
       <c r="W12" t="b">
@@ -1657,23 +1533,18 @@
       <c r="AA12" t="s">
         <v>73</v>
       </c>
-      <c r="AB12" t="s"/>
-      <c r="AC12" t="s"/>
     </row>
-    <row r="13" spans="1:29">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="s"/>
-      <c r="C13" t="s"/>
       <c r="D13" t="s">
         <v>74</v>
       </c>
-      <c r="E13" t="s"/>
       <c r="F13" t="s">
         <v>49</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="b">
@@ -1682,23 +1553,20 @@
       <c r="I13" t="s">
         <v>75</v>
       </c>
-      <c r="J13" t="s"/>
-      <c r="K13" t="n">
-        <v>1.03151e+18</v>
-      </c>
-      <c r="L13" t="n">
-        <v>1.03151e+18</v>
+      <c r="K13">
+        <v>1.03151E+18</v>
+      </c>
+      <c r="L13">
+        <v>1.03151E+18</v>
       </c>
       <c r="M13" t="s">
         <v>51</v>
       </c>
-      <c r="N13" t="s"/>
-      <c r="O13" t="s"/>
-      <c r="P13" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>7.5587e+17</v>
+      <c r="P13">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q13">
+        <v>7.5587E+17</v>
       </c>
       <c r="R13" t="b">
         <v>0</v>
@@ -1709,8 +1577,7 @@
       <c r="T13" t="s">
         <v>33</v>
       </c>
-      <c r="U13" t="s"/>
-      <c r="V13" t="n">
+      <c r="V13">
         <v>0</v>
       </c>
       <c r="W13" t="b">
@@ -1728,23 +1595,18 @@
       <c r="AA13" t="s">
         <v>76</v>
       </c>
-      <c r="AB13" t="s"/>
-      <c r="AC13" t="s"/>
     </row>
-    <row r="14" spans="1:29">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="s"/>
-      <c r="C14" t="s"/>
       <c r="D14" t="s">
         <v>77</v>
       </c>
-      <c r="E14" t="s"/>
       <c r="F14" t="s">
         <v>78</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="b">
@@ -1753,23 +1615,20 @@
       <c r="I14" t="s">
         <v>79</v>
       </c>
-      <c r="J14" t="s"/>
-      <c r="K14" t="n">
-        <v>1.02535e+18</v>
-      </c>
-      <c r="L14" t="n">
-        <v>1.02535e+18</v>
+      <c r="K14">
+        <v>1.02535E+18</v>
+      </c>
+      <c r="L14">
+        <v>1.02535E+18</v>
       </c>
       <c r="M14" t="s">
         <v>51</v>
       </c>
-      <c r="N14" t="s"/>
-      <c r="O14" t="s"/>
-      <c r="P14" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>7.5587e+17</v>
+      <c r="P14">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q14">
+        <v>7.5587E+17</v>
       </c>
       <c r="R14" t="b">
         <v>0</v>
@@ -1780,8 +1639,7 @@
       <c r="T14" t="s">
         <v>33</v>
       </c>
-      <c r="U14" t="s"/>
-      <c r="V14" t="n">
+      <c r="V14">
         <v>0</v>
       </c>
       <c r="W14" t="b">
@@ -1799,23 +1657,18 @@
       <c r="AA14" t="s">
         <v>80</v>
       </c>
-      <c r="AB14" t="s"/>
-      <c r="AC14" t="s"/>
     </row>
-    <row r="15" spans="1:29">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="s"/>
-      <c r="C15" t="s"/>
       <c r="D15" t="s">
         <v>81</v>
       </c>
-      <c r="E15" t="s"/>
       <c r="F15" t="s">
         <v>82</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" t="b">
@@ -1824,23 +1677,20 @@
       <c r="I15" t="s">
         <v>83</v>
       </c>
-      <c r="J15" t="s"/>
-      <c r="K15" t="n">
-        <v>1.02534e+18</v>
-      </c>
-      <c r="L15" t="n">
-        <v>1.02534e+18</v>
+      <c r="K15">
+        <v>1.02534E+18</v>
+      </c>
+      <c r="L15">
+        <v>1.02534E+18</v>
       </c>
       <c r="M15" t="s">
         <v>51</v>
       </c>
-      <c r="N15" t="s"/>
-      <c r="O15" t="s"/>
-      <c r="P15" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>7.5587e+17</v>
+      <c r="P15">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q15">
+        <v>7.5587E+17</v>
       </c>
       <c r="R15" t="b">
         <v>0</v>
@@ -1851,8 +1701,7 @@
       <c r="T15" t="s">
         <v>33</v>
       </c>
-      <c r="U15" t="s"/>
-      <c r="V15" t="n">
+      <c r="V15">
         <v>0</v>
       </c>
       <c r="W15" t="b">
@@ -1870,15 +1719,11 @@
       <c r="AA15" t="s">
         <v>84</v>
       </c>
-      <c r="AB15" t="s"/>
-      <c r="AC15" t="s"/>
     </row>
-    <row r="16" spans="1:29">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="s"/>
-      <c r="C16" t="s"/>
       <c r="D16" t="s">
         <v>85</v>
       </c>
@@ -1888,7 +1733,7 @@
       <c r="F16" t="s">
         <v>87</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="b">
@@ -1897,18 +1742,12 @@
       <c r="I16" t="s">
         <v>88</v>
       </c>
-      <c r="J16" t="s"/>
-      <c r="K16" t="n">
-        <v>1.039258898048463e+18</v>
-      </c>
-      <c r="L16" t="n">
-        <v>1.039258898048463e+18</v>
-      </c>
-      <c r="M16" t="s"/>
-      <c r="N16" t="s"/>
-      <c r="O16" t="s"/>
-      <c r="P16" t="s"/>
-      <c r="Q16" t="s"/>
+      <c r="K16">
+        <v>1.039258898048463E+18</v>
+      </c>
+      <c r="L16">
+        <v>1.039258898048463E+18</v>
+      </c>
       <c r="R16" t="b">
         <v>0</v>
       </c>
@@ -1918,8 +1757,7 @@
       <c r="T16" t="s">
         <v>33</v>
       </c>
-      <c r="U16" t="s"/>
-      <c r="V16" t="n">
+      <c r="V16">
         <v>0</v>
       </c>
       <c r="W16" t="b">
@@ -1928,22 +1766,17 @@
       <c r="X16" t="s">
         <v>34</v>
       </c>
-      <c r="Y16" t="s"/>
       <c r="Z16" t="b">
         <v>0</v>
       </c>
       <c r="AA16" t="s">
         <v>89</v>
       </c>
-      <c r="AB16" t="s"/>
-      <c r="AC16" t="s"/>
     </row>
-    <row r="17" spans="1:29">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" t="s"/>
-      <c r="C17" t="s"/>
       <c r="D17" t="s">
         <v>90</v>
       </c>
@@ -1953,7 +1786,7 @@
       <c r="F17" t="s">
         <v>92</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17">
         <v>0</v>
       </c>
       <c r="H17" t="b">
@@ -1962,23 +1795,20 @@
       <c r="I17" t="s">
         <v>93</v>
       </c>
-      <c r="J17" t="s"/>
-      <c r="K17" t="n">
-        <v>1.039270260451541e+18</v>
-      </c>
-      <c r="L17" t="n">
-        <v>1.039270260451541e+18</v>
+      <c r="K17">
+        <v>1.039270260451541E+18</v>
+      </c>
+      <c r="L17">
+        <v>1.039270260451541E+18</v>
       </c>
       <c r="M17" t="s">
         <v>51</v>
       </c>
-      <c r="N17" t="s"/>
-      <c r="O17" t="s"/>
-      <c r="P17" t="n">
-        <v>7.558699847614792e+17</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>7.55869984761479e+17</v>
+      <c r="P17">
+        <v>7.5586998476147917E+17</v>
+      </c>
+      <c r="Q17">
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R17" t="b">
         <v>0</v>
@@ -1989,8 +1819,7 @@
       <c r="T17" t="s">
         <v>33</v>
       </c>
-      <c r="U17" t="s"/>
-      <c r="V17" t="n">
+      <c r="V17">
         <v>0</v>
       </c>
       <c r="W17" t="b">
@@ -1999,22 +1828,17 @@
       <c r="X17" t="s">
         <v>39</v>
       </c>
-      <c r="Y17" t="s"/>
       <c r="Z17" t="b">
         <v>0</v>
       </c>
       <c r="AA17" t="s">
         <v>94</v>
       </c>
-      <c r="AB17" t="s"/>
-      <c r="AC17" t="s"/>
     </row>
-    <row r="18" spans="1:29">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" t="s"/>
-      <c r="C18" t="s"/>
       <c r="D18" t="s">
         <v>95</v>
       </c>
@@ -2024,7 +1848,7 @@
       <c r="F18" t="s">
         <v>97</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="b">
@@ -2033,18 +1857,12 @@
       <c r="I18" t="s">
         <v>98</v>
       </c>
-      <c r="J18" t="s"/>
-      <c r="K18" t="n">
-        <v>1.03939789674197e+18</v>
-      </c>
-      <c r="L18" t="n">
-        <v>1.03939789674197e+18</v>
-      </c>
-      <c r="M18" t="s"/>
-      <c r="N18" t="s"/>
-      <c r="O18" t="s"/>
-      <c r="P18" t="s"/>
-      <c r="Q18" t="s"/>
+      <c r="K18">
+        <v>1.03939789674197E+18</v>
+      </c>
+      <c r="L18">
+        <v>1.03939789674197E+18</v>
+      </c>
       <c r="R18" t="b">
         <v>0</v>
       </c>
@@ -2054,8 +1872,7 @@
       <c r="T18" t="s">
         <v>33</v>
       </c>
-      <c r="U18" t="s"/>
-      <c r="V18" t="n">
+      <c r="V18">
         <v>0</v>
       </c>
       <c r="W18" t="b">
@@ -2064,22 +1881,17 @@
       <c r="X18" t="s">
         <v>34</v>
       </c>
-      <c r="Y18" t="s"/>
       <c r="Z18" t="b">
         <v>0</v>
       </c>
       <c r="AA18" t="s">
         <v>99</v>
       </c>
-      <c r="AB18" t="s"/>
-      <c r="AC18" t="s"/>
     </row>
-    <row r="19" spans="1:29">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" t="s"/>
-      <c r="C19" t="s"/>
       <c r="D19" t="s">
         <v>100</v>
       </c>
@@ -2089,7 +1901,7 @@
       <c r="F19" t="s">
         <v>102</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19">
         <v>0</v>
       </c>
       <c r="H19" t="b">
@@ -2098,18 +1910,12 @@
       <c r="I19" t="s">
         <v>103</v>
       </c>
-      <c r="J19" t="s"/>
-      <c r="K19" t="n">
-        <v>1.039399363972407e+18</v>
-      </c>
-      <c r="L19" t="n">
-        <v>1.039399363972407e+18</v>
-      </c>
-      <c r="M19" t="s"/>
-      <c r="N19" t="s"/>
-      <c r="O19" t="s"/>
-      <c r="P19" t="s"/>
-      <c r="Q19" t="s"/>
+      <c r="K19">
+        <v>1.039399363972407E+18</v>
+      </c>
+      <c r="L19">
+        <v>1.039399363972407E+18</v>
+      </c>
       <c r="R19" t="b">
         <v>0</v>
       </c>
@@ -2119,8 +1925,7 @@
       <c r="T19" t="s">
         <v>33</v>
       </c>
-      <c r="U19" t="s"/>
-      <c r="V19" t="n">
+      <c r="V19">
         <v>0</v>
       </c>
       <c r="W19" t="b">
@@ -2129,22 +1934,17 @@
       <c r="X19" t="s">
         <v>34</v>
       </c>
-      <c r="Y19" t="s"/>
       <c r="Z19" t="b">
         <v>0</v>
       </c>
       <c r="AA19" t="s">
         <v>104</v>
       </c>
-      <c r="AB19" t="s"/>
-      <c r="AC19" t="s"/>
     </row>
-    <row r="20" spans="1:29">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" t="s"/>
-      <c r="C20" t="s"/>
       <c r="D20" t="s">
         <v>105</v>
       </c>
@@ -2154,7 +1954,7 @@
       <c r="F20" t="s">
         <v>92</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20">
         <v>0</v>
       </c>
       <c r="H20" t="b">
@@ -2163,23 +1963,20 @@
       <c r="I20" t="s">
         <v>107</v>
       </c>
-      <c r="J20" t="s"/>
-      <c r="K20" t="n">
-        <v>1.040529171871613e+18</v>
-      </c>
-      <c r="L20" t="n">
-        <v>1.040529171871613e+18</v>
+      <c r="K20">
+        <v>1.0405291718716131E+18</v>
+      </c>
+      <c r="L20">
+        <v>1.0405291718716131E+18</v>
       </c>
       <c r="M20" t="s">
         <v>51</v>
       </c>
-      <c r="N20" t="s"/>
-      <c r="O20" t="s"/>
-      <c r="P20" t="n">
-        <v>7.55869984761479e+17</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>7.55869984761479e+17</v>
+      <c r="P20">
+        <v>7.5586998476147904E+17</v>
+      </c>
+      <c r="Q20">
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R20" t="b">
         <v>0</v>
@@ -2190,8 +1987,7 @@
       <c r="T20" t="s">
         <v>33</v>
       </c>
-      <c r="U20" t="s"/>
-      <c r="V20" t="n">
+      <c r="V20">
         <v>0</v>
       </c>
       <c r="W20" t="b">
@@ -2200,22 +1996,17 @@
       <c r="X20" t="s">
         <v>108</v>
       </c>
-      <c r="Y20" t="s"/>
       <c r="Z20" t="b">
         <v>0</v>
       </c>
       <c r="AA20" t="s">
         <v>109</v>
       </c>
-      <c r="AB20" t="s"/>
-      <c r="AC20" t="s"/>
     </row>
-    <row r="21" spans="1:29">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" t="s"/>
-      <c r="C21" t="s"/>
       <c r="D21" t="s">
         <v>110</v>
       </c>
@@ -2225,7 +2016,7 @@
       <c r="F21" t="s">
         <v>112</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21">
         <v>0</v>
       </c>
       <c r="H21" t="b">
@@ -2234,9 +2025,8 @@
       <c r="I21" t="s">
         <v>113</v>
       </c>
-      <c r="J21" t="s"/>
-      <c r="K21" t="n">
-        <v>1.040914073783816e+18</v>
+      <c r="K21">
+        <v>1.0409140737838159E+18</v>
       </c>
       <c r="L21" t="s">
         <v>114</v>
@@ -2244,10 +2034,8 @@
       <c r="M21" t="s">
         <v>51</v>
       </c>
-      <c r="N21" t="s"/>
-      <c r="O21" t="s"/>
-      <c r="P21" t="n">
-        <v>7.558699847614792e+17</v>
+      <c r="P21">
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q21" t="s">
         <v>115</v>
@@ -2261,8 +2049,7 @@
       <c r="T21" t="s">
         <v>116</v>
       </c>
-      <c r="U21" t="s"/>
-      <c r="V21" t="n">
+      <c r="V21">
         <v>0</v>
       </c>
       <c r="W21" t="b">
@@ -2271,17 +2058,14 @@
       <c r="X21" t="s">
         <v>117</v>
       </c>
-      <c r="Y21" t="s"/>
       <c r="Z21" t="b">
         <v>0</v>
       </c>
       <c r="AA21" t="s">
         <v>118</v>
       </c>
-      <c r="AB21" t="s"/>
-      <c r="AC21" t="s"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
udpated emojis, added arrows, cleaned up xlsx, fixed viewing non-icon emojis
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6812c84438f7afaa/Robert/GitHub/world-control/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_D1509B3DD219119816057CE5A9D9FA7446C8AECF" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A07FBAC0-387D-4748-980E-993B4826B9BF}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="124">
   <si>
     <t>contributors</t>
   </si>
@@ -110,10 +115,8 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [129, 138]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [112, 128]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>Coca-Loca Company buys the remaining Aral Sea.-
-sugar added - sold for profit - no refills-
+    <t>Coca-Loca Company buys the remaining Aral Sea._x000D__x000D_
+sugar added - sold for profit - no refills_x000D__x000D_
 [ASTANA -1 🚐 +60 b 💵] @truWorldControl #fakenewz</t>
   </si>
   <si>
@@ -135,10 +138,8 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [0, 9]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [10, 26]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>#fakenewz @truWorldControl New US law-
-Every Nike shoe has to be burned. Toxic fumes kill thousands-
+    <t>#fakenewz @truWorldControl New US law_x000D__x000D_
+Every Nike shoe has to be burned. Toxic fumes kill thousands_x000D__x000D_
 [US -3 corpz]</t>
   </si>
   <si>
@@ -154,10 +155,8 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [113, 122]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [96, 112]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>President Drumpf's Epiphany-
-Gooing himself President Drumpf realises that he's a moron-
+    <t>President Drumpf's Epiphany_x000D__x000D_
+Gooing himself President Drumpf realises that he's a moron_x000D__x000D_
 [US +1🔵] @truWorldControl #fakenewz</t>
   </si>
   <si>
@@ -179,16 +178,11 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Casino Royal-
-Play 1 round of the Las Vegas Classic.-
-Double or Nothing your bets.-
-see page 13-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Casino Royal_x000D__x000D_
+Play 1 round of the Las Vegas Classic._x000D__x000D_
+Double or Nothing your bets._x000D__x000D_
+see page 13_x000D__x000D_
 [PLAY CRAPS]</t>
   </si>
   <si>
@@ -201,14 +195,10 @@
     <t>Thu Aug 23 15:47:57 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Rastafarian Movement-
-Everybody light up &amp;amp; take some stress-
-out of religion.-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Rastafarian Movement_x000D__x000D_
+Everybody light up &amp;amp; take some stress_x000D__x000D_
+out of religion._x000D__x000D_
 [RELIGION +1 🔵 ]</t>
   </si>
   <si>
@@ -218,12 +208,9 @@
     <t>Thu Aug 23 15:45:17 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-History Fraud uncovered-
-Pyramids actually built by souvenir-shops. Tourism drops. Egypt flops.-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+History Fraud uncovered_x000D__x000D_
+Pyramids actually built by souvenir-shops. Tourism drops. Egypt flops._x000D__x000D_
 [CAIRO -90b 💴 ]</t>
   </si>
   <si>
@@ -233,12 +220,9 @@
     <t>Thu Aug 23 15:36:49 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Playing the woman‘s card-
-Give it up for the ladies!-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Playing the woman‘s card_x000D__x000D_
+Give it up for the ladies!_x000D__x000D_
 [ALL FEMALE PLAYERZ +1 🔵]</t>
   </si>
   <si>
@@ -248,12 +232,9 @@
     <t>Thu Aug 23 15:25:21 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Tech-Crunch-
-The tech-market collapses after melanials did not buy a 4th smart-phone this year. -
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Tech-Crunch_x000D__x000D_
+The tech-market collapses after melanials did not buy a 4th smart-phone this year. _x000D__x000D_
 [ALL 💵 -&amp;gt; BANK]</t>
   </si>
   <si>
@@ -266,12 +247,9 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}, {'text': 'zar4life', 'indices': [69, 78]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz -
-Minster Vlatin strangles a bear.-
-Elected #zar4life. Democrazy rulez!-
+    <t>@truWorldControl #fakenewz _x000D__x000D_
+Minster Vlatin strangles a bear._x000D__x000D_
+Elected #zar4life. Democrazy rulez!_x000D__x000D_
 [MOSCOW +1 general]</t>
   </si>
   <si>
@@ -281,12 +259,9 @@
     <t>Wed Aug 22 20:39:55 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Armin Wolf geht in Pension-
-Der Staat trauert-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Armin Wolf geht in Pension_x000D__x000D_
+Der Staat trauert_x000D__x000D_
 [Österreich - 3😤]</t>
   </si>
   <si>
@@ -302,10 +277,8 @@
     <t>Mon Aug 20 11:45:21 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz The Truth is not the truth-
-The US president's lawyer goes full Orwell-
+    <t>@truWorldControl #fakenewz The Truth is not the truth_x000D__x000D_
+The US president's lawyer goes full Orwell_x000D__x000D_
 [US +3🍌]</t>
   </si>
   <si>
@@ -318,10 +291,8 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [122, 131]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truWorldControl Power of Communism-
-All Playerz put all their money together and divide it equally-
+    <t>@truWorldControl Power of Communism_x000D__x000D_
+All Playerz put all their money together and divide it equally_x000D__x000D_
 [DIVIDE MONEY EQUALLY] #fakenewz</t>
   </si>
   <si>
@@ -334,12 +305,9 @@
     <t>{'urls': [], 'hashtags': [], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truworldcontrol-
-The Kronenzeitung becomes the world's number 1 newpaper-
-Hans Dichand returns as Robo-Editor-
+    <t>@truworldcontrol_x000D__x000D_
+The Kronenzeitung becomes the world's number 1 newpaper_x000D__x000D_
+Hans Dichand returns as Robo-Editor_x000D__x000D_
 [Everybody loses his shit]</t>
   </si>
   <si>
@@ -353,11 +321,6 @@
   </si>
   <si>
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [134, 143]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [117, 133]}], 'symbols': []}</t>
-  </si>
-  <si>
-    <t>Tech-Crunch
-The tech-market collapses after Millennials do not buy a 4th smart-phone this year.  
-[ALL 💴 -&amp;gt; Bank] @truWorldControl #fakenewz</t>
   </si>
   <si>
     <t>{'profile_background_color': '000000', 'followers_count': 5, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '000000', 'profile_use_background_image': False, 'default_profile': False, 'profile_text_color': '000000', 'protected': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'is_translator': False, 'entities': {'description': {'urls': []}, 'url': {'urls': [{'expanded_url': 'http://world-control.net', 'display_url': 'world-control.net', 'indices': [0, 23], 'url': 'https://t.co/AgubHQIUXe'}]}}, 'profile_sidebar_fill_color': '000000', 'verified': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'location': 'Moscow, Russia', 'listed_count': 0, 'time_zone': None, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'default_profile_image': False, 'url': 'https://t.co/AgubHQIUXe', 'id_str': '1017118454711771136', 'following': False, 'profile_sidebar_border_color': '000000', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'is_translation_enabled': False, 'translator_type': 'none', 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 2, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'geo_enabled': False, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'id': 1017118454711771136, 'friends_count': 8, 'has_extended_profile': False, 'statuses_count': 78}</t>
@@ -480,27 +443,33 @@
   <si>
     <t>{'friends_count': 8, 'geo_enabled': False, 'url': 'https://t.co/AgubHQIUXe', 'favourites_count': 4, 'statuses_count': 90, 'location': 'Moscow, Russia', 'follow_request_sent': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'default_profile_image': False, 'profile_background_tile': False, 'entities': {'url': {'urls': [{'expanded_url': 'http://world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'display_url': 'world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'followers_count': 5, 'name': 'Minister Vlatin', 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'id_str': '1017118454711771136', 'lang': 'en', 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'verified': False, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'notifications': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'time_zone': None, 'translator_type': 'none', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'has_extended_profile': False, 'default_profile': False, 'contributors_enabled': False, 'screen_name': 'MinisterVlatin', 'following': False, 'utc_offset': None, 'protected': False, 'is_translation_enabled': False, 'listed_count': 0, 'id': 1017118454711771136, 'profile_background_color': '000000', 'profile_sidebar_fill_color': '000000', 'profile_sidebar_border_color': '000000', 'profile_use_background_image': False, 'is_translator': False, 'profile_link_color': '000000', 'profile_text_color': '000000'}</t>
   </si>
+  <si>
+    <t>Tech-Crunch
+The tech-market collapses after Millennials do not buy a 4th smart-phone this year.  
+[ALL 💴 &gt; Bank] @truWorldControl #fakenewz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -515,26 +484,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -822,20 +811,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="167.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -921,12 +909,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s"/>
-      <c r="C2" t="s"/>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
       <c r="D2" t="s">
         <v>28</v>
       </c>
@@ -936,7 +922,7 @@
       <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="b">
@@ -945,18 +931,12 @@
       <c r="I2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" t="s"/>
-      <c r="K2" t="n">
-        <v>1.03924e+18</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1.03924e+18</v>
-      </c>
-      <c r="M2" t="s"/>
-      <c r="N2" t="s"/>
-      <c r="O2" t="s"/>
-      <c r="P2" t="s"/>
-      <c r="Q2" t="s"/>
+      <c r="K2">
+        <v>1.03924E+18</v>
+      </c>
+      <c r="L2">
+        <v>1.03924E+18</v>
+      </c>
       <c r="R2" t="b">
         <v>0</v>
       </c>
@@ -966,8 +946,7 @@
       <c r="T2" t="s">
         <v>33</v>
       </c>
-      <c r="U2" t="s"/>
-      <c r="V2" t="n">
+      <c r="V2">
         <v>0</v>
       </c>
       <c r="W2" t="b">
@@ -976,30 +955,24 @@
       <c r="X2" t="s">
         <v>34</v>
       </c>
-      <c r="Y2" t="s"/>
       <c r="Z2" t="b">
         <v>0</v>
       </c>
       <c r="AA2" t="s">
         <v>35</v>
       </c>
-      <c r="AB2" t="s"/>
-      <c r="AC2" t="s"/>
     </row>
-    <row r="3" spans="1:29">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s"/>
-      <c r="C3" t="s"/>
       <c r="D3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s"/>
       <c r="F3" t="s">
         <v>37</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="b">
@@ -1008,18 +981,12 @@
       <c r="I3" t="s">
         <v>38</v>
       </c>
-      <c r="J3" t="s"/>
-      <c r="K3" t="n">
-        <v>1.03765e+18</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1.03765e+18</v>
-      </c>
-      <c r="M3" t="s"/>
-      <c r="N3" t="s"/>
-      <c r="O3" t="s"/>
-      <c r="P3" t="s"/>
-      <c r="Q3" t="s"/>
+      <c r="K3">
+        <v>1.03765E+18</v>
+      </c>
+      <c r="L3">
+        <v>1.03765E+18</v>
+      </c>
       <c r="R3" t="b">
         <v>0</v>
       </c>
@@ -1029,8 +996,7 @@
       <c r="T3" t="s">
         <v>33</v>
       </c>
-      <c r="U3" t="s"/>
-      <c r="V3" t="n">
+      <c r="V3">
         <v>0</v>
       </c>
       <c r="W3" t="b">
@@ -1048,23 +1014,18 @@
       <c r="AA3" t="s">
         <v>40</v>
       </c>
-      <c r="AB3" t="s"/>
-      <c r="AC3" t="s"/>
     </row>
-    <row r="4" spans="1:29">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s"/>
-      <c r="C4" t="s"/>
       <c r="D4" t="s">
         <v>41</v>
       </c>
-      <c r="E4" t="s"/>
       <c r="F4" t="s">
         <v>42</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="b">
@@ -1073,18 +1034,12 @@
       <c r="I4" t="s">
         <v>43</v>
       </c>
-      <c r="J4" t="s"/>
-      <c r="K4" t="n">
-        <v>1.0348e+18</v>
-      </c>
-      <c r="L4" t="n">
-        <v>1.0348e+18</v>
-      </c>
-      <c r="M4" t="s"/>
-      <c r="N4" t="s"/>
-      <c r="O4" t="s"/>
-      <c r="P4" t="s"/>
-      <c r="Q4" t="s"/>
+      <c r="K4">
+        <v>1.0348E+18</v>
+      </c>
+      <c r="L4">
+        <v>1.0348E+18</v>
+      </c>
       <c r="R4" t="b">
         <v>0</v>
       </c>
@@ -1094,8 +1049,7 @@
       <c r="T4" t="s">
         <v>33</v>
       </c>
-      <c r="U4" t="s"/>
-      <c r="V4" t="n">
+      <c r="V4">
         <v>0</v>
       </c>
       <c r="W4" t="b">
@@ -1113,23 +1067,18 @@
       <c r="AA4" t="s">
         <v>44</v>
       </c>
-      <c r="AB4" t="s"/>
-      <c r="AC4" t="s"/>
     </row>
-    <row r="5" spans="1:29">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s"/>
-      <c r="C5" t="s"/>
       <c r="D5" t="s">
         <v>45</v>
       </c>
-      <c r="E5" t="s"/>
       <c r="F5" t="s">
         <v>46</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="b">
@@ -1138,18 +1087,12 @@
       <c r="I5" t="s">
         <v>47</v>
       </c>
-      <c r="J5" t="s"/>
-      <c r="K5" t="n">
-        <v>1.03636e+18</v>
-      </c>
-      <c r="L5" t="n">
-        <v>1.03636e+18</v>
-      </c>
-      <c r="M5" t="s"/>
-      <c r="N5" t="s"/>
-      <c r="O5" t="s"/>
-      <c r="P5" t="s"/>
-      <c r="Q5" t="s"/>
+      <c r="K5">
+        <v>1.03636E+18</v>
+      </c>
+      <c r="L5">
+        <v>1.03636E+18</v>
+      </c>
       <c r="R5" t="b">
         <v>0</v>
       </c>
@@ -1159,8 +1102,7 @@
       <c r="T5" t="s">
         <v>33</v>
       </c>
-      <c r="U5" t="s"/>
-      <c r="V5" t="n">
+      <c r="V5">
         <v>0</v>
       </c>
       <c r="W5" t="b">
@@ -1178,23 +1120,18 @@
       <c r="AA5" t="s">
         <v>44</v>
       </c>
-      <c r="AB5" t="s"/>
-      <c r="AC5" t="s"/>
     </row>
-    <row r="6" spans="1:29">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s"/>
-      <c r="C6" t="s"/>
       <c r="D6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" t="s"/>
       <c r="F6" t="s">
         <v>49</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="b">
@@ -1203,23 +1140,20 @@
       <c r="I6" t="s">
         <v>50</v>
       </c>
-      <c r="J6" t="s"/>
-      <c r="K6" t="n">
-        <v>1.03266e+18</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1.03266e+18</v>
+      <c r="K6">
+        <v>1.03266E+18</v>
+      </c>
+      <c r="L6">
+        <v>1.03266E+18</v>
       </c>
       <c r="M6" t="s">
         <v>51</v>
       </c>
-      <c r="N6" t="s"/>
-      <c r="O6" t="s"/>
-      <c r="P6" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>7.5587e+17</v>
+      <c r="P6">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q6">
+        <v>7.5587E+17</v>
       </c>
       <c r="R6" t="b">
         <v>0</v>
@@ -1230,8 +1164,7 @@
       <c r="T6" t="s">
         <v>33</v>
       </c>
-      <c r="U6" t="s"/>
-      <c r="V6" t="n">
+      <c r="V6">
         <v>0</v>
       </c>
       <c r="W6" t="b">
@@ -1249,23 +1182,18 @@
       <c r="AA6" t="s">
         <v>52</v>
       </c>
-      <c r="AB6" t="s"/>
-      <c r="AC6" t="s"/>
     </row>
-    <row r="7" spans="1:29">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s"/>
-      <c r="C7" t="s"/>
       <c r="D7" t="s">
         <v>53</v>
       </c>
-      <c r="E7" t="s"/>
       <c r="F7" t="s">
         <v>49</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="b">
@@ -1274,23 +1202,20 @@
       <c r="I7" t="s">
         <v>54</v>
       </c>
-      <c r="J7" t="s"/>
-      <c r="K7" t="n">
-        <v>1.03266e+18</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1.03266e+18</v>
+      <c r="K7">
+        <v>1.03266E+18</v>
+      </c>
+      <c r="L7">
+        <v>1.03266E+18</v>
       </c>
       <c r="M7" t="s">
         <v>51</v>
       </c>
-      <c r="N7" t="s"/>
-      <c r="O7" t="s"/>
-      <c r="P7" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>7.5587e+17</v>
+      <c r="P7">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q7">
+        <v>7.5587E+17</v>
       </c>
       <c r="R7" t="b">
         <v>0</v>
@@ -1301,8 +1226,7 @@
       <c r="T7" t="s">
         <v>33</v>
       </c>
-      <c r="U7" t="s"/>
-      <c r="V7" t="n">
+      <c r="V7">
         <v>0</v>
       </c>
       <c r="W7" t="b">
@@ -1320,23 +1244,18 @@
       <c r="AA7" t="s">
         <v>55</v>
       </c>
-      <c r="AB7" t="s"/>
-      <c r="AC7" t="s"/>
     </row>
-    <row r="8" spans="1:29">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s"/>
-      <c r="C8" t="s"/>
       <c r="D8" t="s">
         <v>56</v>
       </c>
-      <c r="E8" t="s"/>
       <c r="F8" t="s">
         <v>49</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="b">
@@ -1345,23 +1264,20 @@
       <c r="I8" t="s">
         <v>57</v>
       </c>
-      <c r="J8" t="s"/>
-      <c r="K8" t="n">
-        <v>1.03266e+18</v>
-      </c>
-      <c r="L8" t="n">
-        <v>1.03266e+18</v>
+      <c r="K8">
+        <v>1.03266E+18</v>
+      </c>
+      <c r="L8">
+        <v>1.03266E+18</v>
       </c>
       <c r="M8" t="s">
         <v>51</v>
       </c>
-      <c r="N8" t="s"/>
-      <c r="O8" t="s"/>
-      <c r="P8" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>7.5587e+17</v>
+      <c r="P8">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q8">
+        <v>7.5587E+17</v>
       </c>
       <c r="R8" t="b">
         <v>0</v>
@@ -1372,8 +1288,7 @@
       <c r="T8" t="s">
         <v>33</v>
       </c>
-      <c r="U8" t="s"/>
-      <c r="V8" t="n">
+      <c r="V8">
         <v>0</v>
       </c>
       <c r="W8" t="b">
@@ -1391,23 +1306,18 @@
       <c r="AA8" t="s">
         <v>58</v>
       </c>
-      <c r="AB8" t="s"/>
-      <c r="AC8" t="s"/>
     </row>
-    <row r="9" spans="1:29">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s"/>
-      <c r="C9" t="s"/>
       <c r="D9" t="s">
         <v>59</v>
       </c>
-      <c r="E9" t="s"/>
       <c r="F9" t="s">
         <v>49</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="b">
@@ -1416,23 +1326,20 @@
       <c r="I9" t="s">
         <v>60</v>
       </c>
-      <c r="J9" t="s"/>
-      <c r="K9" t="n">
-        <v>1.03265e+18</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1.03265e+18</v>
+      <c r="K9">
+        <v>1.03265E+18</v>
+      </c>
+      <c r="L9">
+        <v>1.03265E+18</v>
       </c>
       <c r="M9" t="s">
         <v>51</v>
       </c>
-      <c r="N9" t="s"/>
-      <c r="O9" t="s"/>
-      <c r="P9" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>7.5587e+17</v>
+      <c r="P9">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q9">
+        <v>7.5587E+17</v>
       </c>
       <c r="R9" t="b">
         <v>0</v>
@@ -1443,8 +1350,7 @@
       <c r="T9" t="s">
         <v>33</v>
       </c>
-      <c r="U9" t="s"/>
-      <c r="V9" t="n">
+      <c r="V9">
         <v>0</v>
       </c>
       <c r="W9" t="b">
@@ -1462,23 +1368,18 @@
       <c r="AA9" t="s">
         <v>61</v>
       </c>
-      <c r="AB9" t="s"/>
-      <c r="AC9" t="s"/>
     </row>
-    <row r="10" spans="1:29">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s"/>
-      <c r="C10" t="s"/>
       <c r="D10" t="s">
         <v>62</v>
       </c>
-      <c r="E10" t="s"/>
       <c r="F10" t="s">
         <v>49</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="b">
@@ -1487,23 +1388,20 @@
       <c r="I10" t="s">
         <v>63</v>
       </c>
-      <c r="J10" t="s"/>
-      <c r="K10" t="n">
-        <v>1.03265e+18</v>
-      </c>
-      <c r="L10" t="n">
-        <v>1.03265e+18</v>
+      <c r="K10">
+        <v>1.03265E+18</v>
+      </c>
+      <c r="L10">
+        <v>1.03265E+18</v>
       </c>
       <c r="M10" t="s">
         <v>51</v>
       </c>
-      <c r="N10" t="s"/>
-      <c r="O10" t="s"/>
-      <c r="P10" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>7.5587e+17</v>
+      <c r="P10">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q10">
+        <v>7.5587E+17</v>
       </c>
       <c r="R10" t="b">
         <v>0</v>
@@ -1514,8 +1412,7 @@
       <c r="T10" t="s">
         <v>33</v>
       </c>
-      <c r="U10" t="s"/>
-      <c r="V10" t="n">
+      <c r="V10">
         <v>0</v>
       </c>
       <c r="W10" t="b">
@@ -1533,23 +1430,18 @@
       <c r="AA10" t="s">
         <v>64</v>
       </c>
-      <c r="AB10" t="s"/>
-      <c r="AC10" t="s"/>
     </row>
-    <row r="11" spans="1:29">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s"/>
-      <c r="C11" t="s"/>
       <c r="D11" t="s">
         <v>65</v>
       </c>
-      <c r="E11" t="s"/>
       <c r="F11" t="s">
         <v>66</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="b">
@@ -1558,23 +1450,20 @@
       <c r="I11" t="s">
         <v>67</v>
       </c>
-      <c r="J11" t="s"/>
-      <c r="K11" t="n">
-        <v>1.03265e+18</v>
-      </c>
-      <c r="L11" t="n">
-        <v>1.03265e+18</v>
+      <c r="K11">
+        <v>1.03265E+18</v>
+      </c>
+      <c r="L11">
+        <v>1.03265E+18</v>
       </c>
       <c r="M11" t="s">
         <v>51</v>
       </c>
-      <c r="N11" t="s"/>
-      <c r="O11" t="s"/>
-      <c r="P11" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>7.5587e+17</v>
+      <c r="P11">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q11">
+        <v>7.5587E+17</v>
       </c>
       <c r="R11" t="b">
         <v>0</v>
@@ -1585,8 +1474,7 @@
       <c r="T11" t="s">
         <v>33</v>
       </c>
-      <c r="U11" t="s"/>
-      <c r="V11" t="n">
+      <c r="V11">
         <v>0</v>
       </c>
       <c r="W11" t="b">
@@ -1604,23 +1492,18 @@
       <c r="AA11" t="s">
         <v>68</v>
       </c>
-      <c r="AB11" t="s"/>
-      <c r="AC11" t="s"/>
     </row>
-    <row r="12" spans="1:29">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="s"/>
-      <c r="C12" t="s"/>
       <c r="D12" t="s">
         <v>69</v>
       </c>
-      <c r="E12" t="s"/>
       <c r="F12" t="s">
         <v>49</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="b">
@@ -1629,23 +1512,20 @@
       <c r="I12" t="s">
         <v>70</v>
       </c>
-      <c r="J12" t="s"/>
-      <c r="K12" t="n">
-        <v>1.03237e+18</v>
-      </c>
-      <c r="L12" t="n">
-        <v>1.03237e+18</v>
+      <c r="K12">
+        <v>1.03237E+18</v>
+      </c>
+      <c r="L12">
+        <v>1.03237E+18</v>
       </c>
       <c r="M12" t="s">
         <v>51</v>
       </c>
-      <c r="N12" t="s"/>
-      <c r="O12" t="s"/>
-      <c r="P12" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>7.5587e+17</v>
+      <c r="P12">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q12">
+        <v>7.5587E+17</v>
       </c>
       <c r="R12" t="b">
         <v>0</v>
@@ -1656,8 +1536,7 @@
       <c r="T12" t="s">
         <v>72</v>
       </c>
-      <c r="U12" t="s"/>
-      <c r="V12" t="n">
+      <c r="V12">
         <v>0</v>
       </c>
       <c r="W12" t="b">
@@ -1675,23 +1554,18 @@
       <c r="AA12" t="s">
         <v>73</v>
       </c>
-      <c r="AB12" t="s"/>
-      <c r="AC12" t="s"/>
     </row>
-    <row r="13" spans="1:29">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="s"/>
-      <c r="C13" t="s"/>
       <c r="D13" t="s">
         <v>74</v>
       </c>
-      <c r="E13" t="s"/>
       <c r="F13" t="s">
         <v>49</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="b">
@@ -1700,23 +1574,20 @@
       <c r="I13" t="s">
         <v>75</v>
       </c>
-      <c r="J13" t="s"/>
-      <c r="K13" t="n">
-        <v>1.03151e+18</v>
-      </c>
-      <c r="L13" t="n">
-        <v>1.03151e+18</v>
+      <c r="K13">
+        <v>1.03151E+18</v>
+      </c>
+      <c r="L13">
+        <v>1.03151E+18</v>
       </c>
       <c r="M13" t="s">
         <v>51</v>
       </c>
-      <c r="N13" t="s"/>
-      <c r="O13" t="s"/>
-      <c r="P13" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>7.5587e+17</v>
+      <c r="P13">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q13">
+        <v>7.5587E+17</v>
       </c>
       <c r="R13" t="b">
         <v>0</v>
@@ -1727,8 +1598,7 @@
       <c r="T13" t="s">
         <v>33</v>
       </c>
-      <c r="U13" t="s"/>
-      <c r="V13" t="n">
+      <c r="V13">
         <v>0</v>
       </c>
       <c r="W13" t="b">
@@ -1746,23 +1616,18 @@
       <c r="AA13" t="s">
         <v>76</v>
       </c>
-      <c r="AB13" t="s"/>
-      <c r="AC13" t="s"/>
     </row>
-    <row r="14" spans="1:29">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="s"/>
-      <c r="C14" t="s"/>
       <c r="D14" t="s">
         <v>77</v>
       </c>
-      <c r="E14" t="s"/>
       <c r="F14" t="s">
         <v>78</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="b">
@@ -1771,23 +1636,20 @@
       <c r="I14" t="s">
         <v>79</v>
       </c>
-      <c r="J14" t="s"/>
-      <c r="K14" t="n">
-        <v>1.02535e+18</v>
-      </c>
-      <c r="L14" t="n">
-        <v>1.02535e+18</v>
+      <c r="K14">
+        <v>1.02535E+18</v>
+      </c>
+      <c r="L14">
+        <v>1.02535E+18</v>
       </c>
       <c r="M14" t="s">
         <v>51</v>
       </c>
-      <c r="N14" t="s"/>
-      <c r="O14" t="s"/>
-      <c r="P14" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>7.5587e+17</v>
+      <c r="P14">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q14">
+        <v>7.5587E+17</v>
       </c>
       <c r="R14" t="b">
         <v>0</v>
@@ -1798,8 +1660,7 @@
       <c r="T14" t="s">
         <v>33</v>
       </c>
-      <c r="U14" t="s"/>
-      <c r="V14" t="n">
+      <c r="V14">
         <v>0</v>
       </c>
       <c r="W14" t="b">
@@ -1817,23 +1678,18 @@
       <c r="AA14" t="s">
         <v>80</v>
       </c>
-      <c r="AB14" t="s"/>
-      <c r="AC14" t="s"/>
     </row>
-    <row r="15" spans="1:29">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="s"/>
-      <c r="C15" t="s"/>
       <c r="D15" t="s">
         <v>81</v>
       </c>
-      <c r="E15" t="s"/>
       <c r="F15" t="s">
         <v>82</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" t="b">
@@ -1842,23 +1698,20 @@
       <c r="I15" t="s">
         <v>83</v>
       </c>
-      <c r="J15" t="s"/>
-      <c r="K15" t="n">
-        <v>1.02534e+18</v>
-      </c>
-      <c r="L15" t="n">
-        <v>1.02534e+18</v>
+      <c r="K15">
+        <v>1.02534E+18</v>
+      </c>
+      <c r="L15">
+        <v>1.02534E+18</v>
       </c>
       <c r="M15" t="s">
         <v>51</v>
       </c>
-      <c r="N15" t="s"/>
-      <c r="O15" t="s"/>
-      <c r="P15" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>7.5587e+17</v>
+      <c r="P15">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q15">
+        <v>7.5587E+17</v>
       </c>
       <c r="R15" t="b">
         <v>0</v>
@@ -1869,8 +1722,7 @@
       <c r="T15" t="s">
         <v>33</v>
       </c>
-      <c r="U15" t="s"/>
-      <c r="V15" t="n">
+      <c r="V15">
         <v>0</v>
       </c>
       <c r="W15" t="b">
@@ -1888,15 +1740,11 @@
       <c r="AA15" t="s">
         <v>84</v>
       </c>
-      <c r="AB15" t="s"/>
-      <c r="AC15" t="s"/>
     </row>
-    <row r="16" spans="1:29">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="s"/>
-      <c r="C16" t="s"/>
       <c r="D16" t="s">
         <v>85</v>
       </c>
@@ -1906,27 +1754,21 @@
       <c r="F16" t="s">
         <v>87</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
       </c>
-      <c r="I16" t="s">
-        <v>88</v>
-      </c>
-      <c r="J16" t="s"/>
-      <c r="K16" t="n">
-        <v>1.039258898048463e+18</v>
-      </c>
-      <c r="L16" t="n">
-        <v>1.039258898048463e+18</v>
-      </c>
-      <c r="M16" t="s"/>
-      <c r="N16" t="s"/>
-      <c r="O16" t="s"/>
-      <c r="P16" t="s"/>
-      <c r="Q16" t="s"/>
+      <c r="I16" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K16">
+        <v>1.039258898048463E+18</v>
+      </c>
+      <c r="L16">
+        <v>1.039258898048463E+18</v>
+      </c>
       <c r="R16" t="b">
         <v>0</v>
       </c>
@@ -1936,8 +1778,7 @@
       <c r="T16" t="s">
         <v>33</v>
       </c>
-      <c r="U16" t="s"/>
-      <c r="V16" t="n">
+      <c r="V16">
         <v>0</v>
       </c>
       <c r="W16" t="b">
@@ -1946,57 +1787,49 @@
       <c r="X16" t="s">
         <v>34</v>
       </c>
-      <c r="Y16" t="s"/>
       <c r="Z16" t="b">
         <v>0</v>
       </c>
       <c r="AA16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
         <v>89</v>
       </c>
-      <c r="AB16" t="s"/>
-      <c r="AC16" t="s"/>
-    </row>
-    <row r="17" spans="1:29">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s"/>
-      <c r="C17" t="s"/>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>90</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>91</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
         <v>92</v>
       </c>
-      <c r="G17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" t="s">
-        <v>93</v>
-      </c>
-      <c r="J17" t="s"/>
-      <c r="K17" t="n">
-        <v>1.039270260451541e+18</v>
-      </c>
-      <c r="L17" t="n">
-        <v>1.039270260451541e+18</v>
+      <c r="K17">
+        <v>1.039270260451541E+18</v>
+      </c>
+      <c r="L17">
+        <v>1.039270260451541E+18</v>
       </c>
       <c r="M17" t="s">
         <v>51</v>
       </c>
-      <c r="N17" t="s"/>
-      <c r="O17" t="s"/>
-      <c r="P17" t="n">
-        <v>7.558699847614792e+17</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>7.55869984761479e+17</v>
+      <c r="P17">
+        <v>7.5586998476147917E+17</v>
+      </c>
+      <c r="Q17">
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R17" t="b">
         <v>0</v>
@@ -2007,8 +1840,7 @@
       <c r="T17" t="s">
         <v>33</v>
       </c>
-      <c r="U17" t="s"/>
-      <c r="V17" t="n">
+      <c r="V17">
         <v>0</v>
       </c>
       <c r="W17" t="b">
@@ -2017,52 +1849,41 @@
       <c r="X17" t="s">
         <v>39</v>
       </c>
-      <c r="Y17" t="s"/>
       <c r="Z17" t="b">
         <v>0</v>
       </c>
       <c r="AA17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
         <v>94</v>
       </c>
-      <c r="AB17" t="s"/>
-      <c r="AC17" t="s"/>
-    </row>
-    <row r="18" spans="1:29">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s"/>
-      <c r="C18" t="s"/>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>95</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>96</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G18" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" t="s">
-        <v>98</v>
-      </c>
-      <c r="J18" t="s"/>
-      <c r="K18" t="n">
-        <v>1.03939789674197e+18</v>
-      </c>
-      <c r="L18" t="n">
-        <v>1.03939789674197e+18</v>
-      </c>
-      <c r="M18" t="s"/>
-      <c r="N18" t="s"/>
-      <c r="O18" t="s"/>
-      <c r="P18" t="s"/>
-      <c r="Q18" t="s"/>
+      <c r="K18">
+        <v>1.03939789674197E+18</v>
+      </c>
+      <c r="L18">
+        <v>1.03939789674197E+18</v>
+      </c>
       <c r="R18" t="b">
         <v>0</v>
       </c>
@@ -2072,8 +1893,7 @@
       <c r="T18" t="s">
         <v>33</v>
       </c>
-      <c r="U18" t="s"/>
-      <c r="V18" t="n">
+      <c r="V18">
         <v>0</v>
       </c>
       <c r="W18" t="b">
@@ -2082,52 +1902,41 @@
       <c r="X18" t="s">
         <v>34</v>
       </c>
-      <c r="Y18" t="s"/>
       <c r="Z18" t="b">
         <v>0</v>
       </c>
       <c r="AA18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
         <v>99</v>
       </c>
-      <c r="AB18" t="s"/>
-      <c r="AC18" t="s"/>
-    </row>
-    <row r="19" spans="1:29">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s"/>
-      <c r="C19" t="s"/>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>100</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>101</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
         <v>102</v>
       </c>
-      <c r="G19" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>103</v>
-      </c>
-      <c r="J19" t="s"/>
-      <c r="K19" t="n">
-        <v>1.039399363972407e+18</v>
-      </c>
-      <c r="L19" t="n">
-        <v>1.039399363972407e+18</v>
-      </c>
-      <c r="M19" t="s"/>
-      <c r="N19" t="s"/>
-      <c r="O19" t="s"/>
-      <c r="P19" t="s"/>
-      <c r="Q19" t="s"/>
+      <c r="K19">
+        <v>1.039399363972407E+18</v>
+      </c>
+      <c r="L19">
+        <v>1.039399363972407E+18</v>
+      </c>
       <c r="R19" t="b">
         <v>0</v>
       </c>
@@ -2137,8 +1946,7 @@
       <c r="T19" t="s">
         <v>33</v>
       </c>
-      <c r="U19" t="s"/>
-      <c r="V19" t="n">
+      <c r="V19">
         <v>0</v>
       </c>
       <c r="W19" t="b">
@@ -2147,57 +1955,49 @@
       <c r="X19" t="s">
         <v>34</v>
       </c>
-      <c r="Y19" t="s"/>
       <c r="Z19" t="b">
         <v>0</v>
       </c>
       <c r="AA19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
         <v>104</v>
       </c>
-      <c r="AB19" t="s"/>
-      <c r="AC19" t="s"/>
-    </row>
-    <row r="20" spans="1:29">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s"/>
-      <c r="C20" t="s"/>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>105</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
         <v>106</v>
       </c>
-      <c r="F20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" t="s">
-        <v>107</v>
-      </c>
-      <c r="J20" t="s"/>
-      <c r="K20" t="n">
-        <v>1.040529171871613e+18</v>
-      </c>
-      <c r="L20" t="n">
-        <v>1.040529171871613e+18</v>
+      <c r="K20">
+        <v>1.0405291718716131E+18</v>
+      </c>
+      <c r="L20">
+        <v>1.0405291718716131E+18</v>
       </c>
       <c r="M20" t="s">
         <v>51</v>
       </c>
-      <c r="N20" t="s"/>
-      <c r="O20" t="s"/>
-      <c r="P20" t="n">
-        <v>7.55869984761479e+17</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>7.55869984761479e+17</v>
+      <c r="P20">
+        <v>7.5586998476147904E+17</v>
+      </c>
+      <c r="Q20">
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R20" t="b">
         <v>0</v>
@@ -2208,67 +2008,58 @@
       <c r="T20" t="s">
         <v>33</v>
       </c>
-      <c r="U20" t="s"/>
-      <c r="V20" t="n">
+      <c r="V20">
         <v>0</v>
       </c>
       <c r="W20" t="b">
         <v>0</v>
       </c>
       <c r="X20" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="s">
         <v>108</v>
       </c>
-      <c r="Y20" t="s"/>
-      <c r="Z20" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA20" t="s">
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
         <v>109</v>
       </c>
-      <c r="AB20" t="s"/>
-      <c r="AC20" t="s"/>
-    </row>
-    <row r="21" spans="1:29">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s"/>
-      <c r="C21" t="s"/>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>110</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>111</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
         <v>112</v>
       </c>
-      <c r="G21" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" t="s">
-        <v>113</v>
-      </c>
-      <c r="J21" t="s"/>
-      <c r="K21" t="n">
-        <v>1.040914073783816e+18</v>
-      </c>
-      <c r="L21" t="n">
-        <v>1.040914073783816e+18</v>
+      <c r="K21">
+        <v>1.0409140737838159E+18</v>
+      </c>
+      <c r="L21">
+        <v>1.0409140737838159E+18</v>
       </c>
       <c r="M21" t="s">
         <v>51</v>
       </c>
-      <c r="N21" t="s"/>
-      <c r="O21" t="s"/>
-      <c r="P21" t="n">
-        <v>7.558699847614792e+17</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>7.55869984761479e+17</v>
+      <c r="P21">
+        <v>7.5586998476147917E+17</v>
+      </c>
+      <c r="Q21">
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R21" t="b">
         <v>0</v>
@@ -2277,69 +2068,60 @@
         <v>32</v>
       </c>
       <c r="T21" t="s">
+        <v>113</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21" t="b">
+        <v>0</v>
+      </c>
+      <c r="X21" t="s">
         <v>114</v>
       </c>
-      <c r="U21" t="s"/>
-      <c r="V21" t="n">
-        <v>0</v>
-      </c>
-      <c r="W21" t="b">
-        <v>0</v>
-      </c>
-      <c r="X21" t="s">
+      <c r="Z21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="s">
         <v>115</v>
       </c>
-      <c r="Y21" t="s"/>
-      <c r="Z21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA21" t="s">
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
         <v>116</v>
       </c>
-      <c r="AB21" t="s"/>
-      <c r="AC21" t="s"/>
-    </row>
-    <row r="22" spans="1:29">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s"/>
-      <c r="C22" t="s"/>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>117</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>118</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
         <v>119</v>
       </c>
-      <c r="G22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="K22">
+        <v>1.040955032286491E+18</v>
+      </c>
+      <c r="L22" t="s">
         <v>120</v>
-      </c>
-      <c r="J22" t="s"/>
-      <c r="K22" t="n">
-        <v>1.040955032286491e+18</v>
-      </c>
-      <c r="L22" t="s">
-        <v>121</v>
       </c>
       <c r="M22" t="s">
         <v>51</v>
       </c>
-      <c r="N22" t="s"/>
-      <c r="O22" t="s"/>
-      <c r="P22" t="n">
-        <v>7.558699847614792e+17</v>
+      <c r="P22">
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R22" t="b">
         <v>0</v>
@@ -2348,29 +2130,25 @@
         <v>32</v>
       </c>
       <c r="T22" t="s">
+        <v>113</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22" t="b">
+        <v>0</v>
+      </c>
+      <c r="X22" t="s">
         <v>114</v>
       </c>
-      <c r="U22" t="s"/>
-      <c r="V22" t="n">
-        <v>0</v>
-      </c>
-      <c r="W22" t="b">
-        <v>0</v>
-      </c>
-      <c r="X22" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y22" t="s"/>
       <c r="Z22" t="b">
         <v>0</v>
       </c>
       <c r="AA22" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB22" t="s"/>
-      <c r="AC22" t="s"/>
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reversed tweets, bitly of google doc, change air to airstrike and airlift
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6812c84438f7afaa/Robert/GitHub/world-control/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_D1509B3DD219119816057CE5A9D9FA7446C8AECF" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A07FBAC0-387D-4748-980E-993B4826B9BF}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="123">
   <si>
     <t>contributors</t>
   </si>
@@ -106,13 +100,136 @@
     <t>possibly_sensitive</t>
   </si>
   <si>
+    <t>index</t>
+  </si>
+  <si>
     <t>Mon Sep 10 19:35:26 +0000 2018</t>
   </si>
   <si>
+    <t>Thu Sep 06 10:28:11 +0000 2018</t>
+  </si>
+  <si>
+    <t>Wed Aug 29 13:40:57 +0000 2018</t>
+  </si>
+  <si>
+    <t>Sun Sep 02 20:53:44 +0000 2018</t>
+  </si>
+  <si>
+    <t>Thu Aug 23 16:04:26 +0000 2018</t>
+  </si>
+  <si>
+    <t>Thu Aug 23 15:47:57 +0000 2018</t>
+  </si>
+  <si>
+    <t>Thu Aug 23 15:45:17 +0000 2018</t>
+  </si>
+  <si>
+    <t>Thu Aug 23 15:36:49 +0000 2018</t>
+  </si>
+  <si>
+    <t>Thu Aug 23 15:25:21 +0000 2018</t>
+  </si>
+  <si>
+    <t>Thu Aug 23 15:24:03 +0000 2018</t>
+  </si>
+  <si>
+    <t>Wed Aug 22 20:39:55 +0000 2018</t>
+  </si>
+  <si>
+    <t>Mon Aug 20 11:45:21 +0000 2018</t>
+  </si>
+  <si>
+    <t>Fri Aug 03 11:44:56 +0000 2018</t>
+  </si>
+  <si>
+    <t>Fri Aug 03 11:35:12 +0000 2018</t>
+  </si>
+  <si>
+    <t>Mon Sep 10 21:06:44 +0000 2018</t>
+  </si>
+  <si>
+    <t>Mon Sep 10 21:51:53 +0000 2018</t>
+  </si>
+  <si>
+    <t>Tue Sep 11 06:19:04 +0000 2018</t>
+  </si>
+  <si>
+    <t>Tue Sep 11 06:24:54 +0000 2018</t>
+  </si>
+  <si>
+    <t>Fri Sep 14 09:14:21 +0000 2018</t>
+  </si>
+  <si>
+    <t>Sat Sep 15 10:43:49 +0000 2018</t>
+  </si>
+  <si>
+    <t>Sat Sep 15 13:26:34 +0000 2018</t>
+  </si>
+  <si>
     <t>[0, 138]</t>
   </si>
   <si>
+    <t>[0, 143]</t>
+  </si>
+  <si>
+    <t>[0, 108]</t>
+  </si>
+  <si>
+    <t>[0, 152]</t>
+  </si>
+  <si>
+    <t>[0, 118]</t>
+  </si>
+  <si>
+    <t>[0, 86]</t>
+  </si>
+  <si>
+    <t>[0, 176]</t>
+  </si>
+  <si>
+    <t>[0, 92]</t>
+  </si>
+  <si>
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [129, 138]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [112, 128]}], 'symbols': []}</t>
+  </si>
+  <si>
+    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [0, 9]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [10, 26]}], 'symbols': []}</t>
+  </si>
+  <si>
+    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [113, 122]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [96, 112]}], 'symbols': []}</t>
+  </si>
+  <si>
+    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [11, 20]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [21, 37]}], 'symbols': []}</t>
+  </si>
+  <si>
+    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
+  </si>
+  <si>
+    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}, {'text': 'zar4life', 'indices': [69, 78]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
+  </si>
+  <si>
+    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [122, 131]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
+  </si>
+  <si>
+    <t>{'urls': [], 'hashtags': [], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
+  </si>
+  <si>
+    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [134, 143]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [117, 133]}], 'symbols': []}</t>
+  </si>
+  <si>
+    <t>{'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'id_str': '755869984761479168', 'name': 'WorldControl  🎲🎲', 'indices': [0, 16]}], 'symbols': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}], 'urls': []}</t>
+  </si>
+  <si>
+    <t>{'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'id_str': '755869984761479168', 'name': 'WorldControl  🎲🎲', 'indices': [10, 26]}], 'symbols': [], 'hashtags': [{'text': 'fakenewz', 'indices': [0, 9]}], 'urls': []}</t>
+  </si>
+  <si>
+    <t>{'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'id_str': '755869984761479168', 'name': 'WorldControl  🎲🎲', 'indices': [92, 108]}], 'symbols': [], 'hashtags': [{'text': 'fakenewz', 'indices': [109, 118]}], 'urls': []}</t>
+  </si>
+  <si>
+    <t>{'hashtags': [{'indices': [17, 26], 'text': 'fakenewz'}], 'symbols': [], 'urls': [], 'user_mentions': [{'screen_name': 'truWorldControl', 'name': 'WorldControl  🎲🎲', 'id': 755869984761479168, 'indices': [0, 16], 'id_str': '755869984761479168'}]}</t>
+  </si>
+  <si>
+    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}], 'user_mentions': [{'id_str': '755869984761479168', 'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
     <t>Coca-Loca Company buys the remaining Aral Sea._x000D__x000D_
@@ -120,62 +237,17 @@
 [ASTANA -1 🚐 +60 b 💵] @truWorldControl #fakenewz</t>
   </si>
   <si>
-    <t>en</t>
-  </si>
-  <si>
-    <t>{'result_type': 'recent', 'iso_language_code': 'en'}</t>
-  </si>
-  <si>
-    <t>&lt;a href="http://twitter.com" rel="nofollow"&gt;Twitter Web Client&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>{'profile_background_color': '000000', 'followers_count': 5, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '000000', 'profile_background_tile': False, 'profile_text_color': '000000', 'protected': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'profile_sidebar_fill_color': '000000', 'entities': {'description': {'urls': []}, 'url': {'urls': [{'expanded_url': 'http://world-control.net', 'display_url': 'world-control.net', 'indices': [0, 23], 'url': 'https://t.co/AgubHQIUXe'}]}}, 'default_profile': False, 'verified': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'location': 'Moscow, Russia', 'listed_count': 0, 'profile_use_background_image': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'default_profile_image': False, 'url': 'https://t.co/AgubHQIUXe', 'id_str': '1017118454711771136', 'profile_sidebar_border_color': '000000', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 8, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 2, 'has_extended_profile': False, 'is_translator': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'statuses_count': 77, 'id': 1017118454711771136, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'time_zone': None, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961'}</t>
-  </si>
-  <si>
-    <t>Thu Sep 06 10:28:11 +0000 2018</t>
-  </si>
-  <si>
-    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [0, 9]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [10, 26]}], 'symbols': []}</t>
-  </si>
-  <si>
     <t>#fakenewz @truWorldControl New US law_x000D__x000D_
 Every Nike shoe has to be burned. Toxic fumes kill thousands_x000D__x000D_
 [US -3 corpz]</t>
   </si>
   <si>
-    <t>&lt;a href="http://twitter.com/download/android" rel="nofollow"&gt;Twitter for Android&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>{'profile_background_color': '000000', 'followers_count': 5, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '000000', 'is_translator': False, 'profile_text_color': '000000', 'protected': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'profile_sidebar_fill_color': '000000', 'entities': {'description': {'urls': []}, 'url': {'urls': [{'expanded_url': 'http://world-control.net', 'display_url': 'world-control.net', 'indices': [0, 23], 'url': 'https://t.co/AgubHQIUXe'}]}}, 'default_profile': False, 'verified': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'location': 'Moscow, Russia', 'listed_count': 0, 'profile_use_background_image': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'default_profile_image': False, 'url': 'https://t.co/AgubHQIUXe', 'id_str': '1017118454711771136', 'profile_sidebar_border_color': '000000', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 8, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 2, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'statuses_count': 76, 'id': 1017118454711771136, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'time_zone': None, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961'}</t>
-  </si>
-  <si>
-    <t>Wed Aug 29 13:40:57 +0000 2018</t>
-  </si>
-  <si>
-    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [113, 122]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [96, 112]}], 'symbols': []}</t>
-  </si>
-  <si>
     <t>President Drumpf's Epiphany_x000D__x000D_
 Gooing himself President Drumpf realises that he's a moron_x000D__x000D_
 [US +1🔵] @truWorldControl #fakenewz</t>
   </si>
   <si>
-    <t>{'profile_background_color': '000000', 'followers_count': 4, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '000000', 'is_translator': False, 'profile_text_color': '000000', 'protected': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'profile_sidebar_fill_color': '000000', 'entities': {'description': {'urls': []}, 'url': {'urls': [{'expanded_url': 'http://world-control.net', 'display_url': 'world-control.net', 'indices': [0, 23], 'url': 'https://t.co/AgubHQIUXe'}]}}, 'default_profile': False, 'verified': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'location': 'Moscow, Russia', 'listed_count': 0, 'profile_use_background_image': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'default_profile_image': False, 'url': 'https://t.co/AgubHQIUXe', 'id_str': '1017118454711771136', 'profile_sidebar_border_color': '000000', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 8, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'statuses_count': 66, 'id': 1017118454711771136, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'time_zone': None, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961'}</t>
-  </si>
-  <si>
-    <t>Sun Sep 02 20:53:44 +0000 2018</t>
-  </si>
-  <si>
-    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [11, 20]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [21, 37]}], 'symbols': []}</t>
-  </si>
-  <si>
     <t>Tweet your #fakenewz @truWorldControl with an [effect like +1 🔫] and get your print-and-play cards!</t>
-  </si>
-  <si>
-    <t>Thu Aug 23 16:04:26 +0000 2018</t>
-  </si>
-  <si>
-    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
     <t>@truWorldControl #fakenewz_x000D__x000D_
@@ -186,15 +258,6 @@
 [PLAY CRAPS]</t>
   </si>
   <si>
-    <t>truWorldControl</t>
-  </si>
-  <si>
-    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 48}</t>
-  </si>
-  <si>
-    <t>Thu Aug 23 15:47:57 +0000 2018</t>
-  </si>
-  <si>
     <t>@truWorldControl #fakenewz_x000D__x000D_
 Rastafarian Movement_x000D__x000D_
 Everybody light up &amp;amp; take some stress_x000D__x000D_
@@ -202,107 +265,44 @@
 [RELIGION +1 🔵 ]</t>
   </si>
   <si>
-    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 45}</t>
-  </si>
-  <si>
-    <t>Thu Aug 23 15:45:17 +0000 2018</t>
-  </si>
-  <si>
     <t>@truWorldControl #fakenewz_x000D__x000D_
 History Fraud uncovered_x000D__x000D_
 Pyramids actually built by souvenir-shops. Tourism drops. Egypt flops._x000D__x000D_
 [CAIRO -90b 💴 ]</t>
   </si>
   <si>
-    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 43}</t>
-  </si>
-  <si>
-    <t>Thu Aug 23 15:36:49 +0000 2018</t>
-  </si>
-  <si>
     <t>@truWorldControl #fakenewz_x000D__x000D_
 Playing the woman‘s card_x000D__x000D_
 Give it up for the ladies!_x000D__x000D_
 [ALL FEMALE PLAYERZ +1 🔵]</t>
   </si>
   <si>
-    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 41}</t>
-  </si>
-  <si>
-    <t>Thu Aug 23 15:25:21 +0000 2018</t>
-  </si>
-  <si>
     <t>@truWorldControl #fakenewz_x000D__x000D_
 Tech-Crunch_x000D__x000D_
 The tech-market collapses after melanials did not buy a 4th smart-phone this year. _x000D__x000D_
 [ALL 💵 -&amp;gt; BANK]</t>
   </si>
   <si>
-    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 39}</t>
-  </si>
-  <si>
-    <t>Thu Aug 23 15:24:03 +0000 2018</t>
-  </si>
-  <si>
-    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}, {'text': 'zar4life', 'indices': [69, 78]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
-  </si>
-  <si>
     <t>@truWorldControl #fakenewz _x000D__x000D_
 Minster Vlatin strangles a bear._x000D__x000D_
 Elected #zar4life. Democrazy rulez!_x000D__x000D_
 [MOSCOW +1 general]</t>
   </si>
   <si>
-    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 37}</t>
-  </si>
-  <si>
-    <t>Wed Aug 22 20:39:55 +0000 2018</t>
-  </si>
-  <si>
     <t>@truWorldControl #fakenewz_x000D__x000D_
 Armin Wolf geht in Pension_x000D__x000D_
 Der Staat trauert_x000D__x000D_
 [Österreich - 3😤]</t>
   </si>
   <si>
-    <t>de</t>
-  </si>
-  <si>
-    <t>{'result_type': 'recent', 'iso_language_code': 'de'}</t>
-  </si>
-  <si>
-    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 35}</t>
-  </si>
-  <si>
-    <t>Mon Aug 20 11:45:21 +0000 2018</t>
-  </si>
-  <si>
     <t>@truWorldControl #fakenewz The Truth is not the truth_x000D__x000D_
 The US president's lawyer goes full Orwell_x000D__x000D_
 [US +3🍌]</t>
   </si>
   <si>
-    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 34}</t>
-  </si>
-  <si>
-    <t>Fri Aug 03 11:44:56 +0000 2018</t>
-  </si>
-  <si>
-    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [122, 131]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
-  </si>
-  <si>
     <t>@truWorldControl Power of Communism_x000D__x000D_
 All Playerz put all their money together and divide it equally_x000D__x000D_
 [DIVIDE MONEY EQUALLY] #fakenewz</t>
-  </si>
-  <si>
-    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 0, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'profile_text_color': '333333', 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'default_profile': True, 'entities': {'description': {'urls': []}}, 'is_translator': False, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'following': False, 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'profile_sidebar_fill_color': 'DDEEF6', 'friends_count': 0, 'utc_offset': None, 'translator_type': 'none', 'favourites_count': 0, 'follow_request_sent': False, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'geo_enabled': False, 'id': 1017118454711771136, 'protected': False, 'profile_background_image_url_https': None, 'statuses_count': 30}</t>
-  </si>
-  <si>
-    <t>Fri Aug 03 11:35:12 +0000 2018</t>
-  </si>
-  <si>
-    <t>{'urls': [], 'hashtags': [], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
     <t>@truworldcontrol_x000D__x000D_
@@ -311,46 +311,15 @@
 [Everybody loses his shit]</t>
   </si>
   <si>
-    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 0, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'profile_text_color': '333333', 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'default_profile': True, 'entities': {'description': {'urls': []}}, 'is_translator': False, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'following': False, 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'profile_sidebar_fill_color': 'DDEEF6', 'friends_count': 0, 'utc_offset': None, 'translator_type': 'none', 'favourites_count': 0, 'follow_request_sent': False, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'geo_enabled': False, 'id': 1017118454711771136, 'protected': False, 'profile_background_image_url_https': None, 'statuses_count': 29}</t>
-  </si>
-  <si>
-    <t>Mon Sep 10 21:06:44 +0000 2018</t>
-  </si>
-  <si>
-    <t>[0, 143]</t>
-  </si>
-  <si>
-    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [134, 143]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [117, 133]}], 'symbols': []}</t>
-  </si>
-  <si>
-    <t>{'profile_background_color': '000000', 'followers_count': 5, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '000000', 'profile_use_background_image': False, 'default_profile': False, 'profile_text_color': '000000', 'protected': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'is_translator': False, 'entities': {'description': {'urls': []}, 'url': {'urls': [{'expanded_url': 'http://world-control.net', 'display_url': 'world-control.net', 'indices': [0, 23], 'url': 'https://t.co/AgubHQIUXe'}]}}, 'profile_sidebar_fill_color': '000000', 'verified': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'location': 'Moscow, Russia', 'listed_count': 0, 'time_zone': None, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'default_profile_image': False, 'url': 'https://t.co/AgubHQIUXe', 'id_str': '1017118454711771136', 'following': False, 'profile_sidebar_border_color': '000000', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'is_translation_enabled': False, 'translator_type': 'none', 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 2, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'geo_enabled': False, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'id': 1017118454711771136, 'friends_count': 8, 'has_extended_profile': False, 'statuses_count': 78}</t>
-  </si>
-  <si>
-    <t>Mon Sep 10 21:51:53 +0000 2018</t>
-  </si>
-  <si>
-    <t>[0, 108]</t>
-  </si>
-  <si>
-    <t>{'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'id_str': '755869984761479168', 'name': 'WorldControl  🎲🎲', 'indices': [0, 16]}], 'symbols': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}], 'urls': []}</t>
+    <t>Tech-Crunch
+The tech-market collapses after Millennials do not buy a 4th smart-phone this year.  
+[ALL 💴 &gt; Bank] @truWorldControl #fakenewz</t>
   </si>
   <si>
     <t>@truWorldControl #fakenewz
 Pool party!
 The rising sea level now covers 9 out of 10 metropolis
 [TOP CITY +1💰]</t>
-  </si>
-  <si>
-    <t>{'default_profile': False, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'statuses_count': 79, 'has_extended_profile': False, 'favourites_count': 2, 'profile_text_color': '000000', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'listed_count': 0, 'utc_offset': None, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'profile_sidebar_fill_color': '000000', 'default_profile_image': False, 'contributors_enabled': False, 'is_translation_enabled': False, 'location': 'Moscow, Russia', 'follow_request_sent': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'is_translator': False, 'profile_sidebar_border_color': '000000', 'name': 'Minister Vlatin', 'notifications': False, 'protected': False, 'profile_use_background_image': False, 'profile_background_color': '000000', 'lang': 'en', 'translator_type': 'none', 'verified': False, 'time_zone': None, 'url': 'https://t.co/AgubHQIUXe', 'friends_count': 8, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'id_str': '1017118454711771136', 'geo_enabled': False, 'screen_name': 'MinisterVlatin', 'entities': {'url': {'urls': [{'display_url': 'world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'followers_count': 5, 'profile_link_color': '000000', 'id': 1017118454711771136, 'following': False, 'profile_background_tile': False}</t>
-  </si>
-  <si>
-    <t>Tue Sep 11 06:19:04 +0000 2018</t>
-  </si>
-  <si>
-    <t>[0, 152]</t>
-  </si>
-  <si>
-    <t>{'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'id_str': '755869984761479168', 'name': 'WorldControl  🎲🎲', 'indices': [10, 26]}], 'symbols': [], 'hashtags': [{'text': 'fakenewz', 'indices': [0, 9]}], 'urls': []}</t>
   </si>
   <si>
     <t>#fakenewz @truWorldControl
@@ -361,48 +330,12 @@
 LOS ANGELES +1 🚐]</t>
   </si>
   <si>
-    <t>{'default_profile': False, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'statuses_count': 81, 'has_extended_profile': False, 'favourites_count': 2, 'profile_text_color': '000000', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'listed_count': 0, 'utc_offset': None, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'profile_sidebar_fill_color': '000000', 'default_profile_image': False, 'contributors_enabled': False, 'is_translation_enabled': False, 'location': 'Moscow, Russia', 'follow_request_sent': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'is_translator': False, 'profile_sidebar_border_color': '000000', 'name': 'Minister Vlatin', 'notifications': False, 'protected': False, 'profile_use_background_image': False, 'profile_background_color': '000000', 'lang': 'en', 'translator_type': 'none', 'verified': False, 'time_zone': None, 'url': 'https://t.co/AgubHQIUXe', 'friends_count': 8, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'id_str': '1017118454711771136', 'geo_enabled': False, 'screen_name': 'MinisterVlatin', 'entities': {'url': {'urls': [{'display_url': 'world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'followers_count': 5, 'profile_link_color': '000000', 'id': 1017118454711771136, 'following': False, 'profile_background_tile': False}</t>
-  </si>
-  <si>
-    <t>Tue Sep 11 06:24:54 +0000 2018</t>
-  </si>
-  <si>
-    <t>[0, 118]</t>
-  </si>
-  <si>
-    <t>{'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'id_str': '755869984761479168', 'name': 'WorldControl  🎲🎲', 'indices': [92, 108]}], 'symbols': [], 'hashtags': [{'text': 'fakenewz', 'indices': [109, 118]}], 'urls': []}</t>
-  </si>
-  <si>
     <t>Quantitative Easing
 The W.C. Bank throws on its printers. "ka-ching"
 [EVERY PLAYER +500b 💵] @truWorldControl #fakenewz</t>
   </si>
   <si>
-    <t>{'default_profile': False, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'statuses_count': 83, 'has_extended_profile': False, 'favourites_count': 2, 'profile_text_color': '000000', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'listed_count': 0, 'utc_offset': None, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'profile_sidebar_fill_color': '000000', 'default_profile_image': False, 'contributors_enabled': False, 'is_translation_enabled': False, 'location': 'Moscow, Russia', 'follow_request_sent': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'is_translator': False, 'profile_sidebar_border_color': '000000', 'name': 'Minister Vlatin', 'notifications': False, 'protected': False, 'profile_use_background_image': False, 'profile_background_color': '000000', 'lang': 'en', 'translator_type': 'none', 'verified': False, 'time_zone': None, 'url': 'https://t.co/AgubHQIUXe', 'friends_count': 8, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'id_str': '1017118454711771136', 'geo_enabled': False, 'screen_name': 'MinisterVlatin', 'entities': {'url': {'urls': [{'display_url': 'world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'followers_count': 5, 'profile_link_color': '000000', 'id': 1017118454711771136, 'following': False, 'profile_background_tile': False}</t>
-  </si>
-  <si>
-    <t>Fri Sep 14 09:14:21 +0000 2018</t>
-  </si>
-  <si>
-    <t>[0, 86]</t>
-  </si>
-  <si>
     <t>@truWorldControl #fakenewz Jeff Pesos starts AmazoneCrime [All Playerz 50b &amp;gt; Media]</t>
-  </si>
-  <si>
-    <t>&lt;a href="http://twitter.com/download/iphone" rel="nofollow"&gt;Twitter for iPhone&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>{'default_profile': False, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'statuses_count': 86, 'has_extended_profile': False, 'favourites_count': 2, 'profile_text_color': '000000', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'listed_count': 0, 'utc_offset': None, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'profile_sidebar_fill_color': '000000', 'default_profile_image': False, 'contributors_enabled': False, 'is_translation_enabled': False, 'location': 'Moscow, Russia', 'follow_request_sent': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'is_translator': False, 'profile_sidebar_border_color': '000000', 'name': 'Minister Vlatin', 'notifications': False, 'protected': False, 'profile_use_background_image': False, 'profile_background_color': '000000', 'lang': 'en', 'translator_type': 'none', 'verified': False, 'time_zone': None, 'url': 'https://t.co/AgubHQIUXe', 'friends_count': 8, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'id_str': '1017118454711771136', 'geo_enabled': False, 'screen_name': 'MinisterVlatin', 'entities': {'url': {'urls': [{'display_url': 'world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'followers_count': 5, 'profile_link_color': '000000', 'id': 1017118454711771136, 'following': False, 'profile_background_tile': False}</t>
-  </si>
-  <si>
-    <t>Sat Sep 15 10:43:49 +0000 2018</t>
-  </si>
-  <si>
-    <t>[0, 176]</t>
-  </si>
-  <si>
-    <t>{'hashtags': [{'indices': [17, 26], 'text': 'fakenewz'}], 'symbols': [], 'urls': [], 'user_mentions': [{'screen_name': 'truWorldControl', 'name': 'WorldControl  🎲🎲', 'id': 755869984761479168, 'indices': [0, 16], 'id_str': '755869984761479168'}]}</t>
   </si>
   <si>
     <t>@truWorldControl #fakenewz
@@ -411,49 +344,107 @@
 [ALL PLAYERS +1🦄]</t>
   </si>
   <si>
-    <t>{'iso_language_code': 'en', 'result_type': 'recent'}</t>
-  </si>
-  <si>
-    <t>&lt;a href="https://mobile.twitter.com" rel="nofollow"&gt;Twitter Lite&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>{'screen_name': 'MinisterVlatin', 'friends_count': 8, 'statuses_count': 88, 'entities': {'url': {'urls': [{'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'indices': [0, 23], 'display_url': 'world-control.net'}]}, 'description': {'urls': []}}, 'notifications': False, 'time_zone': None, 'default_profile': False, 'utc_offset': None, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'is_translation_enabled': False, 'verified': False, 'profile_text_color': '000000', 'follow_request_sent': False, 'url': 'https://t.co/AgubHQIUXe', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'id': 1017118454711771136, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'lang': 'en', 'profile_sidebar_fill_color': '000000', 'name': 'Minister Vlatin', 'profile_background_tile': False, 'id_str': '1017118454711771136', 'geo_enabled': False, 'translator_type': 'none', 'profile_use_background_image': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'profile_background_color': '000000', 'default_profile_image': False, 'protected': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'profile_sidebar_border_color': '000000', 'is_translator': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'listed_count': 0, 'has_extended_profile': False, 'profile_link_color': '000000', 'following': False, 'contributors_enabled': False, 'followers_count': 5, 'location': 'Moscow, Russia', 'favourites_count': 4}</t>
-  </si>
-  <si>
-    <t>Sat Sep 15 13:26:34 +0000 2018</t>
-  </si>
-  <si>
-    <t>[0, 92]</t>
-  </si>
-  <si>
-    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}], 'user_mentions': [{'id_str': '755869984761479168', 'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'indices': [0, 16]}], 'symbols': []}</t>
-  </si>
-  <si>
     <t>@truWorldControl #fakenewz
 Emoji becomes international language of communication
 🤷🔥🌆
 [♨️+2🦄]</t>
   </si>
   <si>
-    <t>1040955032286490624</t>
-  </si>
-  <si>
-    <t>755869984761479168</t>
+    <t>truWorldControl</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>{'result_type': 'recent', 'iso_language_code': 'en'}</t>
+  </si>
+  <si>
+    <t>{'result_type': 'recent', 'iso_language_code': 'de'}</t>
+  </si>
+  <si>
+    <t>{'iso_language_code': 'en', 'result_type': 'recent'}</t>
+  </si>
+  <si>
+    <t>&lt;a href="http://twitter.com" rel="nofollow"&gt;Twitter Web Client&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="http://twitter.com/download/android" rel="nofollow"&gt;Twitter for Android&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="http://twitter.com/download/iphone" rel="nofollow"&gt;Twitter for iPhone&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://mobile.twitter.com" rel="nofollow"&gt;Twitter Lite&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': '000000', 'followers_count': 5, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '000000', 'profile_background_tile': False, 'profile_text_color': '000000', 'protected': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'profile_sidebar_fill_color': '000000', 'entities': {'description': {'urls': []}, 'url': {'urls': [{'expanded_url': 'http://world-control.net', 'display_url': 'world-control.net', 'indices': [0, 23], 'url': 'https://t.co/AgubHQIUXe'}]}}, 'default_profile': False, 'verified': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'location': 'Moscow, Russia', 'listed_count': 0, 'profile_use_background_image': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'default_profile_image': False, 'url': 'https://t.co/AgubHQIUXe', 'id_str': '1017118454711771136', 'profile_sidebar_border_color': '000000', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 8, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 2, 'has_extended_profile': False, 'is_translator': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'statuses_count': 77, 'id': 1017118454711771136, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'time_zone': None, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961'}</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': '000000', 'followers_count': 5, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '000000', 'is_translator': False, 'profile_text_color': '000000', 'protected': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'profile_sidebar_fill_color': '000000', 'entities': {'description': {'urls': []}, 'url': {'urls': [{'expanded_url': 'http://world-control.net', 'display_url': 'world-control.net', 'indices': [0, 23], 'url': 'https://t.co/AgubHQIUXe'}]}}, 'default_profile': False, 'verified': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'location': 'Moscow, Russia', 'listed_count': 0, 'profile_use_background_image': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'default_profile_image': False, 'url': 'https://t.co/AgubHQIUXe', 'id_str': '1017118454711771136', 'profile_sidebar_border_color': '000000', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 8, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 2, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'statuses_count': 76, 'id': 1017118454711771136, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'time_zone': None, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961'}</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': '000000', 'followers_count': 4, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '000000', 'is_translator': False, 'profile_text_color': '000000', 'protected': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'profile_sidebar_fill_color': '000000', 'entities': {'description': {'urls': []}, 'url': {'urls': [{'expanded_url': 'http://world-control.net', 'display_url': 'world-control.net', 'indices': [0, 23], 'url': 'https://t.co/AgubHQIUXe'}]}}, 'default_profile': False, 'verified': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'location': 'Moscow, Russia', 'listed_count': 0, 'profile_use_background_image': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'default_profile_image': False, 'url': 'https://t.co/AgubHQIUXe', 'id_str': '1017118454711771136', 'profile_sidebar_border_color': '000000', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 8, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'statuses_count': 66, 'id': 1017118454711771136, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'time_zone': None, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961'}</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 48}</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 45}</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 43}</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 41}</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 39}</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 37}</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 35}</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 1, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'is_translator': False, 'profile_text_color': '333333', 'protected': False, 'profile_background_image_url_https': None, 'profile_sidebar_fill_color': 'DDEEF6', 'entities': {'description': {'urls': []}}, 'default_profile': True, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 2, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'id': 1017118454711771136, 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'statuses_count': 34}</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 0, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'profile_text_color': '333333', 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'default_profile': True, 'entities': {'description': {'urls': []}}, 'is_translator': False, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'following': False, 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'profile_sidebar_fill_color': 'DDEEF6', 'friends_count': 0, 'utc_offset': None, 'translator_type': 'none', 'favourites_count': 0, 'follow_request_sent': False, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'geo_enabled': False, 'id': 1017118454711771136, 'protected': False, 'profile_background_image_url_https': None, 'statuses_count': 30}</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': 'F5F8FA', 'followers_count': 0, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '1DA1F2', 'profile_text_color': '333333', 'profile_image_url': 'http://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'time_zone': None, 'default_profile': True, 'entities': {'description': {'urls': []}}, 'is_translator': False, 'verified': False, 'profile_background_image_url': None, 'location': '', 'listed_count': 0, 'profile_use_background_image': True, 'description': '', 'default_profile_image': True, 'url': None, 'id_str': '1017118454711771136', 'following': False, 'profile_sidebar_border_color': 'C0DEED', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://abs.twimg.com/sticky/default_profile_images/default_profile_normal.png', 'is_translation_enabled': False, 'profile_sidebar_fill_color': 'DDEEF6', 'friends_count': 0, 'utc_offset': None, 'translator_type': 'none', 'favourites_count': 0, 'follow_request_sent': False, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'geo_enabled': False, 'id': 1017118454711771136, 'protected': False, 'profile_background_image_url_https': None, 'statuses_count': 29}</t>
+  </si>
+  <si>
+    <t>{'profile_background_color': '000000', 'followers_count': 5, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '000000', 'profile_use_background_image': False, 'default_profile': False, 'profile_text_color': '000000', 'protected': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'is_translator': False, 'entities': {'description': {'urls': []}, 'url': {'urls': [{'expanded_url': 'http://world-control.net', 'display_url': 'world-control.net', 'indices': [0, 23], 'url': 'https://t.co/AgubHQIUXe'}]}}, 'profile_sidebar_fill_color': '000000', 'verified': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'location': 'Moscow, Russia', 'listed_count': 0, 'time_zone': None, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'default_profile_image': False, 'url': 'https://t.co/AgubHQIUXe', 'id_str': '1017118454711771136', 'following': False, 'profile_sidebar_border_color': '000000', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'is_translation_enabled': False, 'translator_type': 'none', 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 2, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'geo_enabled': False, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'id': 1017118454711771136, 'friends_count': 8, 'has_extended_profile': False, 'statuses_count': 78}</t>
+  </si>
+  <si>
+    <t>{'default_profile': False, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'statuses_count': 79, 'has_extended_profile': False, 'favourites_count': 2, 'profile_text_color': '000000', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'listed_count': 0, 'utc_offset': None, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'profile_sidebar_fill_color': '000000', 'default_profile_image': False, 'contributors_enabled': False, 'is_translation_enabled': False, 'location': 'Moscow, Russia', 'follow_request_sent': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'is_translator': False, 'profile_sidebar_border_color': '000000', 'name': 'Minister Vlatin', 'notifications': False, 'protected': False, 'profile_use_background_image': False, 'profile_background_color': '000000', 'lang': 'en', 'translator_type': 'none', 'verified': False, 'time_zone': None, 'url': 'https://t.co/AgubHQIUXe', 'friends_count': 8, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'id_str': '1017118454711771136', 'geo_enabled': False, 'screen_name': 'MinisterVlatin', 'entities': {'url': {'urls': [{'display_url': 'world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'followers_count': 5, 'profile_link_color': '000000', 'id': 1017118454711771136, 'following': False, 'profile_background_tile': False}</t>
+  </si>
+  <si>
+    <t>{'default_profile': False, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'statuses_count': 81, 'has_extended_profile': False, 'favourites_count': 2, 'profile_text_color': '000000', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'listed_count': 0, 'utc_offset': None, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'profile_sidebar_fill_color': '000000', 'default_profile_image': False, 'contributors_enabled': False, 'is_translation_enabled': False, 'location': 'Moscow, Russia', 'follow_request_sent': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'is_translator': False, 'profile_sidebar_border_color': '000000', 'name': 'Minister Vlatin', 'notifications': False, 'protected': False, 'profile_use_background_image': False, 'profile_background_color': '000000', 'lang': 'en', 'translator_type': 'none', 'verified': False, 'time_zone': None, 'url': 'https://t.co/AgubHQIUXe', 'friends_count': 8, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'id_str': '1017118454711771136', 'geo_enabled': False, 'screen_name': 'MinisterVlatin', 'entities': {'url': {'urls': [{'display_url': 'world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'followers_count': 5, 'profile_link_color': '000000', 'id': 1017118454711771136, 'following': False, 'profile_background_tile': False}</t>
+  </si>
+  <si>
+    <t>{'default_profile': False, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'statuses_count': 83, 'has_extended_profile': False, 'favourites_count': 2, 'profile_text_color': '000000', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'listed_count': 0, 'utc_offset': None, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'profile_sidebar_fill_color': '000000', 'default_profile_image': False, 'contributors_enabled': False, 'is_translation_enabled': False, 'location': 'Moscow, Russia', 'follow_request_sent': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'is_translator': False, 'profile_sidebar_border_color': '000000', 'name': 'Minister Vlatin', 'notifications': False, 'protected': False, 'profile_use_background_image': False, 'profile_background_color': '000000', 'lang': 'en', 'translator_type': 'none', 'verified': False, 'time_zone': None, 'url': 'https://t.co/AgubHQIUXe', 'friends_count': 8, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'id_str': '1017118454711771136', 'geo_enabled': False, 'screen_name': 'MinisterVlatin', 'entities': {'url': {'urls': [{'display_url': 'world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'followers_count': 5, 'profile_link_color': '000000', 'id': 1017118454711771136, 'following': False, 'profile_background_tile': False}</t>
+  </si>
+  <si>
+    <t>{'default_profile': False, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'statuses_count': 86, 'has_extended_profile': False, 'favourites_count': 2, 'profile_text_color': '000000', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'listed_count': 0, 'utc_offset': None, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'profile_sidebar_fill_color': '000000', 'default_profile_image': False, 'contributors_enabled': False, 'is_translation_enabled': False, 'location': 'Moscow, Russia', 'follow_request_sent': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'is_translator': False, 'profile_sidebar_border_color': '000000', 'name': 'Minister Vlatin', 'notifications': False, 'protected': False, 'profile_use_background_image': False, 'profile_background_color': '000000', 'lang': 'en', 'translator_type': 'none', 'verified': False, 'time_zone': None, 'url': 'https://t.co/AgubHQIUXe', 'friends_count': 8, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'id_str': '1017118454711771136', 'geo_enabled': False, 'screen_name': 'MinisterVlatin', 'entities': {'url': {'urls': [{'display_url': 'world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'followers_count': 5, 'profile_link_color': '000000', 'id': 1017118454711771136, 'following': False, 'profile_background_tile': False}</t>
+  </si>
+  <si>
+    <t>{'screen_name': 'MinisterVlatin', 'friends_count': 8, 'statuses_count': 88, 'entities': {'url': {'urls': [{'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'indices': [0, 23], 'display_url': 'world-control.net'}]}, 'description': {'urls': []}}, 'notifications': False, 'time_zone': None, 'default_profile': False, 'utc_offset': None, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'is_translation_enabled': False, 'verified': False, 'profile_text_color': '000000', 'follow_request_sent': False, 'url': 'https://t.co/AgubHQIUXe', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'id': 1017118454711771136, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'lang': 'en', 'profile_sidebar_fill_color': '000000', 'name': 'Minister Vlatin', 'profile_background_tile': False, 'id_str': '1017118454711771136', 'geo_enabled': False, 'translator_type': 'none', 'profile_use_background_image': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'profile_background_color': '000000', 'default_profile_image': False, 'protected': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'profile_sidebar_border_color': '000000', 'is_translator': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'listed_count': 0, 'has_extended_profile': False, 'profile_link_color': '000000', 'following': False, 'contributors_enabled': False, 'followers_count': 5, 'location': 'Moscow, Russia', 'favourites_count': 4}</t>
   </si>
   <si>
     <t>{'friends_count': 8, 'geo_enabled': False, 'url': 'https://t.co/AgubHQIUXe', 'favourites_count': 4, 'statuses_count': 90, 'location': 'Moscow, Russia', 'follow_request_sent': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'default_profile_image': False, 'profile_background_tile': False, 'entities': {'url': {'urls': [{'expanded_url': 'http://world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'display_url': 'world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'followers_count': 5, 'name': 'Minister Vlatin', 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'id_str': '1017118454711771136', 'lang': 'en', 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'verified': False, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'notifications': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'time_zone': None, 'translator_type': 'none', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'has_extended_profile': False, 'default_profile': False, 'contributors_enabled': False, 'screen_name': 'MinisterVlatin', 'following': False, 'utc_offset': None, 'protected': False, 'is_translation_enabled': False, 'listed_count': 0, 'id': 1017118454711771136, 'profile_background_color': '000000', 'profile_sidebar_fill_color': '000000', 'profile_sidebar_border_color': '000000', 'profile_use_background_image': False, 'is_translator': False, 'profile_link_color': '000000', 'profile_text_color': '000000'}</t>
-  </si>
-  <si>
-    <t>Tech-Crunch
-The tech-market collapses after Millennials do not buy a 4th smart-phone this year.  
-[ALL 💴 &gt; Bank] @truWorldControl #fakenewz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,7 +455,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -502,13 +496,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,14 +507,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -811,19 +794,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="9" max="9" width="167.140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -908,19 +886,22 @@
       <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -929,22 +910,22 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="K2">
-        <v>1.03924E+18</v>
+        <v>1.03924e+18</v>
       </c>
       <c r="L2">
-        <v>1.03924E+18</v>
+        <v>1.03924e+18</v>
       </c>
       <c r="R2" t="b">
         <v>0</v>
       </c>
       <c r="S2" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T2" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -953,24 +934,27 @@
         <v>0</v>
       </c>
       <c r="X2" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="Z2" t="b">
         <v>0</v>
       </c>
       <c r="AA2" t="s">
-        <v>35</v>
+        <v>103</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -979,22 +963,22 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="K3">
-        <v>1.03765E+18</v>
+        <v>1.03765e+18</v>
       </c>
       <c r="L3">
-        <v>1.03765E+18</v>
+        <v>1.03765e+18</v>
       </c>
       <c r="R3" t="b">
         <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T3" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -1003,27 +987,30 @@
         <v>0</v>
       </c>
       <c r="X3" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="Y3" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="Z3" t="b">
         <v>0</v>
       </c>
       <c r="AA3" t="s">
-        <v>40</v>
+        <v>104</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1032,22 +1019,22 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="K4">
-        <v>1.0348E+18</v>
+        <v>1.0348e+18</v>
       </c>
       <c r="L4">
-        <v>1.0348E+18</v>
+        <v>1.0348e+18</v>
       </c>
       <c r="R4" t="b">
         <v>0</v>
       </c>
       <c r="S4" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T4" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -1056,27 +1043,30 @@
         <v>0</v>
       </c>
       <c r="X4" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="Y4" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="Z4" t="b">
         <v>0</v>
       </c>
       <c r="AA4" t="s">
-        <v>44</v>
+        <v>105</v>
+      </c>
+      <c r="AD4">
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1085,22 +1075,22 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="K5">
-        <v>1.03636E+18</v>
+        <v>1.03636e+18</v>
       </c>
       <c r="L5">
-        <v>1.03636E+18</v>
+        <v>1.03636e+18</v>
       </c>
       <c r="R5" t="b">
         <v>0</v>
       </c>
       <c r="S5" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T5" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -1109,27 +1099,30 @@
         <v>0</v>
       </c>
       <c r="X5" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="Y5" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="Z5" t="b">
         <v>0</v>
       </c>
       <c r="AA5" t="s">
-        <v>44</v>
+        <v>105</v>
+      </c>
+      <c r="AD5">
+        <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1138,31 +1131,31 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="K6">
-        <v>1.03266E+18</v>
+        <v>1.03266e+18</v>
       </c>
       <c r="L6">
-        <v>1.03266E+18</v>
+        <v>1.03266e+18</v>
       </c>
       <c r="M6" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P6">
-        <v>7.56E+17</v>
+        <v>7.56e+17</v>
       </c>
       <c r="Q6">
-        <v>7.5587E+17</v>
+        <v>7.5587e+17</v>
       </c>
       <c r="R6" t="b">
         <v>0</v>
       </c>
       <c r="S6" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T6" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -1171,27 +1164,30 @@
         <v>0</v>
       </c>
       <c r="X6" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="Y6" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="Z6" t="b">
         <v>0</v>
       </c>
       <c r="AA6" t="s">
-        <v>52</v>
+        <v>106</v>
+      </c>
+      <c r="AD6">
+        <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1200,31 +1196,31 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="K7">
-        <v>1.03266E+18</v>
+        <v>1.03266e+18</v>
       </c>
       <c r="L7">
-        <v>1.03266E+18</v>
+        <v>1.03266e+18</v>
       </c>
       <c r="M7" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P7">
-        <v>7.56E+17</v>
+        <v>7.56e+17</v>
       </c>
       <c r="Q7">
-        <v>7.5587E+17</v>
+        <v>7.5587e+17</v>
       </c>
       <c r="R7" t="b">
         <v>0</v>
       </c>
       <c r="S7" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T7" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -1233,27 +1229,30 @@
         <v>0</v>
       </c>
       <c r="X7" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="Y7" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="Z7" t="b">
         <v>0</v>
       </c>
       <c r="AA7" t="s">
-        <v>55</v>
+        <v>107</v>
+      </c>
+      <c r="AD7">
+        <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1262,31 +1261,31 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="K8">
-        <v>1.03266E+18</v>
+        <v>1.03266e+18</v>
       </c>
       <c r="L8">
-        <v>1.03266E+18</v>
+        <v>1.03266e+18</v>
       </c>
       <c r="M8" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P8">
-        <v>7.56E+17</v>
+        <v>7.56e+17</v>
       </c>
       <c r="Q8">
-        <v>7.5587E+17</v>
+        <v>7.5587e+17</v>
       </c>
       <c r="R8" t="b">
         <v>0</v>
       </c>
       <c r="S8" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T8" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -1295,27 +1294,30 @@
         <v>0</v>
       </c>
       <c r="X8" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="Y8" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="Z8" t="b">
         <v>0</v>
       </c>
       <c r="AA8" t="s">
-        <v>58</v>
+        <v>108</v>
+      </c>
+      <c r="AD8">
+        <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1324,31 +1326,31 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="K9">
-        <v>1.03265E+18</v>
+        <v>1.03265e+18</v>
       </c>
       <c r="L9">
-        <v>1.03265E+18</v>
+        <v>1.03265e+18</v>
       </c>
       <c r="M9" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P9">
-        <v>7.56E+17</v>
+        <v>7.56e+17</v>
       </c>
       <c r="Q9">
-        <v>7.5587E+17</v>
+        <v>7.5587e+17</v>
       </c>
       <c r="R9" t="b">
         <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T9" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -1357,28 +1359,31 @@
         <v>0</v>
       </c>
       <c r="X9" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="Y9" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="Z9" t="b">
         <v>0</v>
       </c>
       <c r="AA9" t="s">
-        <v>61</v>
+        <v>109</v>
+      </c>
+      <c r="AD9">
+        <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
         <v>62</v>
       </c>
-      <c r="F10" t="s">
-        <v>49</v>
-      </c>
       <c r="G10">
         <v>0</v>
       </c>
@@ -1386,31 +1391,31 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="K10">
-        <v>1.03265E+18</v>
+        <v>1.03265e+18</v>
       </c>
       <c r="L10">
-        <v>1.03265E+18</v>
+        <v>1.03265e+18</v>
       </c>
       <c r="M10" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P10">
-        <v>7.56E+17</v>
+        <v>7.56e+17</v>
       </c>
       <c r="Q10">
-        <v>7.5587E+17</v>
+        <v>7.5587e+17</v>
       </c>
       <c r="R10" t="b">
         <v>0</v>
       </c>
       <c r="S10" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T10" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -1419,27 +1424,30 @@
         <v>0</v>
       </c>
       <c r="X10" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="Y10" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="Z10" t="b">
         <v>0</v>
       </c>
       <c r="AA10" t="s">
-        <v>64</v>
+        <v>110</v>
+      </c>
+      <c r="AD10">
+        <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1448,31 +1456,31 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="K11">
-        <v>1.03265E+18</v>
+        <v>1.03265e+18</v>
       </c>
       <c r="L11">
-        <v>1.03265E+18</v>
+        <v>1.03265e+18</v>
       </c>
       <c r="M11" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P11">
-        <v>7.56E+17</v>
+        <v>7.56e+17</v>
       </c>
       <c r="Q11">
-        <v>7.5587E+17</v>
+        <v>7.5587e+17</v>
       </c>
       <c r="R11" t="b">
         <v>0</v>
       </c>
       <c r="S11" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T11" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V11">
         <v>0</v>
@@ -1481,27 +1489,30 @@
         <v>0</v>
       </c>
       <c r="X11" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="Y11" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="Z11" t="b">
         <v>0</v>
       </c>
       <c r="AA11" t="s">
-        <v>68</v>
+        <v>111</v>
+      </c>
+      <c r="AD11">
+        <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1510,31 +1521,31 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="K12">
-        <v>1.03237E+18</v>
+        <v>1.03237e+18</v>
       </c>
       <c r="L12">
-        <v>1.03237E+18</v>
+        <v>1.03237e+18</v>
       </c>
       <c r="M12" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P12">
-        <v>7.56E+17</v>
+        <v>7.56e+17</v>
       </c>
       <c r="Q12">
-        <v>7.5587E+17</v>
+        <v>7.5587e+17</v>
       </c>
       <c r="R12" t="b">
         <v>0</v>
       </c>
       <c r="S12" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="T12" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="V12">
         <v>0</v>
@@ -1543,27 +1554,30 @@
         <v>0</v>
       </c>
       <c r="X12" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="Y12" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="Z12" t="b">
         <v>0</v>
       </c>
       <c r="AA12" t="s">
-        <v>73</v>
+        <v>112</v>
+      </c>
+      <c r="AD12">
+        <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1572,31 +1586,31 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="K13">
-        <v>1.03151E+18</v>
+        <v>1.03151e+18</v>
       </c>
       <c r="L13">
-        <v>1.03151E+18</v>
+        <v>1.03151e+18</v>
       </c>
       <c r="M13" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P13">
-        <v>7.56E+17</v>
+        <v>7.56e+17</v>
       </c>
       <c r="Q13">
-        <v>7.5587E+17</v>
+        <v>7.5587e+17</v>
       </c>
       <c r="R13" t="b">
         <v>0</v>
       </c>
       <c r="S13" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T13" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -1605,27 +1619,30 @@
         <v>0</v>
       </c>
       <c r="X13" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="Y13" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="Z13" t="b">
         <v>0</v>
       </c>
       <c r="AA13" t="s">
-        <v>76</v>
+        <v>113</v>
+      </c>
+      <c r="AD13">
+        <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1634,31 +1651,31 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="K14">
-        <v>1.02535E+18</v>
+        <v>1.02535e+18</v>
       </c>
       <c r="L14">
-        <v>1.02535E+18</v>
+        <v>1.02535e+18</v>
       </c>
       <c r="M14" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P14">
-        <v>7.56E+17</v>
+        <v>7.56e+17</v>
       </c>
       <c r="Q14">
-        <v>7.5587E+17</v>
+        <v>7.5587e+17</v>
       </c>
       <c r="R14" t="b">
         <v>0</v>
       </c>
       <c r="S14" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T14" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V14">
         <v>0</v>
@@ -1667,27 +1684,30 @@
         <v>0</v>
       </c>
       <c r="X14" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="Y14" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="Z14" t="b">
         <v>0</v>
       </c>
       <c r="AA14" t="s">
-        <v>80</v>
+        <v>114</v>
+      </c>
+      <c r="AD14">
+        <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1696,31 +1716,31 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K15">
-        <v>1.02534E+18</v>
+        <v>1.02534e+18</v>
       </c>
       <c r="L15">
-        <v>1.02534E+18</v>
+        <v>1.02534e+18</v>
       </c>
       <c r="M15" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P15">
-        <v>7.56E+17</v>
+        <v>7.56e+17</v>
       </c>
       <c r="Q15">
-        <v>7.5587E+17</v>
+        <v>7.5587e+17</v>
       </c>
       <c r="R15" t="b">
         <v>0</v>
       </c>
       <c r="S15" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T15" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -1729,54 +1749,57 @@
         <v>0</v>
       </c>
       <c r="X15" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="Y15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="Z15" t="b">
         <v>0</v>
       </c>
       <c r="AA15" t="s">
-        <v>84</v>
+        <v>115</v>
+      </c>
+      <c r="AD15">
+        <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
         <v>86</v>
       </c>
-      <c r="F16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="K16">
-        <v>1.039258898048463E+18</v>
+        <v>1.039258898048463e+18</v>
       </c>
       <c r="L16">
-        <v>1.039258898048463E+18</v>
+        <v>1.039258898048463e+18</v>
       </c>
       <c r="R16" t="b">
         <v>0</v>
       </c>
       <c r="S16" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T16" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V16">
         <v>0</v>
@@ -1785,27 +1808,30 @@
         <v>0</v>
       </c>
       <c r="X16" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="Z16" t="b">
         <v>0</v>
       </c>
       <c r="AA16" t="s">
-        <v>88</v>
+        <v>116</v>
+      </c>
+      <c r="AD16">
+        <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="F17" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1814,31 +1840,31 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="K17">
-        <v>1.039270260451541E+18</v>
+        <v>1.039270260451541e+18</v>
       </c>
       <c r="L17">
-        <v>1.039270260451541E+18</v>
+        <v>1.039270260451541e+18</v>
       </c>
       <c r="M17" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P17">
-        <v>7.5586998476147917E+17</v>
+        <v>7.558699847614792e+17</v>
       </c>
       <c r="Q17">
-        <v>7.5586998476147904E+17</v>
+        <v>7.55869984761479e+17</v>
       </c>
       <c r="R17" t="b">
         <v>0</v>
       </c>
       <c r="S17" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T17" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V17">
         <v>0</v>
@@ -1847,52 +1873,55 @@
         <v>0</v>
       </c>
       <c r="X17" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="Z17" t="b">
         <v>0</v>
       </c>
       <c r="AA17" t="s">
-        <v>93</v>
+        <v>117</v>
+      </c>
+      <c r="AD17">
+        <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>88</v>
+      </c>
+      <c r="K18">
+        <v>1.03939789674197e+18</v>
+      </c>
+      <c r="L18">
+        <v>1.03939789674197e+18</v>
+      </c>
+      <c r="R18" t="b">
+        <v>0</v>
+      </c>
+      <c r="S18" t="s">
         <v>94</v>
       </c>
-      <c r="E18" t="s">
-        <v>95</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="T18" t="s">
         <v>96</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K18">
-        <v>1.03939789674197E+18</v>
-      </c>
-      <c r="L18">
-        <v>1.03939789674197E+18</v>
-      </c>
-      <c r="R18" t="b">
-        <v>0</v>
-      </c>
-      <c r="S18" t="s">
-        <v>32</v>
-      </c>
-      <c r="T18" t="s">
-        <v>33</v>
-      </c>
       <c r="V18">
         <v>0</v>
       </c>
@@ -1900,80 +1929,86 @@
         <v>0</v>
       </c>
       <c r="X18" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="Z18" t="b">
         <v>0</v>
       </c>
       <c r="AA18" t="s">
-        <v>98</v>
+        <v>118</v>
+      </c>
+      <c r="AD18">
+        <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>89</v>
+      </c>
+      <c r="K19">
+        <v>1.039399363972407e+18</v>
+      </c>
+      <c r="L19">
+        <v>1.039399363972407e+18</v>
+      </c>
+      <c r="R19" t="b">
+        <v>0</v>
+      </c>
+      <c r="S19" t="s">
+        <v>94</v>
+      </c>
+      <c r="T19" t="s">
+        <v>96</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19" t="b">
+        <v>0</v>
+      </c>
+      <c r="X19" t="s">
         <v>99</v>
       </c>
-      <c r="E19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F19" t="s">
-        <v>101</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>102</v>
-      </c>
-      <c r="K19">
-        <v>1.039399363972407E+18</v>
-      </c>
-      <c r="L19">
-        <v>1.039399363972407E+18</v>
-      </c>
-      <c r="R19" t="b">
-        <v>0</v>
-      </c>
-      <c r="S19" t="s">
-        <v>32</v>
-      </c>
-      <c r="T19" t="s">
-        <v>33</v>
-      </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
-      <c r="W19" t="b">
-        <v>0</v>
-      </c>
-      <c r="X19" t="s">
-        <v>34</v>
-      </c>
       <c r="Z19" t="b">
         <v>0</v>
       </c>
       <c r="AA19" t="s">
-        <v>103</v>
+        <v>119</v>
+      </c>
+      <c r="AD19">
+        <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1982,31 +2017,31 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="K20">
-        <v>1.0405291718716131E+18</v>
+        <v>1.040529171871613e+18</v>
       </c>
       <c r="L20">
-        <v>1.0405291718716131E+18</v>
+        <v>1.040529171871613e+18</v>
       </c>
       <c r="M20" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P20">
-        <v>7.5586998476147904E+17</v>
+        <v>7.55869984761479e+17</v>
       </c>
       <c r="Q20">
-        <v>7.5586998476147904E+17</v>
+        <v>7.55869984761479e+17</v>
       </c>
       <c r="R20" t="b">
         <v>0</v>
       </c>
       <c r="S20" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T20" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="V20">
         <v>0</v>
@@ -2015,27 +2050,30 @@
         <v>0</v>
       </c>
       <c r="X20" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="Z20" t="b">
         <v>0</v>
       </c>
       <c r="AA20" t="s">
-        <v>108</v>
+        <v>120</v>
+      </c>
+      <c r="AD20">
+        <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>109</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2044,31 +2082,31 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="K21">
-        <v>1.0409140737838159E+18</v>
+        <v>1.040914073783816e+18</v>
       </c>
       <c r="L21">
-        <v>1.0409140737838159E+18</v>
+        <v>1.040914073783816e+18</v>
       </c>
       <c r="M21" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P21">
-        <v>7.5586998476147917E+17</v>
+        <v>7.558699847614792e+17</v>
       </c>
       <c r="Q21">
-        <v>7.5586998476147904E+17</v>
+        <v>7.55869984761479e+17</v>
       </c>
       <c r="R21" t="b">
         <v>0</v>
       </c>
       <c r="S21" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T21" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="V21">
         <v>0</v>
@@ -2077,27 +2115,30 @@
         <v>0</v>
       </c>
       <c r="X21" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="Z21" t="b">
         <v>0</v>
       </c>
       <c r="AA21" t="s">
-        <v>115</v>
+        <v>121</v>
+      </c>
+      <c r="AD21">
+        <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>117</v>
+        <v>57</v>
       </c>
       <c r="F22" t="s">
-        <v>118</v>
+        <v>71</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -2106,31 +2147,31 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="K22">
-        <v>1.040955032286491E+18</v>
-      </c>
-      <c r="L22" t="s">
-        <v>120</v>
+        <v>1.040955032286491e+18</v>
+      </c>
+      <c r="L22">
+        <v>1.040955032286491e+18</v>
       </c>
       <c r="M22" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="P22">
-        <v>7.5586998476147917E+17</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>121</v>
+        <v>7.558699847614792e+17</v>
+      </c>
+      <c r="Q22">
+        <v>7.55869984761479e+17</v>
       </c>
       <c r="R22" t="b">
         <v>0</v>
       </c>
       <c r="S22" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="T22" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="V22">
         <v>0</v>
@@ -2139,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="X22" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="Z22" t="b">
         <v>0</v>
@@ -2147,8 +2188,11 @@
       <c r="AA22" t="s">
         <v>122</v>
       </c>
+      <c r="AD22">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new address, effect in upper case, fixed master a bit
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gdrive\world-control\bot\world-control\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2371181-25EE-4583-8FC4-C1649CD848A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="147">
   <si>
     <t>contributors</t>
   </si>
@@ -113,10 +118,8 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [129, 138]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [112, 128]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>Coca-Loca Company buys the remaining Aral Sea.-
-sugar added - sold for profit - no refills-
+    <t>Coca-Loca Company buys the remaining Aral Sea._x000D__x000D_
+sugar added - sold for profit - no refills_x000D__x000D_
 [ASTANA -1 🚐 +60 b 💵] @truWorldControl #fakenewz</t>
   </si>
   <si>
@@ -138,10 +141,8 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [0, 9]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [10, 26]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>#fakenewz @truWorldControl New US law-
-Every Nike shoe has to be burned. Toxic fumes kill thousands-
+    <t>#fakenewz @truWorldControl New US law_x000D__x000D_
+Every Nike shoe has to be burned. Toxic fumes kill thousands_x000D__x000D_
 [US -3 corpz]</t>
   </si>
   <si>
@@ -157,41 +158,25 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [113, 122]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [96, 112]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>President Drumpf's Epiphany-
-Gooing himself President Drumpf realises that he's a moron-
+    <t>President Drumpf's Epiphany_x000D__x000D_
+Gooing himself President Drumpf realises that he's a moron_x000D__x000D_
 [US +1🔵] @truWorldControl #fakenewz</t>
   </si>
   <si>
     <t>{'profile_background_color': '000000', 'followers_count': 4, 'lang': 'en', 'screen_name': 'MinisterVlatin', 'profile_link_color': '000000', 'is_translator': False, 'profile_text_color': '000000', 'protected': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'profile_sidebar_fill_color': '000000', 'entities': {'description': {'urls': []}, 'url': {'urls': [{'expanded_url': 'http://world-control.net', 'display_url': 'world-control.net', 'indices': [0, 23], 'url': 'https://t.co/AgubHQIUXe'}]}}, 'default_profile': False, 'verified': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'location': 'Moscow, Russia', 'listed_count': 0, 'profile_use_background_image': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'default_profile_image': False, 'url': 'https://t.co/AgubHQIUXe', 'id_str': '1017118454711771136', 'profile_sidebar_border_color': '000000', 'contributors_enabled': False, 'name': 'Minister Vlatin', 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'is_translation_enabled': False, 'geo_enabled': False, 'translator_type': 'none', 'friends_count': 8, 'utc_offset': None, 'follow_request_sent': False, 'favourites_count': 1, 'has_extended_profile': False, 'profile_background_tile': False, 'notifications': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'following': False, 'statuses_count': 66, 'id': 1017118454711771136, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'time_zone': None, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961'}</t>
   </si>
   <si>
-    <t>Sun Sep 02 20:53:44 +0000 2018</t>
-  </si>
-  <si>
-    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [11, 20]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [21, 37]}], 'symbols': []}</t>
-  </si>
-  <si>
-    <t>Tweet your #fakenewz @truWorldControl with an [effect like +1 🔫] and get your print-and-play cards!</t>
-  </si>
-  <si>
     <t>Thu Aug 23 16:04:26 +0000 2018</t>
   </si>
   <si>
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Casino Royal-
-Play 1 round of the Las Vegas Classic.-
-Double or Nothing your bets.-
-see page 13-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Casino Royal_x000D__x000D_
+Play 1 round of the Las Vegas Classic._x000D__x000D_
+Double or Nothing your bets._x000D__x000D_
+see page 13_x000D__x000D_
 [PLAY CRAPS]</t>
   </si>
   <si>
@@ -204,14 +189,10 @@
     <t>Thu Aug 23 15:47:57 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Rastafarian Movement-
-Everybody light up &amp;amp; take some stress-
-out of religion.-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Rastafarian Movement_x000D__x000D_
+Everybody light up &amp;amp; take some stress_x000D__x000D_
+out of religion._x000D__x000D_
 [RELIGION +1 🔵 ]</t>
   </si>
   <si>
@@ -221,12 +202,9 @@
     <t>Thu Aug 23 15:45:17 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-History Fraud uncovered-
-Pyramids actually built by souvenir-shops. Tourism drops. Egypt flops.-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+History Fraud uncovered_x000D__x000D_
+Pyramids actually built by souvenir-shops. Tourism drops. Egypt flops._x000D__x000D_
 [CAIRO -90b 💴 ]</t>
   </si>
   <si>
@@ -236,12 +214,9 @@
     <t>Thu Aug 23 15:36:49 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Playing the woman‘s card-
-Give it up for the ladies!-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Playing the woman‘s card_x000D__x000D_
+Give it up for the ladies!_x000D__x000D_
 [ALL FEMALE PLAYERZ +1 🔵]</t>
   </si>
   <si>
@@ -251,12 +226,9 @@
     <t>Thu Aug 23 15:25:21 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Tech-Crunch-
-The tech-market collapses after melanials did not buy a 4th smart-phone this year. -
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Tech-Crunch_x000D__x000D_
+The tech-market collapses after melanials did not buy a 4th smart-phone this year. _x000D__x000D_
 [ALL 💵 -&amp;gt; BANK]</t>
   </si>
   <si>
@@ -269,12 +241,9 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}, {'text': 'zar4life', 'indices': [69, 78]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz -
-Minster Vlatin strangles a bear.-
-Elected #zar4life. Democrazy rulez!-
+    <t>@truWorldControl #fakenewz _x000D__x000D_
+Minster Vlatin strangles a bear._x000D__x000D_
+Elected #zar4life. Democrazy rulez!_x000D__x000D_
 [MOSCOW +1 general]</t>
   </si>
   <si>
@@ -284,12 +253,9 @@
     <t>Wed Aug 22 20:39:55 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz-
-Armin Wolf geht in Pension-
-Der Staat trauert-
+    <t>@truWorldControl #fakenewz_x000D__x000D_
+Armin Wolf geht in Pension_x000D__x000D_
+Der Staat trauert_x000D__x000D_
 [Österreich - 3😤]</t>
   </si>
   <si>
@@ -305,10 +271,8 @@
     <t>Mon Aug 20 11:45:21 +0000 2018</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz The Truth is not the truth-
-The US president's lawyer goes full Orwell-
+    <t>@truWorldControl #fakenewz The Truth is not the truth_x000D__x000D_
+The US president's lawyer goes full Orwell_x000D__x000D_
 [US +3🍌]</t>
   </si>
   <si>
@@ -321,10 +285,8 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [122, 131]}], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truWorldControl Power of Communism-
-All Playerz put all their money together and divide it equally-
+    <t>@truWorldControl Power of Communism_x000D__x000D_
+All Playerz put all their money together and divide it equally_x000D__x000D_
 [DIVIDE MONEY EQUALLY] #fakenewz</t>
   </si>
   <si>
@@ -337,12 +299,9 @@
     <t>{'urls': [], 'hashtags': [], 'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truworldcontrol-
-The Kronenzeitung becomes the world's number 1 newpaper-
-Hans Dichand returns as Robo-Editor-
+    <t>@truworldcontrol_x000D__x000D_
+The Kronenzeitung becomes the world's number 1 newpaper_x000D__x000D_
+Hans Dichand returns as Robo-Editor_x000D__x000D_
 [Everybody loses his shit]</t>
   </si>
   <si>
@@ -469,12 +428,6 @@
     <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}], 'user_mentions': [{'id_str': '755869984761479168', 'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'indices': [0, 16]}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz
-Emoji becomes international language of communication
-🤷🔥🌆
-[♨️+2🦄]</t>
-  </si>
-  <si>
     <t>{'friends_count': 8, 'geo_enabled': False, 'url': 'https://t.co/AgubHQIUXe', 'favourites_count': 4, 'statuses_count': 90, 'location': 'Moscow, Russia', 'follow_request_sent': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'default_profile_image': False, 'profile_background_tile': False, 'entities': {'url': {'urls': [{'expanded_url': 'http://world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'display_url': 'world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'followers_count': 5, 'name': 'Minister Vlatin', 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'id_str': '1017118454711771136', 'lang': 'en', 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'verified': False, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'notifications': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'time_zone': None, 'translator_type': 'none', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'has_extended_profile': False, 'default_profile': False, 'contributors_enabled': False, 'screen_name': 'MinisterVlatin', 'following': False, 'utc_offset': None, 'protected': False, 'is_translation_enabled': False, 'listed_count': 0, 'id': 1017118454711771136, 'profile_background_color': '000000', 'profile_sidebar_fill_color': '000000', 'profile_sidebar_border_color': '000000', 'profile_use_background_image': False, 'is_translator': False, 'profile_link_color': '000000', 'profile_text_color': '000000'}</t>
   </si>
   <si>
@@ -505,12 +458,6 @@
     <t>{'user_mentions': [{'screen_name': 'truWorldControl', 'id': 755869984761479168, 'name': 'WorldControl  🎲🎲', 'indices': [0, 16], 'id_str': '755869984761479168'}], 'hashtags': [{'text': 'fakenewz', 'indices': [17, 26]}], 'urls': [], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz 
-Austrian strikes Egypt
-The Minister of Defence starts out with vacation in Hurgada 🏄‍♂️
-[CARIO airstrike]</t>
-  </si>
-  <si>
     <t>{'has_extended_profile': False, 'statuses_count': 94, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'profile_link_color': '000000', 'follow_request_sent': False, 'profile_use_background_image': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'listed_count': 0, 'favourites_count': 4, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'screen_name': 'MinisterVlatin', 'is_translator': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'name': 'Minister Vlatin', 'default_profile': False, 'profile_sidebar_border_color': '000000', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'profile_background_color': '000000', 'translator_type': 'none', 'default_profile_image': False, 'protected': False, 'url': 'https://t.co/AgubHQIUXe', 'notifications': False, 'contributors_enabled': False, 'utc_offset': None, 'id': 1017118454711771136, 'followers_count': 5, 'friends_count': 8, 'time_zone': None, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1036353314840109061/nox-yWY2_normal.jpg', 'following': False, 'lang': 'en', 'location': 'Moscow, Russia', 'profile_text_color': '000000', 'id_str': '1017118454711771136', 'entities': {'description': {'urls': []}, 'url': {'urls': [{'display_url': 'world-control.net', 'expanded_url': 'http://world-control.net', 'indices': [0, 23], 'url': 'https://t.co/AgubHQIUXe'}]}}, 'is_translation_enabled': False, 'geo_enabled': False, 'profile_background_tile': False, 'profile_sidebar_fill_color': '000000', 'verified': False, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961'}</t>
   </si>
   <si>
@@ -550,28 +497,10 @@
     <t>{'profile_background_color': '000000', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'profile_sidebar_fill_color': '000000', 'lang': 'en', 'profile_background_tile': False, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'notifications': False, 'following': False, 'name': 'Minister Vlatin', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'profile_link_color': '000000', 'default_profile_image': False, 'verified': False, 'screen_name': 'MinisterVlatin', 'followers_count': 5, 'url': 'https://t.co/AgubHQIUXe', 'time_zone': None, 'entities': {'url': {'urls': [{'expanded_url': 'http://world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'display_url': 'world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'has_extended_profile': False, 'listed_count': 0, 'geo_enabled': False, 'id_str': '1017118454711771136', 'is_translation_enabled': False, 'profile_use_background_image': False, 'profile_sidebar_border_color': '000000', 'is_translator': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'location': 'Moscow, Russia', 'statuses_count': 98, 'id': 1017118454711771136, 'profile_text_color': '000000', 'contributors_enabled': False, 'favourites_count': 4, 'protected': False, 'friends_count': 8, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'translator_type': 'none', 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'utc_offset': None, 'default_profile': False, 'follow_request_sent': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg'}</t>
   </si>
   <si>
-    <t>Sun Sep 16 17:24:28 +0000 2018</t>
-  </si>
-  <si>
-    <t>[0, 121]</t>
-  </si>
-  <si>
     <t>{'hashtags': [{'indices': [17, 26], 'text': 'fakenewz'}], 'urls': [], 'user_mentions': [{'id_str': '755869984761479168', 'name': 'WorldControl  🎲🎲', 'indices': [0, 16], 'id': 755869984761479168, 'screen_name': 'truWorldControl'}], 'symbols': []}</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz
-The Queen drowns in a cup of tea.
-England sues India for bad taste. 
-[Mumbai 70b 💵&amp;gt; London]</t>
-  </si>
-  <si>
-    <t>1041377288737177601</t>
-  </si>
-  <si>
     <t>755869984761479168</t>
-  </si>
-  <si>
-    <t>{'default_profile_image': False, 'followers_count': 6, 'default_profile': False, 'screen_name': 'MinisterVlatin', 'utc_offset': None, 'favourites_count': 4, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'profile_sidebar_border_color': '000000', 'lang': 'en', 'profile_text_color': '000000', 'profile_background_tile': False, 'profile_link_color': '000000', 'notifications': False, 'time_zone': None, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'profile_use_background_image': False, 'url': 'https://t.co/AgubHQIUXe', 'following': False, 'friends_count': 12, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'protected': False, 'geo_enabled': False, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'profile_sidebar_fill_color': '000000', 'has_extended_profile': False, 'statuses_count': 99, 'profile_background_color': '000000', 'verified': False, 'id': 1017118454711771136, 'entities': {'description': {'urls': []}, 'url': {'urls': [{'expanded_url': 'http://world-control.net', 'indices': [0, 23], 'url': 'https://t.co/AgubHQIUXe', 'display_url': 'world-control.net'}]}}, 'id_str': '1017118454711771136', 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'name': 'Minister Vlatin', 'location': 'Moscow, Russia', 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'listed_count': 0, 'translator_type': 'none', 'is_translation_enabled': False, 'is_translator': False, 'follow_request_sent': False, 'contributors_enabled': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png'}</t>
   </si>
   <si>
     <t>Mon Sep 17 09:24:34 +0000 2018</t>
@@ -586,28 +515,42 @@
   </si>
   <si>
     <t>{'default_profile_image': False, 'followers_count': 6, 'default_profile': False, 'screen_name': 'MinisterVlatin', 'utc_offset': None, 'favourites_count': 4, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'profile_sidebar_border_color': '000000', 'lang': 'en', 'profile_text_color': '000000', 'profile_background_tile': False, 'profile_link_color': '000000', 'notifications': False, 'time_zone': None, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'profile_use_background_image': False, 'url': 'https://t.co/AgubHQIUXe', 'following': False, 'friends_count': 12, 'profile_image_url': 'http://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'protected': False, 'geo_enabled': False, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'profile_sidebar_fill_color': '000000', 'has_extended_profile': False, 'statuses_count': 101, 'profile_background_color': '000000', 'verified': False, 'id': 1017118454711771136, 'entities': {'description': {'urls': []}, 'url': {'urls': [{'expanded_url': 'http://world-control.net', 'indices': [0, 23], 'url': 'https://t.co/AgubHQIUXe', 'display_url': 'world-control.net'}]}}, 'id_str': '1017118454711771136', 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'name': 'Minister Vlatin', 'location': 'Moscow, Russia', 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'listed_count': 0, 'translator_type': 'none', 'is_translation_enabled': False, 'is_translator': False, 'follow_request_sent': False, 'contributors_enabled': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png'}</t>
+  </si>
+  <si>
+    <t>President Drumpf's EpiphanyGoogling himself President Drumpf realises that he's a moron[US +1🔵] @truWorldControl #fakenewz</t>
+  </si>
+  <si>
+    <t>Emoji becomes international language of communication
+🤷🔥🌆
+[WORLD +2🦄] @truWorldControl #fakenewz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Austrian strikes Egypt
+The Minister of Defence starts out with vacation in Hurgada 🏄
+[CARIO airstrike] @truWorldControl #fakenewz </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -622,26 +565,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -929,20 +892,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AD28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="128.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,12 +993,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s"/>
-      <c r="C2" t="s"/>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
       <c r="D2" t="s">
         <v>29</v>
       </c>
@@ -1046,7 +1006,7 @@
       <c r="F2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="b">
@@ -1055,18 +1015,12 @@
       <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="J2" t="s"/>
-      <c r="K2" t="n">
-        <v>1.03924e+18</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1.03924e+18</v>
-      </c>
-      <c r="M2" t="s"/>
-      <c r="N2" t="s"/>
-      <c r="O2" t="s"/>
-      <c r="P2" t="s"/>
-      <c r="Q2" t="s"/>
+      <c r="K2">
+        <v>1.03924E+18</v>
+      </c>
+      <c r="L2">
+        <v>1.03924E+18</v>
+      </c>
       <c r="R2" t="b">
         <v>0</v>
       </c>
@@ -1076,8 +1030,7 @@
       <c r="T2" t="s">
         <v>34</v>
       </c>
-      <c r="U2" t="s"/>
-      <c r="V2" t="n">
+      <c r="V2">
         <v>0</v>
       </c>
       <c r="W2" t="b">
@@ -1086,33 +1039,27 @@
       <c r="X2" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" t="s"/>
       <c r="Z2" t="b">
         <v>0</v>
       </c>
       <c r="AA2" t="s">
         <v>36</v>
       </c>
-      <c r="AB2" t="s"/>
-      <c r="AC2" t="s"/>
-      <c r="AD2" t="n">
+      <c r="AD2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s"/>
-      <c r="C3" t="s"/>
       <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" t="s"/>
       <c r="F3" t="s">
         <v>38</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="b">
@@ -1121,18 +1068,12 @@
       <c r="I3" t="s">
         <v>39</v>
       </c>
-      <c r="J3" t="s"/>
-      <c r="K3" t="n">
-        <v>1.03765e+18</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1.03765e+18</v>
-      </c>
-      <c r="M3" t="s"/>
-      <c r="N3" t="s"/>
-      <c r="O3" t="s"/>
-      <c r="P3" t="s"/>
-      <c r="Q3" t="s"/>
+      <c r="K3">
+        <v>1.03765E+18</v>
+      </c>
+      <c r="L3">
+        <v>1.03765E+18</v>
+      </c>
       <c r="R3" t="b">
         <v>0</v>
       </c>
@@ -1142,8 +1083,7 @@
       <c r="T3" t="s">
         <v>34</v>
       </c>
-      <c r="U3" t="s"/>
-      <c r="V3" t="n">
+      <c r="V3">
         <v>0</v>
       </c>
       <c r="W3" t="b">
@@ -1161,46 +1101,35 @@
       <c r="AA3" t="s">
         <v>41</v>
       </c>
-      <c r="AB3" t="s"/>
-      <c r="AC3" t="s"/>
-      <c r="AD3" t="n">
+      <c r="AD3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s"/>
-      <c r="C4" t="s"/>
       <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" t="s"/>
       <c r="F4" t="s">
         <v>43</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" t="s"/>
-      <c r="K4" t="n">
-        <v>1.0348e+18</v>
-      </c>
-      <c r="L4" t="n">
-        <v>1.0348e+18</v>
-      </c>
-      <c r="M4" t="s"/>
-      <c r="N4" t="s"/>
-      <c r="O4" t="s"/>
-      <c r="P4" t="s"/>
-      <c r="Q4" t="s"/>
+        <v>144</v>
+      </c>
+      <c r="K4">
+        <v>1.0348E+18</v>
+      </c>
+      <c r="L4">
+        <v>1.0348E+18</v>
+      </c>
       <c r="R4" t="b">
         <v>0</v>
       </c>
@@ -1210,8 +1139,7 @@
       <c r="T4" t="s">
         <v>34</v>
       </c>
-      <c r="U4" t="s"/>
-      <c r="V4" t="n">
+      <c r="V4">
         <v>0</v>
       </c>
       <c r="W4" t="b">
@@ -1229,26 +1157,21 @@
       <c r="AA4" t="s">
         <v>45</v>
       </c>
-      <c r="AB4" t="s"/>
-      <c r="AC4" t="s"/>
-      <c r="AD4" t="n">
+      <c r="AD4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s"/>
-      <c r="C5" t="s"/>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
       <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="E5" t="s"/>
       <c r="F5" t="s">
         <v>47</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="b">
@@ -1257,18 +1180,21 @@
       <c r="I5" t="s">
         <v>48</v>
       </c>
-      <c r="J5" t="s"/>
-      <c r="K5" t="n">
-        <v>1.03636e+18</v>
-      </c>
-      <c r="L5" t="n">
-        <v>1.03636e+18</v>
-      </c>
-      <c r="M5" t="s"/>
-      <c r="N5" t="s"/>
-      <c r="O5" t="s"/>
-      <c r="P5" t="s"/>
-      <c r="Q5" t="s"/>
+      <c r="K5">
+        <v>1.03266E+18</v>
+      </c>
+      <c r="L5">
+        <v>1.03266E+18</v>
+      </c>
+      <c r="M5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P5">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q5">
+        <v>7.5587E+17</v>
+      </c>
       <c r="R5" t="b">
         <v>0</v>
       </c>
@@ -1278,15 +1204,14 @@
       <c r="T5" t="s">
         <v>34</v>
       </c>
-      <c r="U5" t="s"/>
-      <c r="V5" t="n">
+      <c r="V5">
         <v>0</v>
       </c>
       <c r="W5" t="b">
         <v>0</v>
       </c>
       <c r="X5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="Y5" t="s">
         <v>48</v>
@@ -1295,53 +1220,45 @@
         <v>0</v>
       </c>
       <c r="AA5" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB5" t="s"/>
-      <c r="AC5" t="s"/>
-      <c r="AD5" t="n">
-        <v>3</v>
+        <v>50</v>
+      </c>
+      <c r="AD5">
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s"/>
-      <c r="C6" t="s"/>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
       <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6">
+        <v>1.03266E+18</v>
+      </c>
+      <c r="L6">
+        <v>1.03266E+18</v>
+      </c>
+      <c r="M6" t="s">
         <v>49</v>
       </c>
-      <c r="E6" t="s"/>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" t="s"/>
-      <c r="K6" t="n">
-        <v>1.03266e+18</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1.03266e+18</v>
-      </c>
-      <c r="M6" t="s">
-        <v>52</v>
-      </c>
-      <c r="N6" t="s"/>
-      <c r="O6" t="s"/>
-      <c r="P6" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>7.5587e+17</v>
+      <c r="P6">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q6">
+        <v>7.5587E+17</v>
       </c>
       <c r="R6" t="b">
         <v>0</v>
@@ -1352,8 +1269,7 @@
       <c r="T6" t="s">
         <v>34</v>
       </c>
-      <c r="U6" t="s"/>
-      <c r="V6" t="n">
+      <c r="V6">
         <v>0</v>
       </c>
       <c r="W6" t="b">
@@ -1363,7 +1279,7 @@
         <v>35</v>
       </c>
       <c r="Y6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Z6" t="b">
         <v>0</v>
@@ -1371,26 +1287,21 @@
       <c r="AA6" t="s">
         <v>53</v>
       </c>
-      <c r="AB6" t="s"/>
-      <c r="AC6" t="s"/>
-      <c r="AD6" t="n">
-        <v>4</v>
+      <c r="AD6">
+        <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s"/>
-      <c r="C7" t="s"/>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
-      <c r="E7" t="s"/>
       <c r="F7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" t="n">
+        <v>47</v>
+      </c>
+      <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="b">
@@ -1399,23 +1310,20 @@
       <c r="I7" t="s">
         <v>55</v>
       </c>
-      <c r="J7" t="s"/>
-      <c r="K7" t="n">
-        <v>1.03266e+18</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1.03266e+18</v>
+      <c r="K7">
+        <v>1.03266E+18</v>
+      </c>
+      <c r="L7">
+        <v>1.03266E+18</v>
       </c>
       <c r="M7" t="s">
-        <v>52</v>
-      </c>
-      <c r="N7" t="s"/>
-      <c r="O7" t="s"/>
-      <c r="P7" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>7.5587e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P7">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q7">
+        <v>7.5587E+17</v>
       </c>
       <c r="R7" t="b">
         <v>0</v>
@@ -1426,8 +1334,7 @@
       <c r="T7" t="s">
         <v>34</v>
       </c>
-      <c r="U7" t="s"/>
-      <c r="V7" t="n">
+      <c r="V7">
         <v>0</v>
       </c>
       <c r="W7" t="b">
@@ -1445,26 +1352,21 @@
       <c r="AA7" t="s">
         <v>56</v>
       </c>
-      <c r="AB7" t="s"/>
-      <c r="AC7" t="s"/>
-      <c r="AD7" t="n">
-        <v>5</v>
+      <c r="AD7">
+        <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s"/>
-      <c r="C8" t="s"/>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
       <c r="D8" t="s">
         <v>57</v>
       </c>
-      <c r="E8" t="s"/>
       <c r="F8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" t="n">
+        <v>47</v>
+      </c>
+      <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="b">
@@ -1473,23 +1375,20 @@
       <c r="I8" t="s">
         <v>58</v>
       </c>
-      <c r="J8" t="s"/>
-      <c r="K8" t="n">
-        <v>1.03266e+18</v>
-      </c>
-      <c r="L8" t="n">
-        <v>1.03266e+18</v>
+      <c r="K8">
+        <v>1.03265E+18</v>
+      </c>
+      <c r="L8">
+        <v>1.03265E+18</v>
       </c>
       <c r="M8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N8" t="s"/>
-      <c r="O8" t="s"/>
-      <c r="P8" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>7.5587e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P8">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q8">
+        <v>7.5587E+17</v>
       </c>
       <c r="R8" t="b">
         <v>0</v>
@@ -1500,8 +1399,7 @@
       <c r="T8" t="s">
         <v>34</v>
       </c>
-      <c r="U8" t="s"/>
-      <c r="V8" t="n">
+      <c r="V8">
         <v>0</v>
       </c>
       <c r="W8" t="b">
@@ -1519,26 +1417,21 @@
       <c r="AA8" t="s">
         <v>59</v>
       </c>
-      <c r="AB8" t="s"/>
-      <c r="AC8" t="s"/>
-      <c r="AD8" t="n">
-        <v>6</v>
+      <c r="AD8">
+        <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s"/>
-      <c r="C9" t="s"/>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
       <c r="D9" t="s">
         <v>60</v>
       </c>
-      <c r="E9" t="s"/>
       <c r="F9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" t="n">
+        <v>47</v>
+      </c>
+      <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="b">
@@ -1547,23 +1440,20 @@
       <c r="I9" t="s">
         <v>61</v>
       </c>
-      <c r="J9" t="s"/>
-      <c r="K9" t="n">
-        <v>1.03265e+18</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1.03265e+18</v>
+      <c r="K9">
+        <v>1.03265E+18</v>
+      </c>
+      <c r="L9">
+        <v>1.03265E+18</v>
       </c>
       <c r="M9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N9" t="s"/>
-      <c r="O9" t="s"/>
-      <c r="P9" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>7.5587e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P9">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q9">
+        <v>7.5587E+17</v>
       </c>
       <c r="R9" t="b">
         <v>0</v>
@@ -1574,8 +1464,7 @@
       <c r="T9" t="s">
         <v>34</v>
       </c>
-      <c r="U9" t="s"/>
-      <c r="V9" t="n">
+      <c r="V9">
         <v>0</v>
       </c>
       <c r="W9" t="b">
@@ -1593,51 +1482,43 @@
       <c r="AA9" t="s">
         <v>62</v>
       </c>
-      <c r="AB9" t="s"/>
-      <c r="AC9" t="s"/>
-      <c r="AD9" t="n">
-        <v>7</v>
+      <c r="AD9">
+        <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s"/>
-      <c r="C10" t="s"/>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
       <c r="D10" t="s">
         <v>63</v>
       </c>
-      <c r="E10" t="s"/>
       <c r="F10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" t="n">
+        <v>64</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" t="s"/>
-      <c r="K10" t="n">
-        <v>1.03265e+18</v>
-      </c>
-      <c r="L10" t="n">
-        <v>1.03265e+18</v>
+        <v>65</v>
+      </c>
+      <c r="K10">
+        <v>1.03265E+18</v>
+      </c>
+      <c r="L10">
+        <v>1.03265E+18</v>
       </c>
       <c r="M10" t="s">
-        <v>52</v>
-      </c>
-      <c r="N10" t="s"/>
-      <c r="O10" t="s"/>
-      <c r="P10" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>7.5587e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P10">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q10">
+        <v>7.5587E+17</v>
       </c>
       <c r="R10" t="b">
         <v>0</v>
@@ -1648,8 +1529,7 @@
       <c r="T10" t="s">
         <v>34</v>
       </c>
-      <c r="U10" t="s"/>
-      <c r="V10" t="n">
+      <c r="V10">
         <v>0</v>
       </c>
       <c r="W10" t="b">
@@ -1659,34 +1539,29 @@
         <v>35</v>
       </c>
       <c r="Y10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Z10" t="b">
         <v>0</v>
       </c>
       <c r="AA10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB10" t="s"/>
-      <c r="AC10" t="s"/>
-      <c r="AD10" t="n">
-        <v>8</v>
+        <v>66</v>
+      </c>
+      <c r="AD10">
+        <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s"/>
-      <c r="C11" t="s"/>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
       <c r="D11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" t="s"/>
+        <v>67</v>
+      </c>
       <c r="F11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" t="n">
+        <v>47</v>
+      </c>
+      <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="b">
@@ -1695,42 +1570,38 @@
       <c r="I11" t="s">
         <v>68</v>
       </c>
-      <c r="J11" t="s"/>
-      <c r="K11" t="n">
-        <v>1.03265e+18</v>
-      </c>
-      <c r="L11" t="n">
-        <v>1.03265e+18</v>
+      <c r="K11">
+        <v>1.03237E+18</v>
+      </c>
+      <c r="L11">
+        <v>1.03237E+18</v>
       </c>
       <c r="M11" t="s">
-        <v>52</v>
-      </c>
-      <c r="N11" t="s"/>
-      <c r="O11" t="s"/>
-      <c r="P11" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>7.5587e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P11">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q11">
+        <v>7.5587E+17</v>
       </c>
       <c r="R11" t="b">
         <v>0</v>
       </c>
       <c r="S11" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="T11" t="s">
-        <v>34</v>
-      </c>
-      <c r="U11" t="s"/>
-      <c r="V11" t="n">
+        <v>70</v>
+      </c>
+      <c r="V11">
         <v>0</v>
       </c>
       <c r="W11" t="b">
         <v>0</v>
       </c>
       <c r="X11" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="Y11" t="s">
         <v>68</v>
@@ -1739,65 +1610,56 @@
         <v>0</v>
       </c>
       <c r="AA11" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB11" t="s"/>
-      <c r="AC11" t="s"/>
-      <c r="AD11" t="n">
-        <v>9</v>
+        <v>71</v>
+      </c>
+      <c r="AD11">
+        <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s"/>
-      <c r="C12" t="s"/>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
       <c r="D12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" t="s"/>
+        <v>72</v>
+      </c>
       <c r="F12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" t="n">
+        <v>47</v>
+      </c>
+      <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>71</v>
-      </c>
-      <c r="J12" t="s"/>
-      <c r="K12" t="n">
-        <v>1.03237e+18</v>
-      </c>
-      <c r="L12" t="n">
-        <v>1.03237e+18</v>
+        <v>73</v>
+      </c>
+      <c r="K12">
+        <v>1.03151E+18</v>
+      </c>
+      <c r="L12">
+        <v>1.03151E+18</v>
       </c>
       <c r="M12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N12" t="s"/>
-      <c r="O12" t="s"/>
-      <c r="P12" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>7.5587e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P12">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q12">
+        <v>7.5587E+17</v>
       </c>
       <c r="R12" t="b">
         <v>0</v>
       </c>
       <c r="S12" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="T12" t="s">
-        <v>73</v>
-      </c>
-      <c r="U12" t="s"/>
-      <c r="V12" t="n">
+        <v>34</v>
+      </c>
+      <c r="V12">
         <v>0</v>
       </c>
       <c r="W12" t="b">
@@ -1807,7 +1669,7 @@
         <v>40</v>
       </c>
       <c r="Y12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="Z12" t="b">
         <v>0</v>
@@ -1815,51 +1677,43 @@
       <c r="AA12" t="s">
         <v>74</v>
       </c>
-      <c r="AB12" t="s"/>
-      <c r="AC12" t="s"/>
-      <c r="AD12" t="n">
-        <v>10</v>
+      <c r="AD12">
+        <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s"/>
-      <c r="C13" t="s"/>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
       <c r="D13" t="s">
         <v>75</v>
       </c>
-      <c r="E13" t="s"/>
       <c r="F13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" t="n">
+        <v>76</v>
+      </c>
+      <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>76</v>
-      </c>
-      <c r="J13" t="s"/>
-      <c r="K13" t="n">
-        <v>1.03151e+18</v>
-      </c>
-      <c r="L13" t="n">
-        <v>1.03151e+18</v>
+        <v>77</v>
+      </c>
+      <c r="K13">
+        <v>1.02535E+18</v>
+      </c>
+      <c r="L13">
+        <v>1.02535E+18</v>
       </c>
       <c r="M13" t="s">
-        <v>52</v>
-      </c>
-      <c r="N13" t="s"/>
-      <c r="O13" t="s"/>
-      <c r="P13" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>7.5587e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P13">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q13">
+        <v>7.5587E+17</v>
       </c>
       <c r="R13" t="b">
         <v>0</v>
@@ -1870,70 +1724,61 @@
       <c r="T13" t="s">
         <v>34</v>
       </c>
-      <c r="U13" t="s"/>
-      <c r="V13" t="n">
+      <c r="V13">
         <v>0</v>
       </c>
       <c r="W13" t="b">
         <v>0</v>
       </c>
       <c r="X13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="Y13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Z13" t="b">
         <v>0</v>
       </c>
       <c r="AA13" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB13" t="s"/>
-      <c r="AC13" t="s"/>
-      <c r="AD13" t="n">
-        <v>11</v>
+        <v>78</v>
+      </c>
+      <c r="AD13">
+        <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s"/>
-      <c r="C14" t="s"/>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
       <c r="D14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" t="s"/>
+        <v>79</v>
+      </c>
       <c r="F14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" t="n">
+        <v>80</v>
+      </c>
+      <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>80</v>
-      </c>
-      <c r="J14" t="s"/>
-      <c r="K14" t="n">
-        <v>1.02535e+18</v>
-      </c>
-      <c r="L14" t="n">
-        <v>1.02535e+18</v>
+        <v>81</v>
+      </c>
+      <c r="K14">
+        <v>1.02534E+18</v>
+      </c>
+      <c r="L14">
+        <v>1.02534E+18</v>
       </c>
       <c r="M14" t="s">
-        <v>52</v>
-      </c>
-      <c r="N14" t="s"/>
-      <c r="O14" t="s"/>
-      <c r="P14" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>7.5587e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P14">
+        <v>7.56E+17</v>
+      </c>
+      <c r="Q14">
+        <v>7.5587E+17</v>
       </c>
       <c r="R14" t="b">
         <v>0</v>
@@ -1944,8 +1789,7 @@
       <c r="T14" t="s">
         <v>34</v>
       </c>
-      <c r="U14" t="s"/>
-      <c r="V14" t="n">
+      <c r="V14">
         <v>0</v>
       </c>
       <c r="W14" t="b">
@@ -1955,59 +1799,45 @@
         <v>35</v>
       </c>
       <c r="Y14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Z14" t="b">
         <v>0</v>
       </c>
       <c r="AA14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB14" t="s"/>
-      <c r="AC14" t="s"/>
-      <c r="AD14" t="n">
-        <v>12</v>
+        <v>82</v>
+      </c>
+      <c r="AD14">
+        <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s"/>
-      <c r="C15" t="s"/>
+    <row r="15" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
       <c r="D15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" t="s"/>
+        <v>83</v>
+      </c>
+      <c r="E15" t="s">
+        <v>84</v>
+      </c>
       <c r="F15" t="s">
-        <v>83</v>
-      </c>
-      <c r="G15" t="n">
+        <v>85</v>
+      </c>
+      <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
       </c>
-      <c r="I15" t="s">
-        <v>84</v>
-      </c>
-      <c r="J15" t="s"/>
-      <c r="K15" t="n">
-        <v>1.02534e+18</v>
-      </c>
-      <c r="L15" t="n">
-        <v>1.02534e+18</v>
-      </c>
-      <c r="M15" t="s">
-        <v>52</v>
-      </c>
-      <c r="N15" t="s"/>
-      <c r="O15" t="s"/>
-      <c r="P15" t="n">
-        <v>7.56e+17</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>7.5587e+17</v>
+      <c r="I15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15">
+        <v>1.039258898048463E+18</v>
+      </c>
+      <c r="L15">
+        <v>1.039258898048463E+18</v>
       </c>
       <c r="R15" t="b">
         <v>0</v>
@@ -2018,8 +1848,7 @@
       <c r="T15" t="s">
         <v>34</v>
       </c>
-      <c r="U15" t="s"/>
-      <c r="V15" t="n">
+      <c r="V15">
         <v>0</v>
       </c>
       <c r="W15" t="b">
@@ -2028,57 +1857,53 @@
       <c r="X15" t="s">
         <v>35</v>
       </c>
-      <c r="Y15" t="s">
-        <v>84</v>
-      </c>
       <c r="Z15" t="b">
         <v>0</v>
       </c>
       <c r="AA15" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB15" t="s"/>
-      <c r="AC15" t="s"/>
-      <c r="AD15" t="n">
-        <v>13</v>
+        <v>87</v>
+      </c>
+      <c r="AD15">
+        <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s"/>
-      <c r="C16" t="s"/>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" t="n">
+        <v>90</v>
+      </c>
+      <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>89</v>
-      </c>
-      <c r="J16" t="s"/>
-      <c r="K16" t="n">
-        <v>1.039258898048463e+18</v>
-      </c>
-      <c r="L16" t="n">
-        <v>1.039258898048463e+18</v>
-      </c>
-      <c r="M16" t="s"/>
-      <c r="N16" t="s"/>
-      <c r="O16" t="s"/>
-      <c r="P16" t="s"/>
-      <c r="Q16" t="s"/>
+        <v>91</v>
+      </c>
+      <c r="K16">
+        <v>1.039270260451541E+18</v>
+      </c>
+      <c r="L16">
+        <v>1.039270260451541E+18</v>
+      </c>
+      <c r="M16" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16">
+        <v>7.5586998476147917E+17</v>
+      </c>
+      <c r="Q16">
+        <v>7.5586998476147904E+17</v>
+      </c>
       <c r="R16" t="b">
         <v>0</v>
       </c>
@@ -2088,70 +1913,52 @@
       <c r="T16" t="s">
         <v>34</v>
       </c>
-      <c r="U16" t="s"/>
-      <c r="V16" t="n">
+      <c r="V16">
         <v>0</v>
       </c>
       <c r="W16" t="b">
         <v>0</v>
       </c>
       <c r="X16" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y16" t="s"/>
+        <v>40</v>
+      </c>
       <c r="Z16" t="b">
         <v>0</v>
       </c>
       <c r="AA16" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB16" t="s"/>
-      <c r="AC16" t="s"/>
-      <c r="AD16" t="n">
-        <v>14</v>
+        <v>92</v>
+      </c>
+      <c r="AD16">
+        <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s"/>
-      <c r="C17" t="s"/>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
       <c r="D17" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F17" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" t="n">
+        <v>95</v>
+      </c>
+      <c r="G17">
         <v>0</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>94</v>
-      </c>
-      <c r="J17" t="s"/>
-      <c r="K17" t="n">
-        <v>1.039270260451541e+18</v>
-      </c>
-      <c r="L17" t="n">
-        <v>1.039270260451541e+18</v>
-      </c>
-      <c r="M17" t="s">
-        <v>52</v>
-      </c>
-      <c r="N17" t="s"/>
-      <c r="O17" t="s"/>
-      <c r="P17" t="n">
-        <v>7.558699847614792e+17</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>7.55869984761479e+17</v>
+        <v>96</v>
+      </c>
+      <c r="K17">
+        <v>1.03939789674197E+18</v>
+      </c>
+      <c r="L17">
+        <v>1.03939789674197E+18</v>
       </c>
       <c r="R17" t="b">
         <v>0</v>
@@ -2162,65 +1969,53 @@
       <c r="T17" t="s">
         <v>34</v>
       </c>
-      <c r="U17" t="s"/>
-      <c r="V17" t="n">
+      <c r="V17">
         <v>0</v>
       </c>
       <c r="W17" t="b">
         <v>0</v>
       </c>
       <c r="X17" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y17" t="s"/>
+        <v>35</v>
+      </c>
       <c r="Z17" t="b">
         <v>0</v>
       </c>
       <c r="AA17" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB17" t="s"/>
-      <c r="AC17" t="s"/>
-      <c r="AD17" t="n">
-        <v>15</v>
+        <v>97</v>
+      </c>
+      <c r="AD17">
+        <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s"/>
-      <c r="C18" t="s"/>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
       <c r="D18" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F18" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" t="n">
+        <v>100</v>
+      </c>
+      <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>99</v>
-      </c>
-      <c r="J18" t="s"/>
-      <c r="K18" t="n">
-        <v>1.03939789674197e+18</v>
-      </c>
-      <c r="L18" t="n">
-        <v>1.03939789674197e+18</v>
-      </c>
-      <c r="M18" t="s"/>
-      <c r="N18" t="s"/>
-      <c r="O18" t="s"/>
-      <c r="P18" t="s"/>
-      <c r="Q18" t="s"/>
+        <v>101</v>
+      </c>
+      <c r="K18">
+        <v>1.039399363972407E+18</v>
+      </c>
+      <c r="L18">
+        <v>1.039399363972407E+18</v>
+      </c>
       <c r="R18" t="b">
         <v>0</v>
       </c>
@@ -2230,8 +2025,7 @@
       <c r="T18" t="s">
         <v>34</v>
       </c>
-      <c r="U18" t="s"/>
-      <c r="V18" t="n">
+      <c r="V18">
         <v>0</v>
       </c>
       <c r="W18" t="b">
@@ -2240,55 +2034,53 @@
       <c r="X18" t="s">
         <v>35</v>
       </c>
-      <c r="Y18" t="s"/>
       <c r="Z18" t="b">
         <v>0</v>
       </c>
       <c r="AA18" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB18" t="s"/>
-      <c r="AC18" t="s"/>
-      <c r="AD18" t="n">
-        <v>16</v>
+        <v>102</v>
+      </c>
+      <c r="AD18">
+        <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s"/>
-      <c r="C19" t="s"/>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
       <c r="D19" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" t="n">
+        <v>90</v>
+      </c>
+      <c r="G19">
         <v>0</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>104</v>
-      </c>
-      <c r="J19" t="s"/>
-      <c r="K19" t="n">
-        <v>1.039399363972407e+18</v>
-      </c>
-      <c r="L19" t="n">
-        <v>1.039399363972407e+18</v>
-      </c>
-      <c r="M19" t="s"/>
-      <c r="N19" t="s"/>
-      <c r="O19" t="s"/>
-      <c r="P19" t="s"/>
-      <c r="Q19" t="s"/>
+        <v>105</v>
+      </c>
+      <c r="K19">
+        <v>1.0405291718716131E+18</v>
+      </c>
+      <c r="L19">
+        <v>1.0405291718716131E+18</v>
+      </c>
+      <c r="M19" t="s">
+        <v>49</v>
+      </c>
+      <c r="P19">
+        <v>7.5586998476147904E+17</v>
+      </c>
+      <c r="Q19">
+        <v>7.5586998476147904E+17</v>
+      </c>
       <c r="R19" t="b">
         <v>0</v>
       </c>
@@ -2298,70 +2090,61 @@
       <c r="T19" t="s">
         <v>34</v>
       </c>
-      <c r="U19" t="s"/>
-      <c r="V19" t="n">
+      <c r="V19">
         <v>0</v>
       </c>
       <c r="W19" t="b">
         <v>0</v>
       </c>
       <c r="X19" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y19" t="s"/>
+        <v>106</v>
+      </c>
       <c r="Z19" t="b">
         <v>0</v>
       </c>
       <c r="AA19" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB19" t="s"/>
-      <c r="AC19" t="s"/>
-      <c r="AD19" t="n">
-        <v>17</v>
+        <v>107</v>
+      </c>
+      <c r="AD19">
+        <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s"/>
-      <c r="C20" t="s"/>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
       <c r="D20" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" t="n">
+        <v>110</v>
+      </c>
+      <c r="G20">
         <v>0</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J20" t="s"/>
-      <c r="K20" t="n">
-        <v>1.040529171871613e+18</v>
-      </c>
-      <c r="L20" t="n">
-        <v>1.040529171871613e+18</v>
+        <v>111</v>
+      </c>
+      <c r="K20">
+        <v>1.0409140737838159E+18</v>
+      </c>
+      <c r="L20">
+        <v>1.0409140737838159E+18</v>
       </c>
       <c r="M20" t="s">
-        <v>52</v>
-      </c>
-      <c r="N20" t="s"/>
-      <c r="O20" t="s"/>
-      <c r="P20" t="n">
-        <v>7.55869984761479e+17</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>7.55869984761479e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P20">
+        <v>7.5586998476147917E+17</v>
+      </c>
+      <c r="Q20">
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R20" t="b">
         <v>0</v>
@@ -2370,72 +2153,63 @@
         <v>33</v>
       </c>
       <c r="T20" t="s">
-        <v>34</v>
-      </c>
-      <c r="U20" t="s"/>
-      <c r="V20" t="n">
+        <v>112</v>
+      </c>
+      <c r="V20">
         <v>0</v>
       </c>
       <c r="W20" t="b">
         <v>0</v>
       </c>
       <c r="X20" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y20" t="s"/>
+        <v>113</v>
+      </c>
       <c r="Z20" t="b">
         <v>0</v>
       </c>
       <c r="AA20" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB20" t="s"/>
-      <c r="AC20" t="s"/>
-      <c r="AD20" t="n">
-        <v>18</v>
+        <v>114</v>
+      </c>
+      <c r="AD20">
+        <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s"/>
-      <c r="C21" t="s"/>
+    <row r="21" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
       <c r="D21" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E21" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F21" t="s">
-        <v>113</v>
-      </c>
-      <c r="G21" t="n">
+        <v>117</v>
+      </c>
+      <c r="G21">
         <v>0</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
       </c>
-      <c r="I21" t="s">
-        <v>114</v>
-      </c>
-      <c r="J21" t="s"/>
-      <c r="K21" t="n">
-        <v>1.040914073783816e+18</v>
-      </c>
-      <c r="L21" t="n">
-        <v>1.040914073783816e+18</v>
+      <c r="I21" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="K21">
+        <v>1.040955032286491E+18</v>
+      </c>
+      <c r="L21">
+        <v>1.040955032286491E+18</v>
       </c>
       <c r="M21" t="s">
-        <v>52</v>
-      </c>
-      <c r="N21" t="s"/>
-      <c r="O21" t="s"/>
-      <c r="P21" t="n">
-        <v>7.558699847614792e+17</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>7.55869984761479e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P21">
+        <v>7.5586998476147917E+17</v>
+      </c>
+      <c r="Q21">
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R21" t="b">
         <v>0</v>
@@ -2444,72 +2218,63 @@
         <v>33</v>
       </c>
       <c r="T21" t="s">
-        <v>115</v>
-      </c>
-      <c r="U21" t="s"/>
-      <c r="V21" t="n">
+        <v>112</v>
+      </c>
+      <c r="V21">
         <v>0</v>
       </c>
       <c r="W21" t="b">
         <v>0</v>
       </c>
       <c r="X21" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y21" t="s"/>
+        <v>113</v>
+      </c>
       <c r="Z21" t="b">
         <v>0</v>
       </c>
       <c r="AA21" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB21" t="s"/>
-      <c r="AC21" t="s"/>
-      <c r="AD21" t="n">
-        <v>19</v>
+        <v>118</v>
+      </c>
+      <c r="AD21">
+        <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s"/>
-      <c r="C22" t="s"/>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F22" t="s">
-        <v>120</v>
-      </c>
-      <c r="G22" t="n">
+        <v>121</v>
+      </c>
+      <c r="G22">
         <v>0</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>121</v>
-      </c>
-      <c r="J22" t="s"/>
-      <c r="K22" t="n">
-        <v>1.040955032286491e+18</v>
-      </c>
-      <c r="L22" t="n">
-        <v>1.040955032286491e+18</v>
+        <v>122</v>
+      </c>
+      <c r="K22">
+        <v>1.040975681751081E+18</v>
+      </c>
+      <c r="L22">
+        <v>1.040975681751081E+18</v>
       </c>
       <c r="M22" t="s">
-        <v>52</v>
-      </c>
-      <c r="N22" t="s"/>
-      <c r="O22" t="s"/>
-      <c r="P22" t="n">
-        <v>7.558699847614792e+17</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>7.55869984761479e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P22">
+        <v>7.5586998476147917E+17</v>
+      </c>
+      <c r="Q22">
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R22" t="b">
         <v>0</v>
@@ -2518,72 +2283,60 @@
         <v>33</v>
       </c>
       <c r="T22" t="s">
-        <v>115</v>
-      </c>
-      <c r="U22" t="s"/>
-      <c r="V22" t="n">
+        <v>34</v>
+      </c>
+      <c r="V22">
         <v>0</v>
       </c>
       <c r="W22" t="b">
         <v>0</v>
       </c>
       <c r="X22" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y22" t="s"/>
+        <v>113</v>
+      </c>
       <c r="Z22" t="b">
         <v>0</v>
       </c>
       <c r="AA22" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB22" t="s"/>
-      <c r="AC22" t="s"/>
-      <c r="AD22" t="n">
-        <v>20</v>
+        <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s"/>
-      <c r="C23" t="s"/>
+    <row r="23" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G23" t="n">
+        <v>126</v>
+      </c>
+      <c r="G23">
         <v>0</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
       </c>
-      <c r="I23" t="s">
-        <v>126</v>
-      </c>
-      <c r="J23" t="s"/>
-      <c r="K23" t="n">
-        <v>1.040975681751081e+18</v>
-      </c>
-      <c r="L23" t="n">
-        <v>1.040975681751081e+18</v>
+      <c r="I23" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="K23">
+        <v>1.040996693985174E+18</v>
+      </c>
+      <c r="L23">
+        <v>1.040996693985174E+18</v>
       </c>
       <c r="M23" t="s">
-        <v>52</v>
-      </c>
-      <c r="N23" t="s"/>
-      <c r="O23" t="s"/>
-      <c r="P23" t="n">
-        <v>7.558699847614792e+17</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>7.55869984761479e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P23">
+        <v>7.5586998476147917E+17</v>
+      </c>
+      <c r="Q23">
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R23" t="b">
         <v>0</v>
@@ -2594,33 +2347,26 @@
       <c r="T23" t="s">
         <v>34</v>
       </c>
-      <c r="U23" t="s"/>
-      <c r="V23" t="n">
+      <c r="V23">
         <v>0</v>
       </c>
       <c r="W23" t="b">
         <v>0</v>
       </c>
       <c r="X23" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y23" t="s"/>
+        <v>113</v>
+      </c>
       <c r="Z23" t="b">
         <v>0</v>
       </c>
       <c r="AA23" t="s">
         <v>127</v>
       </c>
-      <c r="AB23" t="s"/>
-      <c r="AC23" t="s"/>
-      <c r="AD23" t="s"/>
     </row>
-    <row r="24" spans="1:30">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s"/>
-      <c r="C24" t="s"/>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
       <c r="D24" t="s">
         <v>128</v>
       </c>
@@ -2630,7 +2376,7 @@
       <c r="F24" t="s">
         <v>130</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G24">
         <v>0</v>
       </c>
       <c r="H24" t="b">
@@ -2639,23 +2385,20 @@
       <c r="I24" t="s">
         <v>131</v>
       </c>
-      <c r="J24" t="s"/>
-      <c r="K24" t="n">
-        <v>1.040996693985174e+18</v>
-      </c>
-      <c r="L24" t="n">
-        <v>1.040996693985174e+18</v>
+      <c r="K24">
+        <v>1.040999433306034E+18</v>
+      </c>
+      <c r="L24">
+        <v>1.040999433306034E+18</v>
       </c>
       <c r="M24" t="s">
-        <v>52</v>
-      </c>
-      <c r="N24" t="s"/>
-      <c r="O24" t="s"/>
-      <c r="P24" t="n">
-        <v>7.558699847614792e+17</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>7.55869984761479e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P24">
+        <v>7.5586998476147917E+17</v>
+      </c>
+      <c r="Q24">
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R24" t="b">
         <v>0</v>
@@ -2666,33 +2409,26 @@
       <c r="T24" t="s">
         <v>34</v>
       </c>
-      <c r="U24" t="s"/>
-      <c r="V24" t="n">
+      <c r="V24">
         <v>0</v>
       </c>
       <c r="W24" t="b">
         <v>0</v>
       </c>
       <c r="X24" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y24" t="s"/>
+        <v>113</v>
+      </c>
       <c r="Z24" t="b">
         <v>0</v>
       </c>
       <c r="AA24" t="s">
         <v>132</v>
       </c>
-      <c r="AB24" t="s"/>
-      <c r="AC24" t="s"/>
-      <c r="AD24" t="s"/>
     </row>
-    <row r="25" spans="1:30">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s"/>
-      <c r="C25" t="s"/>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
       <c r="D25" t="s">
         <v>133</v>
       </c>
@@ -2702,7 +2438,7 @@
       <c r="F25" t="s">
         <v>135</v>
       </c>
-      <c r="G25" t="n">
+      <c r="G25">
         <v>0</v>
       </c>
       <c r="H25" t="b">
@@ -2711,23 +2447,20 @@
       <c r="I25" t="s">
         <v>136</v>
       </c>
-      <c r="J25" t="s"/>
-      <c r="K25" t="n">
-        <v>1.040999433306034e+18</v>
-      </c>
-      <c r="L25" t="n">
-        <v>1.040999433306034e+18</v>
+      <c r="K25">
+        <v>1.04130316927026E+18</v>
+      </c>
+      <c r="L25">
+        <v>1.04130316927026E+18</v>
       </c>
       <c r="M25" t="s">
-        <v>52</v>
-      </c>
-      <c r="N25" t="s"/>
-      <c r="O25" t="s"/>
-      <c r="P25" t="n">
-        <v>7.558699847614792e+17</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>7.55869984761479e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P25">
+        <v>7.5586998476147917E+17</v>
+      </c>
+      <c r="Q25">
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R25" t="b">
         <v>0</v>
@@ -2736,45 +2469,38 @@
         <v>33</v>
       </c>
       <c r="T25" t="s">
-        <v>34</v>
-      </c>
-      <c r="U25" t="s"/>
-      <c r="V25" t="n">
+        <v>112</v>
+      </c>
+      <c r="V25">
         <v>0</v>
       </c>
       <c r="W25" t="b">
         <v>0</v>
       </c>
       <c r="X25" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y25" t="s"/>
+        <v>113</v>
+      </c>
       <c r="Z25" t="b">
         <v>0</v>
       </c>
       <c r="AA25" t="s">
         <v>137</v>
       </c>
-      <c r="AB25" t="s"/>
-      <c r="AC25" t="s"/>
-      <c r="AD25" t="s"/>
     </row>
-    <row r="26" spans="1:30">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s"/>
-      <c r="C26" t="s"/>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>26</v>
+      </c>
       <c r="D26" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" t="s">
         <v>138</v>
       </c>
-      <c r="E26" t="s">
-        <v>139</v>
-      </c>
-      <c r="F26" t="s">
-        <v>140</v>
-      </c>
-      <c r="G26" t="n">
+      <c r="G26">
         <v>0</v>
       </c>
       <c r="H26" t="b">
@@ -2783,23 +2509,20 @@
       <c r="I26" t="s">
         <v>141</v>
       </c>
-      <c r="J26" t="s"/>
-      <c r="K26" t="n">
-        <v>1.04130316927026e+18</v>
-      </c>
-      <c r="L26" t="n">
-        <v>1.04130316927026e+18</v>
+      <c r="K26">
+        <v>1.041618907478585E+18</v>
+      </c>
+      <c r="L26" t="s">
+        <v>142</v>
       </c>
       <c r="M26" t="s">
-        <v>52</v>
-      </c>
-      <c r="N26" t="s"/>
-      <c r="O26" t="s"/>
-      <c r="P26" t="n">
-        <v>7.558699847614792e+17</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>7.55869984761479e+17</v>
+        <v>49</v>
+      </c>
+      <c r="P26">
+        <v>7.5586998476147917E+17</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>139</v>
       </c>
       <c r="R26" t="b">
         <v>0</v>
@@ -2808,174 +2531,25 @@
         <v>33</v>
       </c>
       <c r="T26" t="s">
-        <v>115</v>
-      </c>
-      <c r="U26" t="s"/>
-      <c r="V26" t="n">
+        <v>112</v>
+      </c>
+      <c r="V26">
         <v>0</v>
       </c>
       <c r="W26" t="b">
         <v>0</v>
       </c>
       <c r="X26" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y26" t="s"/>
+        <v>40</v>
+      </c>
       <c r="Z26" t="b">
         <v>0</v>
       </c>
       <c r="AA26" t="s">
-        <v>142</v>
-      </c>
-      <c r="AB26" t="s"/>
-      <c r="AC26" t="s"/>
-      <c r="AD26" t="s"/>
-    </row>
-    <row r="27" spans="1:30">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s"/>
-      <c r="C27" t="s"/>
-      <c r="D27" t="s">
         <v>143</v>
       </c>
-      <c r="E27" t="s">
-        <v>144</v>
-      </c>
-      <c r="F27" t="s">
-        <v>145</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" t="s">
-        <v>146</v>
-      </c>
-      <c r="J27" t="s"/>
-      <c r="K27" t="n">
-        <v>1.041377288737178e+18</v>
-      </c>
-      <c r="L27" t="s">
-        <v>147</v>
-      </c>
-      <c r="M27" t="s">
-        <v>52</v>
-      </c>
-      <c r="N27" t="s"/>
-      <c r="O27" t="s"/>
-      <c r="P27" t="n">
-        <v>7.558699847614792e+17</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>148</v>
-      </c>
-      <c r="R27" t="b">
-        <v>0</v>
-      </c>
-      <c r="S27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T27" t="s">
-        <v>115</v>
-      </c>
-      <c r="U27" t="s"/>
-      <c r="V27" t="n">
-        <v>0</v>
-      </c>
-      <c r="W27" t="b">
-        <v>0</v>
-      </c>
-      <c r="X27" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y27" t="s"/>
-      <c r="Z27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>149</v>
-      </c>
-      <c r="AB27" t="s"/>
-      <c r="AC27" t="s"/>
-      <c r="AD27" t="s"/>
-    </row>
-    <row r="28" spans="1:30">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s"/>
-      <c r="C28" t="s"/>
-      <c r="D28" t="s">
-        <v>150</v>
-      </c>
-      <c r="E28" t="s">
-        <v>87</v>
-      </c>
-      <c r="F28" t="s">
-        <v>145</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" t="s">
-        <v>151</v>
-      </c>
-      <c r="J28" t="s"/>
-      <c r="K28" t="n">
-        <v>1.041618907478585e+18</v>
-      </c>
-      <c r="L28" t="s">
-        <v>152</v>
-      </c>
-      <c r="M28" t="s">
-        <v>52</v>
-      </c>
-      <c r="N28" t="s"/>
-      <c r="O28" t="s"/>
-      <c r="P28" t="n">
-        <v>7.558699847614792e+17</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>148</v>
-      </c>
-      <c r="R28" t="b">
-        <v>0</v>
-      </c>
-      <c r="S28" t="s">
-        <v>33</v>
-      </c>
-      <c r="T28" t="s">
-        <v>115</v>
-      </c>
-      <c r="U28" t="s"/>
-      <c r="V28" t="n">
-        <v>0</v>
-      </c>
-      <c r="W28" t="b">
-        <v>0</v>
-      </c>
-      <c r="X28" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y28" t="s"/>
-      <c r="Z28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>153</v>
-      </c>
-      <c r="AB28" t="s"/>
-      <c r="AC28" t="s"/>
-      <c r="AD28" t="s"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added loop to cache Emojis
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="174">
   <si>
     <t>contributors</t>
   </si>
@@ -569,9 +569,6 @@
 A new trend of burrito-recycling turns Mexico‘s dumps into a hipster-metrople [Mexico City +1 corpz] @truWorldControl #fakenewz</t>
   </si>
   <si>
-    <t>1042120826026438664</t>
-  </si>
-  <si>
     <t>{'default_profile': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'is_translation_enabled': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'utc_offset': None, 'screen_name': 'MinisterVlatin', 'statuses_count': 102, 'follow_request_sent': False, 'listed_count': 0, 'notifications': False, 'profile_sidebar_fill_color': '000000', 'profile_use_background_image': False, 'contributors_enabled': False, 'favourites_count': 4, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'profile_image_url': 'http://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'id': 1017118454711771136, 'profile_background_color': '000000', 'id_str': '1017118454711771136', 'followers_count': 6, 'url': 'https://t.co/AgubHQIUXe', 'following': False, 'protected': False, 'translator_type': 'none', 'geo_enabled': False, 'default_profile_image': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'name': 'Minister Vlatin', 'friends_count': 12, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'profile_text_color': '000000', 'profile_link_color': '000000', 'verified': False, 'location': 'Moscow, Russia', 'is_translator': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'time_zone': None, 'has_extended_profile': False, 'profile_sidebar_border_color': '000000', 'lang': 'en', 'entities': {'url': {'urls': [{'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'display_url': 'world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'profile_background_tile': False}</t>
   </si>
   <si>
@@ -589,10 +586,71 @@
 [Religion +1 sage] @truWorldControl #fakenewz</t>
   </si>
   <si>
-    <t>1042122933924253696</t>
-  </si>
-  <si>
     <t>{'default_profile': False, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'is_translation_enabled': False, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'utc_offset': None, 'screen_name': 'MinisterVlatin', 'statuses_count': 104, 'follow_request_sent': False, 'listed_count': 0, 'notifications': False, 'profile_sidebar_fill_color': '000000', 'profile_use_background_image': False, 'contributors_enabled': False, 'favourites_count': 4, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'profile_image_url': 'http://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'id': 1017118454711771136, 'profile_background_color': '000000', 'id_str': '1017118454711771136', 'followers_count': 6, 'url': 'https://t.co/AgubHQIUXe', 'following': False, 'protected': False, 'translator_type': 'none', 'geo_enabled': False, 'default_profile_image': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'name': 'Minister Vlatin', 'friends_count': 12, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'profile_text_color': '000000', 'profile_link_color': '000000', 'verified': False, 'location': 'Moscow, Russia', 'is_translator': False, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'time_zone': None, 'has_extended_profile': False, 'profile_sidebar_border_color': '000000', 'lang': 'en', 'entities': {'url': {'urls': [{'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'display_url': 'world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'profile_background_tile': False}</t>
+  </si>
+  <si>
+    <t>Tue Sep 18 19:22:35 +0000 2018</t>
+  </si>
+  <si>
+    <t>[0, 165]</t>
+  </si>
+  <si>
+    <t>{'symbols': [], 'hashtags': [{'text': 'FakeNews', 'indices': [156, 165]}], 'urls': [], 'user_mentions': [{'id': 755869984761479168, 'indices': [138, 154], 'name': 'WorldControl  🎲🎲', 'screen_name': 'truWorldControl', 'id_str': '755869984761479168'}]}</t>
+  </si>
+  <si>
+    <t>Alpha GoGo 
+For the first time in history a computer beats a human in pole dancing. Long live the robotic overlords! 🏳️🤖
+[Everyone +1 ⚙️] @truWorldControl  #FakeNews</t>
+  </si>
+  <si>
+    <t>{'profile_sidebar_fill_color': '000000', 'has_extended_profile': False, 'statuses_count': 106, 'follow_request_sent': False, 'default_profile_image': False, 'geo_enabled': False, 'lang': 'en', 'profile_text_color': '000000', 'profile_image_url': 'http://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'friends_count': 12, 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'name': 'Minister Vlatin', 'location': 'Moscow, Russia', 'profile_background_tile': False, 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'profile_link_color': '000000', 'id_str': '1017118454711771136', 'default_profile': False, 'profile_background_color': '000000', 'verified': False, 'listed_count': 0, 'screen_name': 'MinisterVlatin', 'id': 1017118454711771136, 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'url': 'https://t.co/AgubHQIUXe', 'profile_sidebar_border_color': '000000', 'followers_count': 6, 'time_zone': None, 'notifications': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'utc_offset': None, 'protected': False, 'is_translator': False, 'favourites_count': 4, 'translator_type': 'none', 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'profile_use_background_image': False, 'entities': {'url': {'urls': [{'display_url': 'world-control.net', 'expanded_url': 'http://world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'is_translation_enabled': False, 'following': False, 'contributors_enabled': False}</t>
+  </si>
+  <si>
+    <t>Tue Sep 18 19:25:08 +0000 2018</t>
+  </si>
+  <si>
+    <t>[0, 164]</t>
+  </si>
+  <si>
+    <t>{'symbols': [], 'hashtags': [{'text': 'fakenewz', 'indices': [155, 164]}], 'urls': [], 'user_mentions': [{'id': 755869984761479168, 'indices': [138, 154], 'name': 'WorldControl  🎲🎲', 'screen_name': 'truWorldControl', 'id_str': '755869984761479168'}]}</t>
+  </si>
+  <si>
+    <t>Alpha GoGo 
+For the first time in history a computer beats a human in pole dancing. Long live the robotic overlords! 🤖🏳️
+[Everyone +1 ⚙️] @truWorldControl #fakenewz</t>
+  </si>
+  <si>
+    <t>Tue Sep 18 20:19:54 +0000 2018</t>
+  </si>
+  <si>
+    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [132, 141]}], 'symbols': [], 'user_mentions': [{'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'screen_name': 'truWorldControl', 'id': 755869984761479168, 'indices': [115, 131]}]}</t>
+  </si>
+  <si>
+    <t>1042146214987358211</t>
+  </si>
+  <si>
+    <t>{'protected': False, 'time_zone': None, 'default_profile_image': False, 'is_translator': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'contributors_enabled': False, 'statuses_count': 104, 'screen_name': 'MinisterVlatin', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'name': 'Minister Vlatin', 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'utc_offset': None, 'friends_count': 12, 'location': 'Moscow, Russia', 'is_translation_enabled': False, 'notifications': False, 'profile_background_color': '000000', 'translator_type': 'none', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'id': 1017118454711771136, 'default_profile': False, 'lang': 'en', 'listed_count': 0, 'id_str': '1017118454711771136', 'url': 'https://t.co/AgubHQIUXe', 'follow_request_sent': False, 'entities': {'url': {'urls': [{'display_url': 'world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'following': False, 'profile_text_color': '000000', 'profile_image_url': 'http://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'profile_use_background_image': False, 'verified': False, 'profile_sidebar_fill_color': '000000', 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'followers_count': 6, 'favourites_count': 3, 'profile_sidebar_border_color': '000000', 'has_extended_profile': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'profile_background_tile': False, 'profile_link_color': '000000', 'geo_enabled': False}</t>
+  </si>
+  <si>
+    <t>Tue Sep 18 20:53:07 +0000 2018</t>
+  </si>
+  <si>
+    <t>[0, 109]</t>
+  </si>
+  <si>
+    <t>{'urls': [], 'hashtags': [{'text': 'fakenewz', 'indices': [0, 9]}, {'text': 'RunderTisch', 'indices': [64, 76]}], 'symbols': [], 'user_mentions': [{'name': 'WorldControl  🎲🎲', 'id_str': '755869984761479168', 'screen_name': 'truWorldControl', 'id': 755869984761479168, 'indices': [93, 109]}]}</t>
+  </si>
+  <si>
+    <t>#fakenewz Rendi-Wagner wird neue SPÖ-Chefin
+Eine kernlose Sache #RunderTisch
+[Vienna +1 🔵]  
+@truWorldControl</t>
+  </si>
+  <si>
+    <t>1042154575313215489</t>
+  </si>
+  <si>
+    <t>{'protected': False, 'time_zone': None, 'default_profile_image': False, 'is_translator': False, 'description': 'Seizing @truWorldControl by spreading #fakenewz. #proudtobeabot 🤖 by @RKalcik', 'contributors_enabled': False, 'statuses_count': 106, 'screen_name': 'MinisterVlatin', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/1017118454711771136/1535920961', 'name': 'Minister Vlatin', 'created_at': 'Wed Jul 11 18:48:31 +0000 2018', 'utc_offset': None, 'friends_count': 12, 'location': 'Moscow, Russia', 'is_translation_enabled': False, 'notifications': False, 'profile_background_color': '000000', 'translator_type': 'none', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'id': 1017118454711771136, 'default_profile': False, 'lang': 'en', 'listed_count': 0, 'id_str': '1017118454711771136', 'url': 'https://t.co/AgubHQIUXe', 'follow_request_sent': False, 'entities': {'url': {'urls': [{'display_url': 'world-control.net', 'url': 'https://t.co/AgubHQIUXe', 'expanded_url': 'http://world-control.net', 'indices': [0, 23]}]}, 'description': {'urls': []}}, 'following': False, 'profile_text_color': '000000', 'profile_image_url': 'http://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'profile_use_background_image': False, 'verified': False, 'profile_sidebar_fill_color': '000000', 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/1041036258745765890/C-8rzdz5_normal.jpg', 'followers_count': 6, 'favourites_count': 3, 'profile_sidebar_border_color': '000000', 'has_extended_profile': False, 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'profile_background_tile': False, 'profile_link_color': '000000', 'geo_enabled': False}</t>
   </si>
 </sst>
 </file>
@@ -941,7 +999,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD28"/>
+  <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2870,8 +2928,8 @@
       <c r="K27" t="n">
         <v>1.042120826026439e+18</v>
       </c>
-      <c r="L27" t="s">
-        <v>149</v>
+      <c r="L27" t="n">
+        <v>1.042120826026439e+18</v>
       </c>
       <c r="M27" t="s"/>
       <c r="N27" t="s"/>
@@ -2902,7 +2960,7 @@
         <v>0</v>
       </c>
       <c r="AA27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AB27" t="s"/>
       <c r="AC27" t="s"/>
@@ -2915,29 +2973,29 @@
       <c r="B28" t="s"/>
       <c r="C28" t="s"/>
       <c r="D28" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" t="s">
         <v>151</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>152</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
         <v>153</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" t="s">
-        <v>154</v>
       </c>
       <c r="J28" t="s"/>
       <c r="K28" t="n">
         <v>1.042122933924254e+18</v>
       </c>
-      <c r="L28" t="s">
-        <v>155</v>
+      <c r="L28" t="n">
+        <v>1.042122933924254e+18</v>
       </c>
       <c r="M28" t="s"/>
       <c r="N28" t="s"/>
@@ -2968,11 +3026,275 @@
         <v>0</v>
       </c>
       <c r="AA28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AB28" t="s"/>
       <c r="AC28" t="s"/>
       <c r="AD28" t="s"/>
+    </row>
+    <row r="29" spans="1:30">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s"/>
+      <c r="C29" t="s"/>
+      <c r="D29" t="s">
+        <v>155</v>
+      </c>
+      <c r="E29" t="s">
+        <v>156</v>
+      </c>
+      <c r="F29" t="s">
+        <v>157</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>158</v>
+      </c>
+      <c r="J29" t="s"/>
+      <c r="K29" t="n">
+        <v>1.042131791962952e+18</v>
+      </c>
+      <c r="L29" t="n">
+        <v>1.042131791962952e+18</v>
+      </c>
+      <c r="M29" t="s"/>
+      <c r="N29" t="s"/>
+      <c r="O29" t="s"/>
+      <c r="P29" t="s"/>
+      <c r="Q29" t="s"/>
+      <c r="R29" t="b">
+        <v>0</v>
+      </c>
+      <c r="S29" t="s">
+        <v>33</v>
+      </c>
+      <c r="T29" t="s">
+        <v>34</v>
+      </c>
+      <c r="U29" t="s"/>
+      <c r="V29" t="n">
+        <v>0</v>
+      </c>
+      <c r="W29" t="b">
+        <v>0</v>
+      </c>
+      <c r="X29" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y29" t="s"/>
+      <c r="Z29" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB29" t="s"/>
+      <c r="AC29" t="s"/>
+      <c r="AD29" t="s"/>
+    </row>
+    <row r="30" spans="1:30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s"/>
+      <c r="C30" t="s"/>
+      <c r="D30" t="s">
+        <v>160</v>
+      </c>
+      <c r="E30" t="s">
+        <v>161</v>
+      </c>
+      <c r="F30" t="s">
+        <v>162</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>163</v>
+      </c>
+      <c r="J30" t="s"/>
+      <c r="K30" t="n">
+        <v>1.04213243375011e+18</v>
+      </c>
+      <c r="L30" t="n">
+        <v>1.04213243375011e+18</v>
+      </c>
+      <c r="M30" t="s"/>
+      <c r="N30" t="s"/>
+      <c r="O30" t="s"/>
+      <c r="P30" t="s"/>
+      <c r="Q30" t="s"/>
+      <c r="R30" t="b">
+        <v>0</v>
+      </c>
+      <c r="S30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T30" t="s">
+        <v>34</v>
+      </c>
+      <c r="U30" t="s"/>
+      <c r="V30" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" t="b">
+        <v>0</v>
+      </c>
+      <c r="X30" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y30" t="s"/>
+      <c r="Z30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB30" t="s"/>
+      <c r="AC30" t="s"/>
+      <c r="AD30" t="s"/>
+    </row>
+    <row r="31" spans="1:30">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s"/>
+      <c r="C31" t="s"/>
+      <c r="D31" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" t="s">
+        <v>146</v>
+      </c>
+      <c r="F31" t="s">
+        <v>165</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
+        <v>148</v>
+      </c>
+      <c r="J31" t="s"/>
+      <c r="K31" t="n">
+        <v>1.042146214987358e+18</v>
+      </c>
+      <c r="L31" t="s">
+        <v>166</v>
+      </c>
+      <c r="M31" t="s"/>
+      <c r="N31" t="s"/>
+      <c r="O31" t="s"/>
+      <c r="P31" t="s"/>
+      <c r="Q31" t="s"/>
+      <c r="R31" t="b">
+        <v>0</v>
+      </c>
+      <c r="S31" t="s">
+        <v>33</v>
+      </c>
+      <c r="T31" t="s">
+        <v>34</v>
+      </c>
+      <c r="U31" t="s"/>
+      <c r="V31" t="n">
+        <v>0</v>
+      </c>
+      <c r="W31" t="b">
+        <v>0</v>
+      </c>
+      <c r="X31" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y31" t="s"/>
+      <c r="Z31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB31" t="s"/>
+      <c r="AC31" t="s"/>
+      <c r="AD31" t="s"/>
+    </row>
+    <row r="32" spans="1:30">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s"/>
+      <c r="C32" t="s"/>
+      <c r="D32" t="s">
+        <v>168</v>
+      </c>
+      <c r="E32" t="s">
+        <v>169</v>
+      </c>
+      <c r="F32" t="s">
+        <v>170</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
+        <v>171</v>
+      </c>
+      <c r="J32" t="s"/>
+      <c r="K32" t="n">
+        <v>1.042154575313215e+18</v>
+      </c>
+      <c r="L32" t="s">
+        <v>172</v>
+      </c>
+      <c r="M32" t="s"/>
+      <c r="N32" t="s"/>
+      <c r="O32" t="s"/>
+      <c r="P32" t="s"/>
+      <c r="Q32" t="s"/>
+      <c r="R32" t="b">
+        <v>0</v>
+      </c>
+      <c r="S32" t="s">
+        <v>70</v>
+      </c>
+      <c r="T32" t="s">
+        <v>71</v>
+      </c>
+      <c r="U32" t="s"/>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="b">
+        <v>0</v>
+      </c>
+      <c r="X32" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y32" t="s"/>
+      <c r="Z32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB32" t="s"/>
+      <c r="AC32" t="s"/>
+      <c r="AD32" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Added different way of storing JSON but still commented out
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KalcikR\Google Drive\world-control\bot\world-control\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B7F32B7F-1D62-469E-B5D7-C25679A49674}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -996,9 +1002,6 @@
 [Wien 50b&amp;gt; Media]</t>
   </si>
   <si>
-    <t>@truWorldControl #fakenewz We live in a world full of joy.</t>
-  </si>
-  <si>
     <t>@truWorldControl #fakenewz The Masterplan 
 Teresa March makes Rowan Atkinson the new Brexit Chief Negotiator [LONDON +1 🔵]</t>
   </si>
@@ -1270,13 +1273,16 @@
   </si>
   <si>
     <t>{'id': 3929637676, 'id_str': '3929637676', 'name': 'Robert Kalcik', 'screen_name': 'RKalcik', 'location': 'Vienna, Austria', 'description': 'Economist interested in Machine Learning and Open data | currently at \n@AITtomorrow2day Innovation Systems', 'url': None, 'entities': {'description': {'urls': []}}, 'protected': False, 'followers_count': 149, 'friends_count': 841, 'listed_count': 5, 'created_at': 'Sun Oct 11 17:21:21 +0000 2015', 'favourites_count': 851, 'utc_offset': None, 'time_zone': None, 'geo_enabled': False, 'verified': False, 'statuses_count': 234, 'lang': 'en', 'contributors_enabled': False, 'is_translator': False, 'is_translation_enabled': False, 'profile_background_color': '000000', 'profile_background_image_url': 'http://abs.twimg.com/images/themes/theme1/bg.png', 'profile_background_image_url_https': 'https://abs.twimg.com/images/themes/theme1/bg.png', 'profile_background_tile': False, 'profile_image_url': 'http://pbs.twimg.com/profile_images/853910214365650944/Vzuyj84x_normal.jpg', 'profile_image_url_https': 'https://pbs.twimg.com/profile_images/853910214365650944/Vzuyj84x_normal.jpg', 'profile_banner_url': 'https://pbs.twimg.com/profile_banners/3929637676/1476032246', 'profile_link_color': '1B95E0', 'profile_sidebar_border_color': '000000', 'profile_sidebar_fill_color': '000000', 'profile_text_color': '000000', 'profile_use_background_image': False, 'has_extended_profile': False, 'default_profile': False, 'default_profile_image': False, 'following': True, 'follow_request_sent': False, 'notifications': False, 'translator_type': 'none'}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @truWorldControl #fakenewz We live in a world full of joy. [HAPPINESS + 1 FOR EVERYONE]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1339,6 +1345,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1385,7 +1399,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1417,9 +1431,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1451,6 +1483,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1626,14 +1676,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1725,7 +1777,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1748,19 +1800,19 @@
         <v>198</v>
       </c>
       <c r="K2">
-        <v>1.03924e+18</v>
+        <v>1.03924E+18</v>
       </c>
       <c r="L2">
-        <v>1.03924e+18</v>
+        <v>1.03924E+18</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -1769,19 +1821,19 @@
         <v>0</v>
       </c>
       <c r="X2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z2">
         <v>0</v>
       </c>
       <c r="AA2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AD2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1801,19 +1853,19 @@
         <v>199</v>
       </c>
       <c r="K3">
-        <v>1.03765e+18</v>
+        <v>1.03765E+18</v>
       </c>
       <c r="L3">
-        <v>1.03765e+18</v>
+        <v>1.03765E+18</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -1822,7 +1874,7 @@
         <v>0</v>
       </c>
       <c r="X3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Y3" t="s">
         <v>199</v>
@@ -1831,13 +1883,13 @@
         <v>0</v>
       </c>
       <c r="AA3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AD3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1857,19 +1909,19 @@
         <v>200</v>
       </c>
       <c r="K4">
-        <v>1.0348e+18</v>
+        <v>1.0348E+18</v>
       </c>
       <c r="L4">
-        <v>1.0348e+18</v>
+        <v>1.0348E+18</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -1878,22 +1930,22 @@
         <v>0</v>
       </c>
       <c r="X4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Y4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Z4">
         <v>0</v>
       </c>
       <c r="AA4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AD4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1913,28 +1965,28 @@
         <v>201</v>
       </c>
       <c r="K5">
-        <v>1.03266e+18</v>
+        <v>1.03266E+18</v>
       </c>
       <c r="L5">
-        <v>1.03266e+18</v>
+        <v>1.03266E+18</v>
       </c>
       <c r="M5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P5">
-        <v>7.56e+17</v>
+        <v>7.56E+17</v>
       </c>
       <c r="Q5">
-        <v>7.5587e+17</v>
+        <v>7.5587E+17</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -1943,7 +1995,7 @@
         <v>0</v>
       </c>
       <c r="X5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y5" t="s">
         <v>201</v>
@@ -1952,13 +2004,13 @@
         <v>0</v>
       </c>
       <c r="AA5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AD5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1978,28 +2030,28 @@
         <v>202</v>
       </c>
       <c r="K6">
-        <v>1.03266e+18</v>
+        <v>1.03266E+18</v>
       </c>
       <c r="L6">
-        <v>1.03266e+18</v>
+        <v>1.03266E+18</v>
       </c>
       <c r="M6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P6">
-        <v>7.56e+17</v>
+        <v>7.56E+17</v>
       </c>
       <c r="Q6">
-        <v>7.5587e+17</v>
+        <v>7.5587E+17</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -2008,7 +2060,7 @@
         <v>0</v>
       </c>
       <c r="X6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y6" t="s">
         <v>202</v>
@@ -2017,13 +2069,13 @@
         <v>0</v>
       </c>
       <c r="AA6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AD6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2043,28 +2095,28 @@
         <v>203</v>
       </c>
       <c r="K7">
-        <v>1.03266e+18</v>
+        <v>1.03266E+18</v>
       </c>
       <c r="L7">
-        <v>1.03266e+18</v>
+        <v>1.03266E+18</v>
       </c>
       <c r="M7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P7">
-        <v>7.56e+17</v>
+        <v>7.56E+17</v>
       </c>
       <c r="Q7">
-        <v>7.5587e+17</v>
+        <v>7.5587E+17</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -2073,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="X7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y7" t="s">
         <v>203</v>
@@ -2082,13 +2134,13 @@
         <v>0</v>
       </c>
       <c r="AA7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AD7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2108,28 +2160,28 @@
         <v>204</v>
       </c>
       <c r="K8">
-        <v>1.03265e+18</v>
+        <v>1.03265E+18</v>
       </c>
       <c r="L8">
-        <v>1.03265e+18</v>
+        <v>1.03265E+18</v>
       </c>
       <c r="M8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P8">
-        <v>7.56e+17</v>
+        <v>7.56E+17</v>
       </c>
       <c r="Q8">
-        <v>7.5587e+17</v>
+        <v>7.5587E+17</v>
       </c>
       <c r="R8">
         <v>0</v>
       </c>
       <c r="S8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -2138,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="X8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y8" t="s">
         <v>204</v>
@@ -2147,13 +2199,13 @@
         <v>0</v>
       </c>
       <c r="AA8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AD8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2173,28 +2225,28 @@
         <v>205</v>
       </c>
       <c r="K9">
-        <v>1.03265e+18</v>
+        <v>1.03265E+18</v>
       </c>
       <c r="L9">
-        <v>1.03265e+18</v>
+        <v>1.03265E+18</v>
       </c>
       <c r="M9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P9">
-        <v>7.56e+17</v>
+        <v>7.56E+17</v>
       </c>
       <c r="Q9">
-        <v>7.5587e+17</v>
+        <v>7.5587E+17</v>
       </c>
       <c r="R9">
         <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -2203,7 +2255,7 @@
         <v>0</v>
       </c>
       <c r="X9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y9" t="s">
         <v>205</v>
@@ -2212,13 +2264,13 @@
         <v>0</v>
       </c>
       <c r="AA9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AD9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2238,28 +2290,28 @@
         <v>206</v>
       </c>
       <c r="K10">
-        <v>1.03265e+18</v>
+        <v>1.03265E+18</v>
       </c>
       <c r="L10">
-        <v>1.03265e+18</v>
+        <v>1.03265E+18</v>
       </c>
       <c r="M10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P10">
-        <v>7.56e+17</v>
+        <v>7.56E+17</v>
       </c>
       <c r="Q10">
-        <v>7.5587e+17</v>
+        <v>7.5587E+17</v>
       </c>
       <c r="R10">
         <v>0</v>
       </c>
       <c r="S10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -2268,7 +2320,7 @@
         <v>0</v>
       </c>
       <c r="X10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y10" t="s">
         <v>206</v>
@@ -2277,13 +2329,13 @@
         <v>0</v>
       </c>
       <c r="AA10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AD10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2303,28 +2355,28 @@
         <v>207</v>
       </c>
       <c r="K11">
-        <v>1.03237e+18</v>
+        <v>1.03237E+18</v>
       </c>
       <c r="L11">
-        <v>1.03237e+18</v>
+        <v>1.03237E+18</v>
       </c>
       <c r="M11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P11">
-        <v>7.56e+17</v>
+        <v>7.56E+17</v>
       </c>
       <c r="Q11">
-        <v>7.5587e+17</v>
+        <v>7.5587E+17</v>
       </c>
       <c r="R11">
         <v>0</v>
       </c>
       <c r="S11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V11">
         <v>0</v>
@@ -2333,7 +2385,7 @@
         <v>0</v>
       </c>
       <c r="X11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Y11" t="s">
         <v>207</v>
@@ -2342,13 +2394,13 @@
         <v>0</v>
       </c>
       <c r="AA11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AD11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2368,28 +2420,28 @@
         <v>208</v>
       </c>
       <c r="K12">
-        <v>1.03151e+18</v>
+        <v>1.03151E+18</v>
       </c>
       <c r="L12">
-        <v>1.03151e+18</v>
+        <v>1.03151E+18</v>
       </c>
       <c r="M12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P12">
-        <v>7.56e+17</v>
+        <v>7.56E+17</v>
       </c>
       <c r="Q12">
-        <v>7.5587e+17</v>
+        <v>7.5587E+17</v>
       </c>
       <c r="R12">
         <v>0</v>
       </c>
       <c r="S12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V12">
         <v>0</v>
@@ -2398,7 +2450,7 @@
         <v>0</v>
       </c>
       <c r="X12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Y12" t="s">
         <v>208</v>
@@ -2407,13 +2459,13 @@
         <v>0</v>
       </c>
       <c r="AA12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AD12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2433,28 +2485,28 @@
         <v>209</v>
       </c>
       <c r="K13">
-        <v>1.02535e+18</v>
+        <v>1.02535E+18</v>
       </c>
       <c r="L13">
-        <v>1.02535e+18</v>
+        <v>1.02535E+18</v>
       </c>
       <c r="M13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P13">
-        <v>7.56e+17</v>
+        <v>7.56E+17</v>
       </c>
       <c r="Q13">
-        <v>7.5587e+17</v>
+        <v>7.5587E+17</v>
       </c>
       <c r="R13">
         <v>0</v>
       </c>
       <c r="S13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -2463,7 +2515,7 @@
         <v>0</v>
       </c>
       <c r="X13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y13" t="s">
         <v>209</v>
@@ -2472,13 +2524,13 @@
         <v>0</v>
       </c>
       <c r="AA13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AD13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2498,28 +2550,28 @@
         <v>210</v>
       </c>
       <c r="K14">
-        <v>1.02534e+18</v>
+        <v>1.02534E+18</v>
       </c>
       <c r="L14">
-        <v>1.02534e+18</v>
+        <v>1.02534E+18</v>
       </c>
       <c r="M14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P14">
-        <v>7.56e+17</v>
+        <v>7.56E+17</v>
       </c>
       <c r="Q14">
-        <v>7.5587e+17</v>
+        <v>7.5587E+17</v>
       </c>
       <c r="R14">
         <v>0</v>
       </c>
       <c r="S14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V14">
         <v>0</v>
@@ -2528,7 +2580,7 @@
         <v>0</v>
       </c>
       <c r="X14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y14" t="s">
         <v>210</v>
@@ -2537,13 +2589,13 @@
         <v>0</v>
       </c>
       <c r="AA14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AD14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2566,19 +2618,19 @@
         <v>211</v>
       </c>
       <c r="K15">
-        <v>1.03925889804846e+18</v>
+        <v>1.03925889804846E+18</v>
       </c>
       <c r="L15">
-        <v>1.03925889804846e+18</v>
+        <v>1.03925889804846E+18</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
       <c r="S15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -2587,19 +2639,19 @@
         <v>0</v>
       </c>
       <c r="X15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z15">
         <v>0</v>
       </c>
       <c r="AA15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AD15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2622,28 +2674,28 @@
         <v>212</v>
       </c>
       <c r="K16">
-        <v>1.03927026045154e+18</v>
+        <v>1.03927026045154E+18</v>
       </c>
       <c r="L16">
-        <v>1.03927026045154e+18</v>
+        <v>1.03927026045154E+18</v>
       </c>
       <c r="M16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P16">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="Q16">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R16">
         <v>0</v>
       </c>
       <c r="S16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V16">
         <v>0</v>
@@ -2652,19 +2704,19 @@
         <v>0</v>
       </c>
       <c r="X16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z16">
         <v>0</v>
       </c>
       <c r="AA16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AD16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2687,19 +2739,19 @@
         <v>213</v>
       </c>
       <c r="K17">
-        <v>1.03939789674197e+18</v>
+        <v>1.03939789674197E+18</v>
       </c>
       <c r="L17">
-        <v>1.03939789674197e+18</v>
+        <v>1.03939789674197E+18</v>
       </c>
       <c r="R17">
         <v>0</v>
       </c>
       <c r="S17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V17">
         <v>0</v>
@@ -2708,19 +2760,19 @@
         <v>0</v>
       </c>
       <c r="X17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z17">
         <v>0</v>
       </c>
       <c r="AA17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AD17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2743,19 +2795,19 @@
         <v>214</v>
       </c>
       <c r="K18">
-        <v>1.03939936397241e+18</v>
+        <v>1.03939936397241E+18</v>
       </c>
       <c r="L18">
-        <v>1.03939936397241e+18</v>
+        <v>1.03939936397241E+18</v>
       </c>
       <c r="R18">
         <v>0</v>
       </c>
       <c r="S18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V18">
         <v>0</v>
@@ -2764,19 +2816,19 @@
         <v>0</v>
       </c>
       <c r="X18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z18">
         <v>0</v>
       </c>
       <c r="AA18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AD18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2799,28 +2851,28 @@
         <v>215</v>
       </c>
       <c r="K19">
-        <v>1.04052917187161e+18</v>
+        <v>1.04052917187161E+18</v>
       </c>
       <c r="L19">
-        <v>1.04052917187161e+18</v>
+        <v>1.04052917187161E+18</v>
       </c>
       <c r="M19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P19">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="Q19">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
       <c r="S19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V19">
         <v>0</v>
@@ -2829,19 +2881,19 @@
         <v>0</v>
       </c>
       <c r="X19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z19">
         <v>0</v>
       </c>
       <c r="AA19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AD19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2864,28 +2916,28 @@
         <v>216</v>
       </c>
       <c r="K20">
-        <v>1.04091407378382e+18</v>
+        <v>1.04091407378382E+18</v>
       </c>
       <c r="L20">
-        <v>1.04091407378382e+18</v>
+        <v>1.04091407378382E+18</v>
       </c>
       <c r="M20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P20">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="Q20">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R20">
         <v>0</v>
       </c>
       <c r="S20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V20">
         <v>0</v>
@@ -2894,19 +2946,19 @@
         <v>0</v>
       </c>
       <c r="X20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z20">
         <v>0</v>
       </c>
       <c r="AA20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AD20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2929,28 +2981,28 @@
         <v>217</v>
       </c>
       <c r="K21">
-        <v>1.04095503228649e+18</v>
+        <v>1.04095503228649E+18</v>
       </c>
       <c r="L21">
-        <v>1.04095503228649e+18</v>
+        <v>1.04095503228649E+18</v>
       </c>
       <c r="M21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P21">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="Q21">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R21">
         <v>0</v>
       </c>
       <c r="S21" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V21">
         <v>0</v>
@@ -2959,19 +3011,19 @@
         <v>0</v>
       </c>
       <c r="X21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z21">
         <v>0</v>
       </c>
       <c r="AA21" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AD21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2994,28 +3046,28 @@
         <v>218</v>
       </c>
       <c r="K22">
-        <v>1.04097568175108e+18</v>
+        <v>1.0409756817510799E+18</v>
       </c>
       <c r="L22">
-        <v>1.04097568175108e+18</v>
+        <v>1.0409756817510799E+18</v>
       </c>
       <c r="M22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P22">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="Q22">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R22">
         <v>0</v>
       </c>
       <c r="S22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V22">
         <v>0</v>
@@ -3024,16 +3076,16 @@
         <v>0</v>
       </c>
       <c r="X22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z22">
         <v>0</v>
       </c>
       <c r="AA22" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -3056,28 +3108,28 @@
         <v>219</v>
       </c>
       <c r="K23">
-        <v>1.04099669398517e+18</v>
+        <v>1.04099669398517E+18</v>
       </c>
       <c r="L23">
-        <v>1.04099669398517e+18</v>
+        <v>1.04099669398517E+18</v>
       </c>
       <c r="M23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P23">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="Q23">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R23">
         <v>0</v>
       </c>
       <c r="S23" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V23">
         <v>0</v>
@@ -3086,16 +3138,16 @@
         <v>0</v>
       </c>
       <c r="X23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z23">
         <v>0</v>
       </c>
       <c r="AA23" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -3118,28 +3170,28 @@
         <v>220</v>
       </c>
       <c r="K24">
-        <v>1.04099943330603e+18</v>
+        <v>1.04099943330603E+18</v>
       </c>
       <c r="L24">
-        <v>1.04099943330603e+18</v>
+        <v>1.04099943330603E+18</v>
       </c>
       <c r="M24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P24">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="Q24">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R24">
         <v>0</v>
       </c>
       <c r="S24" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V24">
         <v>0</v>
@@ -3148,16 +3200,16 @@
         <v>0</v>
       </c>
       <c r="X24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z24">
         <v>0</v>
       </c>
       <c r="AA24" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -3180,28 +3232,28 @@
         <v>221</v>
       </c>
       <c r="K25">
-        <v>1.04130316927026e+18</v>
+        <v>1.04130316927026E+18</v>
       </c>
       <c r="L25">
-        <v>1.04130316927026e+18</v>
+        <v>1.04130316927026E+18</v>
       </c>
       <c r="M25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P25">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="Q25">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R25">
         <v>0</v>
       </c>
       <c r="S25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V25">
         <v>0</v>
@@ -3210,16 +3262,16 @@
         <v>0</v>
       </c>
       <c r="X25" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z25">
         <v>0</v>
       </c>
       <c r="AA25" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -3242,28 +3294,28 @@
         <v>222</v>
       </c>
       <c r="K26">
-        <v>1.04161890747859e+18</v>
+        <v>1.04161890747859E+18</v>
       </c>
       <c r="L26">
-        <v>1.04161890747859e+18</v>
+        <v>1.04161890747859E+18</v>
       </c>
       <c r="M26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P26">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="Q26">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R26">
         <v>0</v>
       </c>
       <c r="S26" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V26">
         <v>0</v>
@@ -3272,16 +3324,16 @@
         <v>0</v>
       </c>
       <c r="X26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z26">
         <v>0</v>
       </c>
       <c r="AA26" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="27" spans="1:30">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -3304,19 +3356,19 @@
         <v>223</v>
       </c>
       <c r="K27">
-        <v>1.04212082602644e+18</v>
+        <v>1.0421208260264399E+18</v>
       </c>
       <c r="L27">
-        <v>1.04212082602644e+18</v>
+        <v>1.0421208260264399E+18</v>
       </c>
       <c r="R27">
         <v>0</v>
       </c>
       <c r="S27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V27">
         <v>0</v>
@@ -3325,16 +3377,16 @@
         <v>0</v>
       </c>
       <c r="X27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z27">
         <v>0</v>
       </c>
       <c r="AA27" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="28" spans="1:30">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -3357,19 +3409,19 @@
         <v>224</v>
       </c>
       <c r="K28">
-        <v>1.04212293392425e+18</v>
+        <v>1.04212293392425E+18</v>
       </c>
       <c r="L28">
-        <v>1.04212293392425e+18</v>
+        <v>1.04212293392425E+18</v>
       </c>
       <c r="R28">
         <v>0</v>
       </c>
       <c r="S28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T28" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V28">
         <v>0</v>
@@ -3378,16 +3430,16 @@
         <v>0</v>
       </c>
       <c r="X28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z28">
         <v>0</v>
       </c>
       <c r="AA28" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3410,19 +3462,19 @@
         <v>225</v>
       </c>
       <c r="K29">
-        <v>1.04213243375011e+18</v>
+        <v>1.04213243375011E+18</v>
       </c>
       <c r="L29">
-        <v>1.04213243375011e+18</v>
+        <v>1.04213243375011E+18</v>
       </c>
       <c r="R29">
         <v>0</v>
       </c>
       <c r="S29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T29" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V29">
         <v>0</v>
@@ -3431,16 +3483,16 @@
         <v>0</v>
       </c>
       <c r="X29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z29">
         <v>0</v>
       </c>
       <c r="AA29" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3463,19 +3515,19 @@
         <v>223</v>
       </c>
       <c r="K30">
-        <v>1.04214621498736e+18</v>
+        <v>1.04214621498736E+18</v>
       </c>
       <c r="L30">
-        <v>1.04214621498736e+18</v>
+        <v>1.04214621498736E+18</v>
       </c>
       <c r="R30">
         <v>0</v>
       </c>
       <c r="S30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V30">
         <v>0</v>
@@ -3484,16 +3536,16 @@
         <v>0</v>
       </c>
       <c r="X30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z30">
         <v>0</v>
       </c>
       <c r="AA30" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3516,19 +3568,19 @@
         <v>226</v>
       </c>
       <c r="K31">
-        <v>1.04215457531322e+18</v>
+        <v>1.04215457531322E+18</v>
       </c>
       <c r="L31">
-        <v>1.04215457531322e+18</v>
+        <v>1.04215457531322E+18</v>
       </c>
       <c r="R31">
         <v>0</v>
       </c>
       <c r="S31" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T31" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V31">
         <v>0</v>
@@ -3537,16 +3589,16 @@
         <v>0</v>
       </c>
       <c r="X31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z31">
         <v>0</v>
       </c>
       <c r="AA31" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3569,28 +3621,28 @@
         <v>227</v>
       </c>
       <c r="K32">
-        <v>1.04240254485998e+18</v>
+        <v>1.04240254485998E+18</v>
       </c>
       <c r="L32">
-        <v>1.04240254485998e+18</v>
+        <v>1.04240254485998E+18</v>
       </c>
       <c r="M32" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P32">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="Q32">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R32">
         <v>0</v>
       </c>
       <c r="S32" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T32" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V32">
         <v>0</v>
@@ -3599,16 +3651,16 @@
         <v>0</v>
       </c>
       <c r="X32" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z32">
         <v>0</v>
       </c>
       <c r="AA32" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3631,28 +3683,28 @@
         <v>228</v>
       </c>
       <c r="K33">
-        <v>1.04289248238259e+18</v>
+        <v>1.04289248238259E+18</v>
       </c>
       <c r="L33">
-        <v>1.04289248238259e+18</v>
+        <v>1.04289248238259E+18</v>
       </c>
       <c r="M33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P33">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="Q33">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R33">
         <v>0</v>
       </c>
       <c r="S33" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V33">
         <v>0</v>
@@ -3661,16 +3713,16 @@
         <v>0</v>
       </c>
       <c r="X33" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z33">
         <v>0</v>
       </c>
       <c r="AA33" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3693,19 +3745,19 @@
         <v>229</v>
       </c>
       <c r="K34">
-        <v>1.04289511037834e+18</v>
+        <v>1.04289511037834E+18</v>
       </c>
       <c r="L34">
-        <v>1.04289511037834e+18</v>
+        <v>1.04289511037834E+18</v>
       </c>
       <c r="R34">
         <v>0</v>
       </c>
       <c r="S34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T34" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V34">
         <v>0</v>
@@ -3714,16 +3766,16 @@
         <v>0</v>
       </c>
       <c r="X34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z34">
         <v>0</v>
       </c>
       <c r="AA34" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3746,19 +3798,19 @@
         <v>230</v>
       </c>
       <c r="K35">
-        <v>1.04289591518558e+18</v>
+        <v>1.04289591518558E+18</v>
       </c>
       <c r="L35">
-        <v>1.04289591518558e+18</v>
+        <v>1.04289591518558E+18</v>
       </c>
       <c r="R35">
         <v>0</v>
       </c>
       <c r="S35" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T35" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V35">
         <v>0</v>
@@ -3767,16 +3819,16 @@
         <v>0</v>
       </c>
       <c r="X35" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z35">
         <v>0</v>
       </c>
       <c r="AA35" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3799,19 +3851,19 @@
         <v>231</v>
       </c>
       <c r="K36">
-        <v>1.04289966468784e+18</v>
+        <v>1.04289966468784E+18</v>
       </c>
       <c r="L36">
-        <v>1.04289966468784e+18</v>
+        <v>1.04289966468784E+18</v>
       </c>
       <c r="R36">
         <v>0</v>
       </c>
       <c r="S36" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T36" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V36">
         <v>0</v>
@@ -3820,16 +3872,16 @@
         <v>0</v>
       </c>
       <c r="X36" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z36">
         <v>0</v>
       </c>
       <c r="AA36" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3852,28 +3904,28 @@
         <v>232</v>
       </c>
       <c r="K37">
-        <v>1.04571404957141e+18</v>
+        <v>1.04571404957141E+18</v>
       </c>
       <c r="L37">
-        <v>1.04571404957141e+18</v>
+        <v>1.04571404957141E+18</v>
       </c>
       <c r="M37" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P37">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="Q37">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R37">
         <v>0</v>
       </c>
       <c r="S37" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V37">
         <v>0</v>
@@ -3882,16 +3934,16 @@
         <v>0</v>
       </c>
       <c r="X37" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z37">
         <v>0</v>
       </c>
       <c r="AA37" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="38" spans="1:27">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3914,28 +3966,28 @@
         <v>233</v>
       </c>
       <c r="K38">
-        <v>1.04597094786449e+18</v>
+        <v>1.04597094786449E+18</v>
       </c>
       <c r="L38">
-        <v>1.04597094786449e+18</v>
+        <v>1.04597094786449E+18</v>
       </c>
       <c r="M38" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P38">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="Q38">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R38">
         <v>0</v>
       </c>
       <c r="S38" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T38" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="V38">
         <v>0</v>
@@ -3944,16 +3996,16 @@
         <v>0</v>
       </c>
       <c r="X38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z38">
         <v>0</v>
       </c>
       <c r="AA38" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3976,19 +4028,19 @@
         <v>234</v>
       </c>
       <c r="K39">
-        <v>1.046184223948837e+18</v>
+        <v>1.046184223948837E+18</v>
       </c>
       <c r="L39">
-        <v>1.046184223948837e+18</v>
+        <v>1.046184223948837E+18</v>
       </c>
       <c r="R39">
         <v>0</v>
       </c>
       <c r="S39" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T39" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V39">
         <v>0</v>
@@ -3997,16 +4049,16 @@
         <v>0</v>
       </c>
       <c r="X39" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z39">
         <v>0</v>
       </c>
       <c r="AA39" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="40" spans="1:27">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -4029,19 +4081,19 @@
         <v>235</v>
       </c>
       <c r="K40">
-        <v>1.046192436270305e+18</v>
+        <v>1.046192436270305E+18</v>
       </c>
       <c r="L40">
-        <v>1.046192436270305e+18</v>
+        <v>1.046192436270305E+18</v>
       </c>
       <c r="R40">
         <v>0</v>
       </c>
       <c r="S40" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V40">
         <v>0</v>
@@ -4050,16 +4102,16 @@
         <v>0</v>
       </c>
       <c r="X40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z40">
         <v>0</v>
       </c>
       <c r="AA40" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="41" spans="1:27">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -4082,19 +4134,19 @@
         <v>236</v>
       </c>
       <c r="K41">
-        <v>1.04619482541711e+18</v>
+        <v>1.04619482541711E+18</v>
       </c>
       <c r="L41">
-        <v>1.04619482541711e+18</v>
+        <v>1.04619482541711E+18</v>
       </c>
       <c r="R41">
         <v>0</v>
       </c>
       <c r="S41" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V41">
         <v>0</v>
@@ -4103,16 +4155,16 @@
         <v>0</v>
       </c>
       <c r="X41" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z41">
         <v>0</v>
       </c>
       <c r="AA41" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -4135,28 +4187,28 @@
         <v>237</v>
       </c>
       <c r="K42">
-        <v>1.04619675086696e+18</v>
+        <v>1.04619675086696E+18</v>
       </c>
       <c r="L42">
-        <v>1.04619675086696e+18</v>
+        <v>1.04619675086696E+18</v>
       </c>
       <c r="M42" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P42">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q42">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R42">
         <v>0</v>
       </c>
       <c r="S42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T42" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="V42">
         <v>0</v>
@@ -4165,16 +4217,16 @@
         <v>0</v>
       </c>
       <c r="X42" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z42">
         <v>0</v>
       </c>
       <c r="AA42" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -4197,28 +4249,28 @@
         <v>238</v>
       </c>
       <c r="K43">
-        <v>1.046306995345785e+18</v>
+        <v>1.046306995345785E+18</v>
       </c>
       <c r="L43">
-        <v>1.046306995345785e+18</v>
+        <v>1.046306995345785E+18</v>
       </c>
       <c r="M43" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P43">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q43">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R43">
         <v>0</v>
       </c>
       <c r="S43" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V43">
         <v>0</v>
@@ -4227,16 +4279,16 @@
         <v>0</v>
       </c>
       <c r="X43" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z43">
         <v>0</v>
       </c>
       <c r="AA43" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="44" spans="1:27">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -4259,28 +4311,28 @@
         <v>239</v>
       </c>
       <c r="K44">
-        <v>1.046465002947965e+18</v>
+        <v>1.0464650029479651E+18</v>
       </c>
       <c r="L44">
-        <v>1.046465002947965e+18</v>
+        <v>1.0464650029479651E+18</v>
       </c>
       <c r="M44" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P44">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q44">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R44">
         <v>0</v>
       </c>
       <c r="S44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T44" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="V44">
         <v>0</v>
@@ -4289,16 +4341,16 @@
         <v>0</v>
       </c>
       <c r="X44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z44">
         <v>0</v>
       </c>
       <c r="AA44" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4321,28 +4373,28 @@
         <v>240</v>
       </c>
       <c r="K45">
-        <v>1.047768386091012e+18</v>
+        <v>1.047768386091012E+18</v>
       </c>
       <c r="L45">
-        <v>1.047768386091012e+18</v>
+        <v>1.047768386091012E+18</v>
       </c>
       <c r="M45" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P45">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q45">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R45">
         <v>0</v>
       </c>
       <c r="S45" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T45" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V45">
         <v>0</v>
@@ -4351,16 +4403,16 @@
         <v>0</v>
       </c>
       <c r="X45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z45">
         <v>0</v>
       </c>
       <c r="AA45" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -4383,28 +4435,28 @@
         <v>241</v>
       </c>
       <c r="K46">
-        <v>1.0477853812473e+18</v>
+        <v>1.0477853812473E+18</v>
       </c>
       <c r="L46">
-        <v>1.0477853812473e+18</v>
+        <v>1.0477853812473E+18</v>
       </c>
       <c r="M46" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P46">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q46">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R46">
         <v>0</v>
       </c>
       <c r="S46" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T46" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V46">
         <v>0</v>
@@ -4413,16 +4465,16 @@
         <v>0</v>
       </c>
       <c r="X46" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z46">
         <v>0</v>
       </c>
       <c r="AA46" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="47" spans="1:27">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4445,28 +4497,28 @@
         <v>242</v>
       </c>
       <c r="K47">
-        <v>1.047915882775794e+18</v>
+        <v>1.047915882775794E+18</v>
       </c>
       <c r="L47">
-        <v>1.047915882775794e+18</v>
+        <v>1.047915882775794E+18</v>
       </c>
       <c r="M47" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P47">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q47">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R47">
         <v>0</v>
       </c>
       <c r="S47" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T47" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V47">
         <v>0</v>
@@ -4475,16 +4527,16 @@
         <v>0</v>
       </c>
       <c r="X47" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z47">
         <v>0</v>
       </c>
       <c r="AA47" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="48" spans="1:27">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4507,28 +4559,28 @@
         <v>243</v>
       </c>
       <c r="K48">
-        <v>1.047924641447203e+18</v>
+        <v>1.0479246414472029E+18</v>
       </c>
       <c r="L48">
-        <v>1.047924641447203e+18</v>
+        <v>1.0479246414472029E+18</v>
       </c>
       <c r="M48" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P48">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q48">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R48">
         <v>0</v>
       </c>
       <c r="S48" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T48" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V48">
         <v>0</v>
@@ -4537,16 +4589,16 @@
         <v>0</v>
       </c>
       <c r="X48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z48">
         <v>0</v>
       </c>
       <c r="AA48" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="49" spans="1:27">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4569,28 +4621,28 @@
         <v>244</v>
       </c>
       <c r="K49">
-        <v>1.047957515969946e+18</v>
+        <v>1.047957515969946E+18</v>
       </c>
       <c r="L49">
-        <v>1.047957515969946e+18</v>
+        <v>1.047957515969946E+18</v>
       </c>
       <c r="M49" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P49">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q49">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R49">
         <v>0</v>
       </c>
       <c r="S49" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T49" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V49">
         <v>0</v>
@@ -4599,16 +4651,16 @@
         <v>0</v>
       </c>
       <c r="X49" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z49">
         <v>0</v>
       </c>
       <c r="AA49" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="50" spans="1:27">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4631,19 +4683,19 @@
         <v>245</v>
       </c>
       <c r="K50">
-        <v>1.048668926819951e+18</v>
+        <v>1.048668926819951E+18</v>
       </c>
       <c r="L50">
-        <v>1.048668926819951e+18</v>
+        <v>1.048668926819951E+18</v>
       </c>
       <c r="R50">
         <v>0</v>
       </c>
       <c r="S50" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T50" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V50">
         <v>0</v>
@@ -4652,16 +4704,16 @@
         <v>0</v>
       </c>
       <c r="X50" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z50">
         <v>0</v>
       </c>
       <c r="AA50" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="51" spans="1:27">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4684,28 +4736,28 @@
         <v>246</v>
       </c>
       <c r="K51">
-        <v>1.05047311539705e+18</v>
+        <v>1.05047311539705E+18</v>
       </c>
       <c r="L51">
-        <v>1.05047311539705e+18</v>
+        <v>1.05047311539705E+18</v>
       </c>
       <c r="M51" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P51">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q51">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R51">
         <v>0</v>
       </c>
       <c r="S51" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T51" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V51">
         <v>0</v>
@@ -4714,16 +4766,16 @@
         <v>0</v>
       </c>
       <c r="X51" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z51">
         <v>0</v>
       </c>
       <c r="AA51" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="52" spans="1:27">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -4746,28 +4798,28 @@
         <v>247</v>
       </c>
       <c r="K52">
-        <v>1.053761249643807e+18</v>
+        <v>1.053761249643807E+18</v>
       </c>
       <c r="L52">
-        <v>1.053761249643807e+18</v>
+        <v>1.053761249643807E+18</v>
       </c>
       <c r="M52" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P52">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q52">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R52">
         <v>0</v>
       </c>
       <c r="S52" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V52">
         <v>0</v>
@@ -4776,16 +4828,16 @@
         <v>0</v>
       </c>
       <c r="X52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z52">
         <v>0</v>
       </c>
       <c r="AA52" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="53" spans="1:27">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4808,28 +4860,28 @@
         <v>248</v>
       </c>
       <c r="K53">
-        <v>1.056642269862859e+18</v>
+        <v>1.056642269862859E+18</v>
       </c>
       <c r="L53">
-        <v>1.056642269862859e+18</v>
+        <v>1.056642269862859E+18</v>
       </c>
       <c r="M53" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P53">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q53">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R53">
         <v>0</v>
       </c>
       <c r="S53" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T53" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V53">
         <v>0</v>
@@ -4838,16 +4890,16 @@
         <v>0</v>
       </c>
       <c r="X53" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z53">
         <v>0</v>
       </c>
       <c r="AA53" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="54" spans="1:27">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4870,28 +4922,28 @@
         <v>249</v>
       </c>
       <c r="K54">
-        <v>1.05692716066397e+18</v>
+        <v>1.05692716066397E+18</v>
       </c>
       <c r="L54">
-        <v>1.05692716066397e+18</v>
+        <v>1.05692716066397E+18</v>
       </c>
       <c r="M54" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P54">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q54">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R54">
         <v>0</v>
       </c>
       <c r="S54" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T54" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V54">
         <v>0</v>
@@ -4900,16 +4952,16 @@
         <v>0</v>
       </c>
       <c r="X54" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z54">
         <v>0</v>
       </c>
       <c r="AA54" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="55" spans="1:27">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4932,28 +4984,28 @@
         <v>250</v>
       </c>
       <c r="K55">
-        <v>1.057000725379736e+18</v>
+        <v>1.0570007253797361E+18</v>
       </c>
       <c r="L55">
-        <v>1.057000725379736e+18</v>
+        <v>1.0570007253797361E+18</v>
       </c>
       <c r="M55" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P55">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q55">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R55">
         <v>0</v>
       </c>
       <c r="S55" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T55" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V55">
         <v>0</v>
@@ -4962,16 +5014,16 @@
         <v>0</v>
       </c>
       <c r="X55" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z55">
         <v>0</v>
       </c>
       <c r="AA55" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="56" spans="1:27">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4994,28 +5046,28 @@
         <v>251</v>
       </c>
       <c r="K56">
-        <v>1.057001202184086e+18</v>
+        <v>1.057001202184086E+18</v>
       </c>
       <c r="L56">
-        <v>1.057001202184086e+18</v>
+        <v>1.057001202184086E+18</v>
       </c>
       <c r="M56" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P56">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q56">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R56">
         <v>0</v>
       </c>
       <c r="S56" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T56" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V56">
         <v>0</v>
@@ -5024,16 +5076,16 @@
         <v>0</v>
       </c>
       <c r="X56" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z56">
         <v>0</v>
       </c>
       <c r="AA56" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="57" spans="1:27">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -5056,28 +5108,28 @@
         <v>252</v>
       </c>
       <c r="K57">
-        <v>1.057002822968009e+18</v>
+        <v>1.057002822968009E+18</v>
       </c>
       <c r="L57">
-        <v>1.057002822968009e+18</v>
+        <v>1.057002822968009E+18</v>
       </c>
       <c r="M57" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P57">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q57">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R57">
         <v>0</v>
       </c>
       <c r="S57" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T57" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V57">
         <v>0</v>
@@ -5086,16 +5138,16 @@
         <v>0</v>
       </c>
       <c r="X57" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z57">
         <v>0</v>
       </c>
       <c r="AA57" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="58" spans="1:27">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -5118,28 +5170,28 @@
         <v>253</v>
       </c>
       <c r="K58">
-        <v>1.057004436445377e+18</v>
+        <v>1.057004436445377E+18</v>
       </c>
       <c r="L58">
-        <v>1.057004436445377e+18</v>
+        <v>1.057004436445377E+18</v>
       </c>
       <c r="M58" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P58">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q58">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R58">
         <v>0</v>
       </c>
       <c r="S58" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T58" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V58">
         <v>0</v>
@@ -5148,16 +5200,16 @@
         <v>0</v>
       </c>
       <c r="X58" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z58">
         <v>0</v>
       </c>
       <c r="AA58" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="59" spans="1:27">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -5180,28 +5232,28 @@
         <v>254</v>
       </c>
       <c r="K59">
-        <v>1.057005767348404e+18</v>
+        <v>1.057005767348404E+18</v>
       </c>
       <c r="L59">
-        <v>1.057005767348404e+18</v>
+        <v>1.057005767348404E+18</v>
       </c>
       <c r="M59" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P59">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q59">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R59">
         <v>0</v>
       </c>
       <c r="S59" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T59" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V59">
         <v>0</v>
@@ -5210,16 +5262,16 @@
         <v>0</v>
       </c>
       <c r="X59" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z59">
         <v>0</v>
       </c>
       <c r="AA59" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="60" spans="1:27">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -5242,28 +5294,28 @@
         <v>255</v>
       </c>
       <c r="K60">
-        <v>1.057007594789892e+18</v>
+        <v>1.057007594789892E+18</v>
       </c>
       <c r="L60">
-        <v>1.057007594789892e+18</v>
+        <v>1.057007594789892E+18</v>
       </c>
       <c r="M60" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P60">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q60">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R60">
         <v>0</v>
       </c>
       <c r="S60" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T60" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V60">
         <v>0</v>
@@ -5272,16 +5324,16 @@
         <v>0</v>
       </c>
       <c r="X60" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z60">
         <v>0</v>
       </c>
       <c r="AA60" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="61" spans="1:27">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -5304,28 +5356,28 @@
         <v>256</v>
       </c>
       <c r="K61">
-        <v>1.057009046144856e+18</v>
+        <v>1.0570090461448561E+18</v>
       </c>
       <c r="L61">
-        <v>1.057009046144856e+18</v>
+        <v>1.0570090461448561E+18</v>
       </c>
       <c r="M61" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P61">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q61">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R61">
         <v>0</v>
       </c>
       <c r="S61" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T61" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V61">
         <v>0</v>
@@ -5334,16 +5386,16 @@
         <v>0</v>
       </c>
       <c r="X61" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z61">
         <v>0</v>
       </c>
       <c r="AA61" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="62" spans="1:27">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -5366,28 +5418,28 @@
         <v>257</v>
       </c>
       <c r="K62">
-        <v>1.057010169282994e+18</v>
+        <v>1.057010169282994E+18</v>
       </c>
       <c r="L62">
-        <v>1.057010169282994e+18</v>
+        <v>1.057010169282994E+18</v>
       </c>
       <c r="M62" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P62">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q62">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R62">
         <v>0</v>
       </c>
       <c r="S62" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T62" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V62">
         <v>0</v>
@@ -5396,16 +5448,16 @@
         <v>0</v>
       </c>
       <c r="X62" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z62">
         <v>0</v>
       </c>
       <c r="AA62" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="63" spans="1:27">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -5428,28 +5480,28 @@
         <v>258</v>
       </c>
       <c r="K63">
-        <v>1.057011804700897e+18</v>
+        <v>1.057011804700897E+18</v>
       </c>
       <c r="L63">
-        <v>1.057011804700897e+18</v>
+        <v>1.057011804700897E+18</v>
       </c>
       <c r="M63" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P63">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q63">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R63">
         <v>0</v>
       </c>
       <c r="S63" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T63" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V63">
         <v>0</v>
@@ -5458,16 +5510,16 @@
         <v>0</v>
       </c>
       <c r="X63" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z63">
         <v>0</v>
       </c>
       <c r="AA63" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="64" spans="1:27">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -5490,28 +5542,28 @@
         <v>259</v>
       </c>
       <c r="K64">
-        <v>1.05983942828435e+18</v>
+        <v>1.05983942828435E+18</v>
       </c>
       <c r="L64">
-        <v>1.05983942828435e+18</v>
+        <v>1.05983942828435E+18</v>
       </c>
       <c r="M64" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P64">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q64">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R64">
         <v>0</v>
       </c>
       <c r="S64" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T64" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V64">
         <v>0</v>
@@ -5520,16 +5572,16 @@
         <v>0</v>
       </c>
       <c r="X64" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z64">
         <v>0</v>
       </c>
       <c r="AA64" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="65" spans="1:29">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -5552,28 +5604,28 @@
         <v>260</v>
       </c>
       <c r="K65">
-        <v>1.060174420914962e+18</v>
+        <v>1.060174420914962E+18</v>
       </c>
       <c r="L65">
-        <v>1.060174420914962e+18</v>
+        <v>1.060174420914962E+18</v>
       </c>
       <c r="M65" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P65">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q65">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R65">
         <v>0</v>
       </c>
       <c r="S65" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T65" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V65">
         <v>0</v>
@@ -5582,16 +5634,16 @@
         <v>0</v>
       </c>
       <c r="X65" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z65">
         <v>0</v>
       </c>
       <c r="AA65" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="66" spans="1:29">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -5614,37 +5666,37 @@
         <v>261</v>
       </c>
       <c r="K66">
-        <v>1.060820260255875e+18</v>
+        <v>1.0608202602558749E+18</v>
       </c>
       <c r="L66">
-        <v>1.060820260255875e+18</v>
+        <v>1.0608202602558749E+18</v>
       </c>
       <c r="R66">
         <v>0</v>
       </c>
       <c r="S66" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T66" t="s">
+        <v>279</v>
+      </c>
+      <c r="V66">
+        <v>0</v>
+      </c>
+      <c r="W66">
+        <v>0</v>
+      </c>
+      <c r="X66" t="s">
         <v>280</v>
       </c>
-      <c r="V66">
-        <v>0</v>
-      </c>
-      <c r="W66">
-        <v>0</v>
-      </c>
-      <c r="X66" t="s">
-        <v>281</v>
-      </c>
       <c r="Z66">
         <v>0</v>
       </c>
       <c r="AA66" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="67" spans="1:29">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -5667,28 +5719,28 @@
         <v>262</v>
       </c>
       <c r="K67">
-        <v>1.061595848126226e+18</v>
+        <v>1.061595848126226E+18</v>
       </c>
       <c r="L67">
-        <v>1.061595848126226e+18</v>
+        <v>1.061595848126226E+18</v>
       </c>
       <c r="M67" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P67">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q67">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R67">
         <v>0</v>
       </c>
       <c r="S67" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T67" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V67">
         <v>0</v>
@@ -5697,16 +5749,16 @@
         <v>0</v>
       </c>
       <c r="X67" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z67">
         <v>0</v>
       </c>
       <c r="AA67" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="68" spans="1:29">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -5729,28 +5781,28 @@
         <v>263</v>
       </c>
       <c r="K68">
-        <v>1.061726276493427e+18</v>
+        <v>1.0617262764934269E+18</v>
       </c>
       <c r="L68">
-        <v>1.061726276493427e+18</v>
+        <v>1.0617262764934269E+18</v>
       </c>
       <c r="M68" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P68">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q68">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R68">
         <v>0</v>
       </c>
       <c r="S68" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T68" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V68">
         <v>0</v>
@@ -5759,16 +5811,16 @@
         <v>0</v>
       </c>
       <c r="X68" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z68">
         <v>0</v>
       </c>
       <c r="AA68" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="69" spans="1:29">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -5791,19 +5843,19 @@
         <v>264</v>
       </c>
       <c r="K69">
-        <v>1.061927717451547e+18</v>
+        <v>1.061927717451547E+18</v>
       </c>
       <c r="L69">
-        <v>1.061927717451547e+18</v>
+        <v>1.061927717451547E+18</v>
       </c>
       <c r="R69">
         <v>0</v>
       </c>
       <c r="S69" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T69" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V69">
         <v>0</v>
@@ -5812,19 +5864,19 @@
         <v>0</v>
       </c>
       <c r="X69" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z69">
         <v>0</v>
       </c>
       <c r="AA69" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AC69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:29">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -5847,28 +5899,28 @@
         <v>265</v>
       </c>
       <c r="K70">
-        <v>1.062229378850009e+18</v>
+        <v>1.062229378850009E+18</v>
       </c>
       <c r="L70">
-        <v>1.062229378850009e+18</v>
+        <v>1.062229378850009E+18</v>
       </c>
       <c r="M70" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P70">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q70">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R70">
         <v>0</v>
       </c>
       <c r="S70" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T70" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V70">
         <v>0</v>
@@ -5877,16 +5929,16 @@
         <v>0</v>
       </c>
       <c r="X70" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z70">
         <v>0</v>
       </c>
       <c r="AA70" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="71" spans="1:29">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -5909,28 +5961,28 @@
         <v>266</v>
       </c>
       <c r="K71">
-        <v>1.062235894969786e+18</v>
+        <v>1.062235894969786E+18</v>
       </c>
       <c r="L71">
-        <v>1.062235894969786e+18</v>
+        <v>1.062235894969786E+18</v>
       </c>
       <c r="M71" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P71">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q71">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R71">
         <v>0</v>
       </c>
       <c r="S71" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T71" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V71">
         <v>0</v>
@@ -5939,16 +5991,16 @@
         <v>0</v>
       </c>
       <c r="X71" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z71">
         <v>0</v>
       </c>
       <c r="AA71" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="72" spans="1:29">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -5971,19 +6023,19 @@
         <v>267</v>
       </c>
       <c r="K72">
-        <v>1.062636416210031e+18</v>
+        <v>1.062636416210031E+18</v>
       </c>
       <c r="L72">
-        <v>1.062636416210031e+18</v>
+        <v>1.062636416210031E+18</v>
       </c>
       <c r="R72">
         <v>0</v>
       </c>
       <c r="S72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T72" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V72">
         <v>0</v>
@@ -5992,16 +6044,16 @@
         <v>0</v>
       </c>
       <c r="X72" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z72">
         <v>0</v>
       </c>
       <c r="AA72" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="73" spans="1:29">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -6024,28 +6076,28 @@
         <v>268</v>
       </c>
       <c r="K73">
-        <v>1.063364043090653e+18</v>
+        <v>1.0633640430906531E+18</v>
       </c>
       <c r="L73">
-        <v>1.063364043090653e+18</v>
+        <v>1.0633640430906531E+18</v>
       </c>
       <c r="M73" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P73">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q73">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R73">
         <v>0</v>
       </c>
       <c r="S73" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T73" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V73">
         <v>0</v>
@@ -6054,16 +6106,16 @@
         <v>0</v>
       </c>
       <c r="X73" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z73">
         <v>0</v>
       </c>
       <c r="AA73" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="74" spans="1:29">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -6086,28 +6138,28 @@
         <v>269</v>
       </c>
       <c r="K74">
-        <v>1.063385364583391e+18</v>
+        <v>1.063385364583391E+18</v>
       </c>
       <c r="L74">
-        <v>1.063385364583391e+18</v>
+        <v>1.063385364583391E+18</v>
       </c>
       <c r="M74" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P74">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q74">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R74">
         <v>0</v>
       </c>
       <c r="S74" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T74" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V74">
         <v>0</v>
@@ -6116,16 +6168,16 @@
         <v>0</v>
       </c>
       <c r="X74" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z74">
         <v>0</v>
       </c>
       <c r="AA74" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="75" spans="1:29">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -6145,31 +6197,31 @@
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>270</v>
+        <v>360</v>
       </c>
       <c r="K75">
-        <v>1.06339232383549e+18</v>
+        <v>1.06339232383549E+18</v>
       </c>
       <c r="L75">
-        <v>1.06339232383549e+18</v>
+        <v>1.06339232383549E+18</v>
       </c>
       <c r="M75" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P75">
-        <v>7.558699847614792e+17</v>
+        <v>7.5586998476147917E+17</v>
       </c>
       <c r="Q75">
-        <v>7.55869984761479e+17</v>
+        <v>7.5586998476147904E+17</v>
       </c>
       <c r="R75">
         <v>0</v>
       </c>
       <c r="S75" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T75" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V75">
         <v>0</v>
@@ -6178,16 +6230,16 @@
         <v>0</v>
       </c>
       <c r="X75" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z75">
         <v>0</v>
       </c>
       <c r="AA75" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="76" spans="1:29">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -6207,31 +6259,31 @@
         <v>0</v>
       </c>
       <c r="I76" t="s">
+        <v>270</v>
+      </c>
+      <c r="K76">
+        <v>1.06345701487616E+18</v>
+      </c>
+      <c r="L76" t="s">
         <v>271</v>
       </c>
-      <c r="K76">
-        <v>1.06345701487616e+18</v>
-      </c>
-      <c r="L76" t="s">
+      <c r="M76" t="s">
         <v>272</v>
       </c>
-      <c r="M76" t="s">
+      <c r="P76">
+        <v>7.5586998476147917E+17</v>
+      </c>
+      <c r="Q76" t="s">
         <v>273</v>
       </c>
-      <c r="P76">
-        <v>7.558699847614792e+17</v>
-      </c>
-      <c r="Q76" t="s">
+      <c r="R76">
+        <v>0</v>
+      </c>
+      <c r="S76" t="s">
         <v>274</v>
       </c>
-      <c r="R76">
-        <v>0</v>
-      </c>
-      <c r="S76" t="s">
-        <v>275</v>
-      </c>
       <c r="T76" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V76">
         <v>0</v>
@@ -6240,13 +6292,13 @@
         <v>0</v>
       </c>
       <c r="X76" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z76">
         <v>0</v>
       </c>
       <c r="AA76" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>